<commit_message>
Updated for August 2020
</commit_message>
<xml_diff>
--- a/PV_investment_electricity_cost.xlsx
+++ b/PV_investment_electricity_cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ElectricityCalculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9721494E-6B04-40C0-9D9E-66C46D588058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA1A18C-7398-47F5-9745-00FC1EB0E6A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="2850" windowWidth="43425" windowHeight="15435" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity 2020" sheetId="2" r:id="rId1"/>
@@ -37,6 +37,7 @@
   <authors>
     <author>Magnus Pernemark</author>
     <author>tc={76BFE69C-7F47-48F2-A438-4C262BA666B7}</author>
+    <author>tc={3B4F1765-4E89-4343-A705-3C134C1B6F43}</author>
   </authors>
   <commentList>
     <comment ref="B3" authorId="0" shapeId="0" xr:uid="{1B664088-23FD-473D-8C06-557FDE18B3AE}">
@@ -113,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{B02FA356-B083-43AD-ABF5-E9CEB24B2DF3}">
+    <comment ref="AB3" authorId="0" shapeId="0" xr:uid="{B02FA356-B083-43AD-ABF5-E9CEB24B2DF3}">
       <text>
         <r>
           <rPr>
@@ -137,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC3" authorId="0" shapeId="0" xr:uid="{2971E639-60A4-4DF2-84FB-60FBFF742701}">
+    <comment ref="AD3" authorId="0" shapeId="0" xr:uid="{2971E639-60A4-4DF2-84FB-60FBFF742701}">
       <text>
         <r>
           <rPr>
@@ -169,12 +170,20 @@
     Only 22 days of production (adjusted accordingly)</t>
       </text>
     </comment>
+    <comment ref="B11" authorId="2" shapeId="0" xr:uid="{3B4F1765-4E89-4343-A705-3C134C1B6F43}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Few more cells where added, value is original 19.11kWp</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>kWh</t>
   </si>
@@ -365,6 +374,9 @@
   </si>
   <si>
     <t>(enter this value into SolarEdge Dashboard per 2020-01-01)</t>
+  </si>
+  <si>
+    <t>Percentage of selfconsumption (%)</t>
   </si>
 </sst>
 </file>
@@ -378,7 +390,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;????\ &quot;kr&quot;_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.000\ &quot;kr&quot;_-;\-* #,##0.000\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,6 +494,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF21CC72"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -674,7 +692,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -759,17 +777,22 @@
     </xf>
     <xf numFmtId="166" fontId="13" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="13" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -792,7 +815,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Magnus" id="{D9B1315B-F406-4F34-B1AC-A9B4C068D828}" userId="S::magnus.pernemark@evry.com::3d6e99da-d1b8-46ff-806b-3424a54f5ab4" providerId="AD"/>
+  <person displayName="Magnus Pernemark" id="{D9B1315B-F406-4F34-B1AC-A9B4C068D828}" userId="S::magnus.pernemark@evry.com::3d6e99da-d1b8-46ff-806b-3424a54f5ab4" providerId="AD"/>
 </personList>
 </file>
 
@@ -1096,15 +1119,18 @@
   <threadedComment ref="H9" dT="2020-07-06T22:23:19.89" personId="{D9B1315B-F406-4F34-B1AC-A9B4C068D828}" id="{76BFE69C-7F47-48F2-A438-4C262BA666B7}">
     <text>Only 22 days of production (adjusted accordingly)</text>
   </threadedComment>
+  <threadedComment ref="B11" dT="2020-09-07T18:17:49.06" personId="{D9B1315B-F406-4F34-B1AC-A9B4C068D828}" id="{3B4F1765-4E89-4343-A705-3C134C1B6F43}">
+    <text>Few more cells where added, value is original 19.11kWp</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1623E28-38CC-4E14-8F03-C1FE1A23361C}">
-  <dimension ref="A1:AE28"/>
+  <dimension ref="A1:AF28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,96 +1143,97 @@
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" customWidth="1"/>
-    <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" customWidth="1"/>
-    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="15.85546875" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" customWidth="1"/>
+    <col min="11" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" customWidth="1"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="15.85546875" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="10">
         <v>2020</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="50"/>
+      <c r="J1" s="52"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50" t="s">
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="52"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="C2" s="51" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="C2" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51" t="s">
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="M2" s="51" t="s">
+      <c r="J2" s="53"/>
+      <c r="N2" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51" t="s">
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="53"/>
     </row>
-    <row r="3" spans="1:31" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>42</v>
       </c>
@@ -1240,61 +1267,64 @@
       <c r="L3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="Q3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="R3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="S3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="U3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="V3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="V3" s="13" t="s">
+      <c r="W3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="X3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="13" t="s">
+      <c r="Y3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="Z3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" s="13" t="s">
+      <c r="AA3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AB3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AC3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AC3" s="36" t="s">
+      <c r="AD3" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="AD3" s="11"/>
       <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1327,68 +1357,72 @@
         <v>0</v>
       </c>
       <c r="K4" s="20">
-        <f t="shared" ref="K4:K10" si="0">(G4/1000)+I4-J4</f>
+        <f t="shared" ref="K4:K11" si="0">(G4/1000)+I4-J4</f>
         <v>2451</v>
       </c>
       <c r="L4" s="20">
         <f>K4-I4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="54">
+        <f>L4/K4</f>
         <v>0</v>
       </c>
       <c r="N4" s="18">
+        <v>0</v>
+      </c>
+      <c r="O4" s="18">
         <v>383.75</v>
       </c>
-      <c r="O4" s="19">
+      <c r="P4" s="19">
         <v>36.5</v>
       </c>
-      <c r="P4" s="19">
+      <c r="Q4" s="19">
         <v>14.4</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="R4" s="19">
         <v>44.13</v>
       </c>
-      <c r="R4" s="19"/>
       <c r="S4" s="19"/>
-      <c r="T4" s="14">
-        <f>(K4*(O4+P4+Q4)/100)+M4+N4</f>
+      <c r="T4" s="19"/>
+      <c r="U4" s="14">
+        <f>(K4*(P4+Q4+R4)/100)+N4+O4</f>
         <v>2712.9353000000001</v>
       </c>
-      <c r="U4" s="14">
-        <f t="shared" ref="U4:U8" si="1">(I4*(O4+P4+Q4)/100)+M4+N4</f>
+      <c r="V4" s="14">
+        <f t="shared" ref="V4:V8" si="1">(I4*(P4+Q4+R4)/100)+N4+O4</f>
         <v>2712.9353000000001</v>
       </c>
-      <c r="V4" s="14">
-        <f>J4*(R4+S4)/100</f>
-        <v>0</v>
-      </c>
       <c r="W4" s="14">
-        <f t="shared" ref="W4:W8" si="2">T4-U4</f>
+        <f>J4*(S4+T4)/100</f>
         <v>0</v>
       </c>
       <c r="X4" s="14">
-        <f>V4+W4</f>
-        <v>0</v>
-      </c>
-      <c r="Y4" s="15">
+        <f t="shared" ref="X4:X8" si="2">U4-V4</f>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="14">
+        <f>W4+X4</f>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="15">
         <f>J4*0.6</f>
         <v>0</v>
       </c>
-      <c r="Z4" s="14">
-        <f>Y4+X4</f>
-        <v>0</v>
-      </c>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="35">
-        <f>(O4+P4+Q4)/100</f>
+      <c r="AA4" s="14">
+        <f>Z4+Y4</f>
+        <v>0</v>
+      </c>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="35">
+        <f>(P4+Q4+R4)/100</f>
         <v>0.95030000000000003</v>
       </c>
-      <c r="AC4" s="37">
+      <c r="AD4" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1425,64 +1459,68 @@
         <v>2291</v>
       </c>
       <c r="L5" s="20">
-        <f t="shared" ref="L5:L10" si="3">K5-I5</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="18">
+        <f t="shared" ref="L5:L11" si="3">K5-I5</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="54">
+        <f t="shared" ref="M5:M18" si="4">L5/K5</f>
         <v>0</v>
       </c>
       <c r="N5" s="18">
+        <v>0</v>
+      </c>
+      <c r="O5" s="18">
         <v>383.75</v>
       </c>
-      <c r="O5" s="19">
+      <c r="P5" s="19">
         <v>30.19</v>
       </c>
-      <c r="P5" s="19">
+      <c r="Q5" s="19">
         <v>14.4</v>
       </c>
-      <c r="Q5" s="19">
+      <c r="R5" s="19">
         <v>44.13</v>
       </c>
-      <c r="R5" s="19"/>
       <c r="S5" s="19"/>
-      <c r="T5" s="14">
-        <f t="shared" ref="T5:T10" si="4">(K5*(O5+P5+Q5)/100)+M5+N5</f>
+      <c r="T5" s="19"/>
+      <c r="U5" s="14">
+        <f t="shared" ref="U5:U11" si="5">(K5*(P5+Q5+R5)/100)+N5+O5</f>
         <v>2416.3252000000002</v>
       </c>
-      <c r="U5" s="14">
+      <c r="V5" s="14">
         <f t="shared" si="1"/>
         <v>2416.3252000000002</v>
       </c>
-      <c r="V5" s="14">
-        <f t="shared" ref="V5:V9" si="5">J5*(R5+S5)/100</f>
-        <v>0</v>
-      </c>
       <c r="W5" s="14">
+        <f t="shared" ref="W5:W9" si="6">J5*(S5+T5)/100</f>
+        <v>0</v>
+      </c>
+      <c r="X5" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X5" s="14">
-        <f t="shared" ref="X5:X9" si="6">V5+W5</f>
-        <v>0</v>
-      </c>
-      <c r="Y5" s="15">
-        <f t="shared" ref="Y5:Y10" si="7">J5*0.6</f>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="14">
-        <f t="shared" ref="Z5:Z9" si="8">Y5+X5</f>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="35">
-        <f t="shared" ref="AB5:AB10" si="9">(O5+P5+Q5)/100</f>
+      <c r="Y5" s="14">
+        <f t="shared" ref="Y5:Y9" si="7">W5+X5</f>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="15">
+        <f t="shared" ref="Z5:Z9" si="8">J5*0.6</f>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="14">
+        <f t="shared" ref="AA5:AA9" si="9">Z5+Y5</f>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="35">
+        <f t="shared" ref="AC5:AC9" si="10">(P5+Q5+R5)/100</f>
         <v>0.88719999999999999</v>
       </c>
-      <c r="AC5" s="37">
+      <c r="AD5" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1522,61 +1560,65 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="54">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N6" s="18">
+        <v>0</v>
+      </c>
+      <c r="O6" s="18">
         <v>383.75</v>
       </c>
-      <c r="O6" s="19">
+      <c r="P6" s="19">
         <v>24.06</v>
       </c>
-      <c r="P6" s="19">
+      <c r="Q6" s="19">
         <v>14.4</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="R6" s="19">
         <v>44.13</v>
       </c>
-      <c r="R6" s="19"/>
       <c r="S6" s="19"/>
-      <c r="T6" s="14">
-        <f t="shared" si="4"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="14">
+        <f t="shared" si="5"/>
         <v>2227.9847</v>
       </c>
-      <c r="U6" s="14">
+      <c r="V6" s="14">
         <f t="shared" si="1"/>
         <v>2227.9847</v>
       </c>
-      <c r="V6" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="W6" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X6" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X6" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Y6" s="15">
+      <c r="Y6" s="14">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Z6" s="14">
+      <c r="Z6" s="15">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="35">
+      <c r="AA6" s="14">
         <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="35">
+        <f t="shared" si="10"/>
         <v>0.82590000000000008</v>
       </c>
-      <c r="AC6" s="37">
+      <c r="AD6" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1616,61 +1658,65 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="54">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N7" s="18">
+        <v>0</v>
+      </c>
+      <c r="O7" s="18">
         <v>383.75</v>
       </c>
-      <c r="O7" s="19">
+      <c r="P7" s="19">
         <v>17.059999999999999</v>
       </c>
-      <c r="P7" s="19">
+      <c r="Q7" s="19">
         <v>14.4</v>
       </c>
-      <c r="Q7" s="19">
+      <c r="R7" s="19">
         <v>44.13</v>
       </c>
-      <c r="R7" s="19"/>
       <c r="S7" s="19"/>
-      <c r="T7" s="14">
-        <f t="shared" si="4"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="14">
+        <f t="shared" si="5"/>
         <v>1641.5676000000001</v>
       </c>
-      <c r="U7" s="14">
+      <c r="V7" s="14">
         <f t="shared" si="1"/>
         <v>1641.5676000000001</v>
       </c>
-      <c r="V7" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="W7" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X7" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X7" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="15">
+      <c r="Y7" s="14">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Z7" s="14">
+      <c r="Z7" s="15">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AA7" s="15"/>
-      <c r="AB7" s="35">
+      <c r="AA7" s="14">
         <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="35">
+        <f t="shared" si="10"/>
         <v>0.75590000000000002</v>
       </c>
-      <c r="AC7" s="37">
+      <c r="AD7" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1710,61 +1756,65 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="54">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N8" s="18">
+        <v>0</v>
+      </c>
+      <c r="O8" s="18">
         <v>383.75</v>
       </c>
-      <c r="O8" s="19">
+      <c r="P8" s="19">
         <v>22.54</v>
       </c>
-      <c r="P8" s="19">
+      <c r="Q8" s="19">
         <v>14.4</v>
       </c>
-      <c r="Q8" s="19">
+      <c r="R8" s="19">
         <v>44.13</v>
       </c>
-      <c r="R8" s="19"/>
       <c r="S8" s="19"/>
-      <c r="T8" s="14">
-        <f t="shared" si="4"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="14">
+        <f t="shared" si="5"/>
         <v>1564.1291999999999</v>
       </c>
-      <c r="U8" s="14">
+      <c r="V8" s="14">
         <f t="shared" si="1"/>
         <v>1564.1291999999999</v>
       </c>
-      <c r="V8" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="W8" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X8" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X8" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Y8" s="15">
+      <c r="Y8" s="14">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Z8" s="14">
+      <c r="Z8" s="15">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="35">
+      <c r="AA8" s="14">
         <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="35">
+        <f t="shared" si="10"/>
         <v>0.81069999999999998</v>
       </c>
-      <c r="AC8" s="37">
+      <c r="AD8" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1804,68 +1854,72 @@
         <f t="shared" si="3"/>
         <v>625.29</v>
       </c>
-      <c r="M9" s="18">
-        <v>0</v>
+      <c r="M9" s="54">
+        <f t="shared" si="4"/>
+        <v>0.62698914057094723</v>
       </c>
       <c r="N9" s="18">
+        <v>0</v>
+      </c>
+      <c r="O9" s="18">
         <v>383.75</v>
       </c>
-      <c r="O9" s="19">
+      <c r="P9" s="19">
         <v>37.08</v>
       </c>
-      <c r="P9" s="19">
+      <c r="Q9" s="19">
         <v>14.4</v>
       </c>
-      <c r="Q9" s="19">
+      <c r="R9" s="19">
         <v>44.13</v>
       </c>
-      <c r="R9" s="19">
+      <c r="S9" s="19">
         <v>45.66</v>
       </c>
-      <c r="S9" s="19">
+      <c r="T9" s="19">
         <v>2.92</v>
       </c>
-      <c r="T9" s="14">
-        <f t="shared" si="4"/>
+      <c r="U9" s="14">
+        <f t="shared" si="5"/>
         <v>1337.258969</v>
       </c>
-      <c r="U9" s="14">
-        <f>(I9*(O9+P9+Q9)/100)+M9+N9</f>
+      <c r="V9" s="14">
+        <f>(I9*(P9+Q9+R9)/100)+N9+O9</f>
         <v>739.41920000000005</v>
       </c>
-      <c r="V9" s="14">
-        <f t="shared" si="5"/>
+      <c r="W9" s="14">
+        <f t="shared" si="6"/>
         <v>906.01699999999994</v>
       </c>
-      <c r="W9" s="14">
-        <f>T9-U9</f>
+      <c r="X9" s="14">
+        <f>U9-V9</f>
         <v>597.83976899999993</v>
       </c>
-      <c r="X9" s="14">
-        <f t="shared" si="6"/>
+      <c r="Y9" s="14">
+        <f t="shared" si="7"/>
         <v>1503.856769</v>
       </c>
-      <c r="Y9" s="15">
-        <f t="shared" si="7"/>
+      <c r="Z9" s="15">
+        <f t="shared" si="8"/>
         <v>1119</v>
       </c>
-      <c r="Z9" s="14">
-        <f t="shared" si="8"/>
+      <c r="AA9" s="14">
+        <f t="shared" si="9"/>
         <v>2622.856769</v>
       </c>
-      <c r="AA9" s="35">
-        <f>Z9/(G9/1000)</f>
+      <c r="AB9" s="35">
+        <f>AA9/(G9/1000)</f>
         <v>1.0532334663834333</v>
       </c>
-      <c r="AB9" s="35">
-        <f t="shared" si="9"/>
+      <c r="AC9" s="35">
+        <f t="shared" si="10"/>
         <v>0.95609999999999995</v>
       </c>
-      <c r="AC9" s="37">
+      <c r="AD9" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1888,7 +1942,7 @@
         <v>2627765</v>
       </c>
       <c r="H10" s="22">
-        <f t="shared" ref="H10:H15" si="10">(G10/1000)/B10</f>
+        <f t="shared" ref="H10:H15" si="11">(G10/1000)/B10</f>
         <v>1.0091263440860214</v>
       </c>
       <c r="I10" s="7">
@@ -1905,68 +1959,72 @@
         <f t="shared" si="3"/>
         <v>636.76499999999987</v>
       </c>
-      <c r="M10" s="18">
-        <v>0</v>
+      <c r="M10" s="54">
+        <f t="shared" si="4"/>
+        <v>0.67757896921038763</v>
       </c>
       <c r="N10" s="18">
+        <v>0</v>
+      </c>
+      <c r="O10" s="18">
         <v>383.75</v>
       </c>
-      <c r="O10" s="19">
+      <c r="P10" s="19">
         <v>17.03</v>
       </c>
-      <c r="P10" s="19">
+      <c r="Q10" s="19">
         <v>14.4</v>
       </c>
-      <c r="Q10" s="19">
+      <c r="R10" s="19">
         <v>44.13</v>
       </c>
-      <c r="R10" s="19">
+      <c r="S10" s="19">
         <v>21.45</v>
       </c>
-      <c r="S10" s="18">
+      <c r="T10" s="18">
         <v>2.92</v>
       </c>
-      <c r="T10" s="14">
-        <f t="shared" si="4"/>
+      <c r="U10" s="14">
+        <f t="shared" si="5"/>
         <v>1093.8364339999998</v>
       </c>
-      <c r="U10" s="14">
-        <f>(I10*(O10+P10+Q10)/100)+M10+N10</f>
+      <c r="V10" s="14">
+        <f>(I10*(P10+Q10+R10)/100)+N10+O10</f>
         <v>612.69679999999994</v>
       </c>
-      <c r="V10" s="14">
-        <f t="shared" ref="V10" si="11">J10*(R10+S10)/100</f>
+      <c r="W10" s="14">
+        <f>J10*(S10+T10)/100</f>
         <v>485.20669999999996</v>
       </c>
-      <c r="W10" s="14">
-        <f>T10-U10</f>
+      <c r="X10" s="14">
+        <f>U10-V10</f>
         <v>481.13963399999989</v>
       </c>
-      <c r="X10" s="14">
-        <f t="shared" ref="X10" si="12">V10+W10</f>
+      <c r="Y10" s="14">
+        <f t="shared" ref="Y10:Y11" si="12">W10+X10</f>
         <v>966.34633399999984</v>
       </c>
-      <c r="Y10" s="15">
-        <f t="shared" ref="Y10" si="13">J10*0.6</f>
+      <c r="Z10" s="15">
+        <f t="shared" ref="Z10:Z11" si="13">J10*0.6</f>
         <v>1194.5999999999999</v>
       </c>
-      <c r="Z10" s="14">
-        <f t="shared" ref="Z10" si="14">Y10+X10</f>
+      <c r="AA10" s="14">
+        <f t="shared" ref="AA10:AA15" si="14">Z10+Y10</f>
         <v>2160.9463339999998</v>
       </c>
-      <c r="AA10" s="35">
-        <f>Z10/(G10/1000)</f>
+      <c r="AB10" s="35">
+        <f>AA10/(G10/1000)</f>
         <v>0.82235144086324308</v>
       </c>
-      <c r="AB10" s="35">
-        <f t="shared" ref="AB10" si="15">(O10+P10+Q10)/100</f>
+      <c r="AC10" s="35">
+        <f t="shared" ref="AC10:AC11" si="15">(P10+Q10+R10)/100</f>
         <v>0.75560000000000005</v>
       </c>
-      <c r="AC10" s="37">
+      <c r="AD10" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1974,56 +2032,109 @@
         <v>2173</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
+        <v>911026</v>
       </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>1885712</v>
       </c>
       <c r="E11" s="3">
-        <v>0</v>
+        <v>345331</v>
       </c>
       <c r="F11" s="3">
-        <v>0</v>
+        <v>565695</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
+        <v>2451407</v>
       </c>
       <c r="H11" s="22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="18">
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>1.1281210308329499</v>
+      </c>
+      <c r="I11" s="7">
+        <v>345</v>
+      </c>
+      <c r="J11" s="7">
+        <v>1882</v>
+      </c>
+      <c r="K11" s="20">
+        <f t="shared" si="0"/>
+        <v>914.40700000000015</v>
+      </c>
+      <c r="L11" s="20">
+        <f t="shared" si="3"/>
+        <v>569.40700000000015</v>
+      </c>
+      <c r="M11" s="54">
+        <f t="shared" si="4"/>
+        <v>0.62270630036734198</v>
       </c>
       <c r="N11" s="18">
         <v>0</v>
       </c>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="15"/>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="37"/>
+      <c r="O11" s="18">
+        <v>383.75</v>
+      </c>
+      <c r="P11" s="19">
+        <v>50.91</v>
+      </c>
+      <c r="Q11" s="19">
+        <v>14.4</v>
+      </c>
+      <c r="R11" s="19">
+        <v>44.13</v>
+      </c>
+      <c r="S11" s="19">
+        <v>54.63</v>
+      </c>
+      <c r="T11" s="18">
+        <v>2.92</v>
+      </c>
+      <c r="U11" s="14">
+        <f t="shared" si="5"/>
+        <v>1384.4770208000002</v>
+      </c>
+      <c r="V11" s="14">
+        <f>(I11*(P11+Q11+R11)/100)+N11+O11</f>
+        <v>761.31799999999998</v>
+      </c>
+      <c r="W11" s="14">
+        <f>J11*(S11+T11)/100</f>
+        <v>1083.0910000000001</v>
+      </c>
+      <c r="X11" s="15">
+        <f>U11-V11</f>
+        <v>623.15902080000023</v>
+      </c>
+      <c r="Y11" s="14">
+        <f t="shared" si="12"/>
+        <v>1706.2500208000004</v>
+      </c>
+      <c r="Z11" s="15">
+        <f t="shared" si="13"/>
+        <v>1129.2</v>
+      </c>
+      <c r="AA11" s="14">
+        <f t="shared" si="14"/>
+        <v>2835.4500208000004</v>
+      </c>
+      <c r="AB11" s="35">
+        <f>AA11/(G11/1000)</f>
+        <v>1.1566622844758134</v>
+      </c>
+      <c r="AC11" s="15">
+        <f t="shared" si="15"/>
+        <v>1.0944</v>
+      </c>
+      <c r="AD11" s="37">
+        <v>300</v>
+      </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="21">
-        <v>1454</v>
+      <c r="B12" s="56">
+        <v>1649</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -2041,41 +2152,61 @@
         <v>0</v>
       </c>
       <c r="H12" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
-      <c r="M12" s="18">
-        <v>0</v>
-      </c>
+      <c r="M12" s="54"/>
       <c r="N12" s="18">
         <v>0</v>
       </c>
-      <c r="O12" s="19"/>
+      <c r="O12" s="18">
+        <v>0</v>
+      </c>
       <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="14"/>
+      <c r="Q12" s="19">
+        <v>14.4</v>
+      </c>
+      <c r="R12" s="19">
+        <v>44.13</v>
+      </c>
+      <c r="S12" s="19"/>
+      <c r="T12" s="18"/>
       <c r="U12" s="14"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="15"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="37"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14">
+        <f>J12*(S12+T12)/100</f>
+        <v>0</v>
+      </c>
+      <c r="X12" s="15">
+        <f t="shared" ref="X12:X15" si="16">U12-V12</f>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="14">
+        <f t="shared" ref="Y12:Y15" si="17">W12+X12</f>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="15">
+        <f>J12*0.6</f>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AB12" s="35"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="37"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="21">
-        <v>696</v>
+      <c r="B13" s="56">
+        <v>785</v>
       </c>
       <c r="C13" s="3">
         <v>0</v>
@@ -2093,41 +2224,61 @@
         <v>0</v>
       </c>
       <c r="H13" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="18">
-        <v>0</v>
-      </c>
+      <c r="M13" s="54"/>
       <c r="N13" s="18">
         <v>0</v>
       </c>
-      <c r="O13" s="19"/>
+      <c r="O13" s="18">
+        <v>0</v>
+      </c>
       <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="14"/>
+      <c r="Q13" s="19">
+        <v>14.4</v>
+      </c>
+      <c r="R13" s="19">
+        <v>44.13</v>
+      </c>
+      <c r="S13" s="19"/>
+      <c r="T13" s="18"/>
       <c r="U13" s="14"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="15"/>
-      <c r="AB13" s="15"/>
-      <c r="AC13" s="37"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14">
+        <f>J13*(S13+T13)/100</f>
+        <v>0</v>
+      </c>
+      <c r="X13" s="15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="14">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="15">
+        <f>J13*0.6</f>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="35"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="37"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="21">
-        <v>227</v>
+      <c r="B14" s="56">
+        <v>252</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -2145,41 +2296,61 @@
         <v>0</v>
       </c>
       <c r="H14" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
-      <c r="M14" s="18">
-        <v>0</v>
-      </c>
+      <c r="M14" s="54"/>
       <c r="N14" s="18">
         <v>0</v>
       </c>
-      <c r="O14" s="19"/>
+      <c r="O14" s="18">
+        <v>0</v>
+      </c>
       <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="14"/>
+      <c r="Q14" s="19">
+        <v>14.4</v>
+      </c>
+      <c r="R14" s="19">
+        <v>44.13</v>
+      </c>
+      <c r="S14" s="19"/>
+      <c r="T14" s="18"/>
       <c r="U14" s="14"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="37"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14">
+        <f>J14*(S14+T14)/100</f>
+        <v>0</v>
+      </c>
+      <c r="X14" s="15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="14">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="15">
+        <f>J14*0.6</f>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="35"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="37"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="21">
-        <v>117</v>
+      <c r="B15" s="56">
+        <v>129</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -2197,36 +2368,56 @@
         <v>0</v>
       </c>
       <c r="H15" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
-      <c r="M15" s="18">
-        <v>0</v>
-      </c>
+      <c r="M15" s="54"/>
       <c r="N15" s="18">
         <v>0</v>
       </c>
-      <c r="O15" s="19"/>
+      <c r="O15" s="18">
+        <v>0</v>
+      </c>
       <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="14"/>
+      <c r="Q15" s="19">
+        <v>14.4</v>
+      </c>
+      <c r="R15" s="19">
+        <v>44.13</v>
+      </c>
+      <c r="S15" s="19"/>
+      <c r="T15" s="18"/>
       <c r="U15" s="14"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="15"/>
-      <c r="AC15" s="37"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14">
+        <f>J15*(S15+T15)/100</f>
+        <v>0</v>
+      </c>
+      <c r="X15" s="15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="14">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="15">
+        <f>J15*0.6</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="35"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="37"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="21"/>
       <c r="C16" s="3"/>
@@ -2239,25 +2430,26 @@
       <c r="J16" s="7"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
-      <c r="M16" s="18"/>
+      <c r="M16" s="54"/>
       <c r="N16" s="18"/>
-      <c r="O16" s="19"/>
+      <c r="O16" s="18"/>
       <c r="P16" s="19"/>
       <c r="Q16" s="19"/>
       <c r="R16" s="19"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="14"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="18"/>
       <c r="U16" s="14"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
       <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
+      <c r="Y16" s="14"/>
       <c r="Z16" s="15"/>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="15"/>
-      <c r="AC16" s="37"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="35"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="37"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
         <v>0</v>
       </c>
@@ -2289,14 +2481,14 @@
       <c r="L17" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="M17" s="39" t="s">
-        <v>39</v>
+      <c r="M17" s="38" t="s">
+        <v>0</v>
       </c>
       <c r="N17" s="39" t="s">
         <v>39</v>
       </c>
       <c r="O17" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P17" s="39" t="s">
         <v>40</v>
@@ -2311,7 +2503,7 @@
         <v>40</v>
       </c>
       <c r="T17" s="39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U17" s="39" t="s">
         <v>39</v>
@@ -2340,122 +2532,129 @@
       <c r="AC17" s="39" t="s">
         <v>39</v>
       </c>
+      <c r="AD17" s="39" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="18" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="41">
         <f>SUM(B4:B17)</f>
-        <v>16657</v>
+        <v>16978</v>
       </c>
       <c r="C18" s="42">
         <f>SUM(C4:C17)/1000</f>
-        <v>1943.731</v>
+        <v>2854.7570000000001</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D4:D17)/1000</f>
-        <v>4064.223</v>
+        <v>5949.9350000000004</v>
       </c>
       <c r="E18" s="42">
         <f>SUM(E4:E17)/1000</f>
-        <v>881.39200000000005</v>
+        <v>1226.723</v>
       </c>
       <c r="F18" s="42">
         <f>SUM(F4:F17)/1000</f>
-        <v>1047.31</v>
+        <v>1613.0050000000001</v>
       </c>
       <c r="G18" s="42">
         <f>SUM(G4:G17)/1000</f>
-        <v>5118.0550000000003</v>
+        <v>7569.4620000000004</v>
       </c>
       <c r="H18" s="42"/>
       <c r="I18" s="43">
-        <f t="shared" ref="I18:N18" si="16">SUM(I4:I15)</f>
-        <v>10770</v>
+        <f t="shared" ref="I18:O18" si="18">SUM(I4:I15)</f>
+        <v>11115</v>
       </c>
       <c r="J18" s="43">
-        <f t="shared" si="16"/>
-        <v>3856</v>
+        <f t="shared" si="18"/>
+        <v>5738</v>
       </c>
       <c r="K18" s="43">
-        <f t="shared" si="16"/>
-        <v>12032.055</v>
+        <f t="shared" si="18"/>
+        <v>12946.462</v>
       </c>
       <c r="L18" s="43">
-        <f t="shared" si="16"/>
-        <v>1262.0549999999998</v>
-      </c>
-      <c r="M18" s="43">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="44">
-        <f t="shared" si="16"/>
-        <v>2686.25</v>
+        <f t="shared" si="18"/>
+        <v>1831.462</v>
+      </c>
+      <c r="M18" s="55">
+        <f t="shared" si="4"/>
+        <v>0.14146428576394077</v>
+      </c>
+      <c r="N18" s="43">
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
       <c r="O18" s="44">
-        <f>AVERAGE(O4:O15)</f>
-        <v>26.351428571428574</v>
+        <f t="shared" si="18"/>
+        <v>3070</v>
       </c>
       <c r="P18" s="44">
         <f>AVERAGE(P4:P15)</f>
-        <v>14.400000000000002</v>
+        <v>29.421250000000001</v>
       </c>
       <c r="Q18" s="44">
         <f>AVERAGE(Q4:Q15)</f>
-        <v>44.13</v>
+        <v>14.400000000000004</v>
       </c>
       <c r="R18" s="44">
         <f>AVERAGE(R4:R15)</f>
-        <v>33.555</v>
+        <v>44.13</v>
       </c>
       <c r="S18" s="44">
         <f>AVERAGE(S4:S15)</f>
+        <v>40.580000000000005</v>
+      </c>
+      <c r="T18" s="44">
+        <f>AVERAGE(T4:T15)</f>
         <v>2.92</v>
       </c>
-      <c r="T18" s="44">
-        <f t="shared" ref="T18:Z18" si="17">SUM(T4:T15)</f>
-        <v>12994.037402999998</v>
-      </c>
       <c r="U18" s="44">
-        <f t="shared" si="17"/>
-        <v>11915.057999999999</v>
+        <f t="shared" ref="U18:AA18" si="19">SUM(U4:U15)</f>
+        <v>14378.514423799999</v>
       </c>
       <c r="V18" s="44">
-        <f t="shared" si="17"/>
-        <v>1391.2237</v>
+        <f t="shared" si="19"/>
+        <v>12676.375999999998</v>
       </c>
       <c r="W18" s="44">
-        <f t="shared" si="17"/>
-        <v>1078.9794029999998</v>
+        <f t="shared" si="19"/>
+        <v>2474.3146999999999</v>
       </c>
       <c r="X18" s="44">
-        <f t="shared" si="17"/>
-        <v>2470.2031029999998</v>
+        <f t="shared" si="19"/>
+        <v>1702.1384238000001</v>
       </c>
       <c r="Y18" s="44">
-        <f t="shared" si="17"/>
-        <v>2313.6</v>
+        <f t="shared" si="19"/>
+        <v>4176.4531238</v>
       </c>
       <c r="Z18" s="44">
-        <f t="shared" si="17"/>
-        <v>4783.8031030000002</v>
-      </c>
-      <c r="AA18" s="45">
-        <f>AVERAGE(AA4:AA15)</f>
-        <v>0.93779245362333818</v>
+        <f t="shared" si="19"/>
+        <v>3442.8</v>
+      </c>
+      <c r="AA18" s="44">
+        <f t="shared" si="19"/>
+        <v>7619.253123800001</v>
       </c>
       <c r="AB18" s="45">
         <f>AVERAGE(AB4:AB15)</f>
-        <v>0.84881428571428585</v>
-      </c>
-      <c r="AC18" s="44">
-        <f>SUM(AC4:AC15)</f>
-        <v>900</v>
+        <v>1.0107490639074965</v>
+      </c>
+      <c r="AC18" s="45">
+        <f>AVERAGE(AC4:AC15)</f>
+        <v>0.87951250000000014</v>
+      </c>
+      <c r="AD18" s="44">
+        <f>SUM(AD4:AD15)</f>
+        <v>1200</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -2468,8 +2667,9 @@
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
     </row>
-    <row r="20" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -2482,8 +2682,9 @@
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
     </row>
-    <row r="21" spans="1:29" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="46" t="s">
         <v>45</v>
       </c>
@@ -2506,36 +2707,37 @@
       </c>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="N21" s="52" t="s">
+      <c r="N21" s="6"/>
+      <c r="O21" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="O21" s="52"/>
-      <c r="P21" s="6"/>
+      <c r="P21" s="50"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
     </row>
-    <row r="22" spans="1:29" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="47">
         <f>G18</f>
-        <v>5118.0550000000003</v>
+        <v>7569.4620000000004</v>
       </c>
       <c r="D22" s="47">
         <f>J18</f>
-        <v>3856</v>
+        <v>5738</v>
       </c>
       <c r="E22" s="47">
         <f>I18</f>
-        <v>10770</v>
+        <v>11115</v>
       </c>
       <c r="F22" s="47">
         <f>K18</f>
-        <v>12032.055</v>
+        <v>12946.462</v>
       </c>
       <c r="G22" s="47">
         <f>L18</f>
-        <v>1262.0549999999998</v>
+        <v>1831.462</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -2547,18 +2749,19 @@
       </c>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="53">
+      <c r="N22" s="6"/>
+      <c r="O22" s="51">
         <f>G24/(G18)</f>
-        <v>0.93469161683491087</v>
-      </c>
-      <c r="O22" s="53"/>
-      <c r="P22" s="6"/>
+        <v>1.0065778946773232</v>
+      </c>
+      <c r="P22" s="51"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C23" s="23"/>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
@@ -2567,11 +2770,11 @@
       <c r="K23" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="O23" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" ht="21" x14ac:dyDescent="0.35">
       <c r="C24" s="26" t="s">
         <v>52</v>
       </c>
@@ -2579,25 +2782,25 @@
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
       <c r="G24" s="49">
-        <f>Z18+K22</f>
-        <v>4783.8031030000002</v>
+        <f>AA18+K22</f>
+        <v>7619.253123800001</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="28"/>
       <c r="D25" s="29"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
       <c r="G25" s="31"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C26" s="23"/>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="25"/>
     </row>
-    <row r="27" spans="1:29" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:30" ht="21" x14ac:dyDescent="0.35">
       <c r="C27" s="32" t="s">
         <v>54</v>
       </c>
@@ -2605,11 +2808,11 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="48">
-        <f>G24-AC18</f>
-        <v>3883.8031030000002</v>
+        <f>G24-AD18</f>
+        <v>6419.253123800001</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="28"/>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
@@ -2618,16 +2821,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="T1:AB1"/>
-    <mergeCell ref="T2:AB2"/>
-    <mergeCell ref="I2:J2"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="M1:S1"/>
-    <mergeCell ref="M2:S2"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="U1:AC1"/>
+    <mergeCell ref="U2:AC2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated for September 2020
</commit_message>
<xml_diff>
--- a/PV_investment_electricity_cost.xlsx
+++ b/PV_investment_electricity_cost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ElectricityCalculations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devstuff\ElectricityCalculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA1A18C-7398-47F5-9745-00FC1EB0E6A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0148763-4B2A-44B8-BEB9-F004A9CD03A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
   </bookViews>
@@ -777,11 +777,10 @@
     </xf>
     <xf numFmtId="166" fontId="13" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="13" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -789,10 +788,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1129,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1623E28-38CC-4E14-8F03-C1FE1A23361C}">
   <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,75 +1163,75 @@
         <v>2020</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52" t="s">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="52"/>
+      <c r="J1" s="53"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52" t="s">
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="52"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="53"/>
-      <c r="N2" s="53" t="s">
+      <c r="J2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
     </row>
     <row r="3" spans="1:32" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -1357,14 +1357,14 @@
         <v>0</v>
       </c>
       <c r="K4" s="20">
-        <f t="shared" ref="K4:K11" si="0">(G4/1000)+I4-J4</f>
+        <f t="shared" ref="K4:K12" si="0">(G4/1000)+I4-J4</f>
         <v>2451</v>
       </c>
       <c r="L4" s="20">
         <f>K4-I4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="54">
+      <c r="M4" s="50">
         <f>L4/K4</f>
         <v>0</v>
       </c>
@@ -1459,10 +1459,10 @@
         <v>2291</v>
       </c>
       <c r="L5" s="20">
-        <f t="shared" ref="L5:L11" si="3">K5-I5</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="54">
+        <f t="shared" ref="L5:L12" si="3">K5-I5</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="50">
         <f t="shared" ref="M5:M18" si="4">L5/K5</f>
         <v>0</v>
       </c>
@@ -1484,7 +1484,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
       <c r="U5" s="14">
-        <f t="shared" ref="U5:U11" si="5">(K5*(P5+Q5+R5)/100)+N5+O5</f>
+        <f t="shared" ref="U5:U12" si="5">(K5*(P5+Q5+R5)/100)+N5+O5</f>
         <v>2416.3252000000002</v>
       </c>
       <c r="V5" s="14">
@@ -1560,7 +1560,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M6" s="54">
+      <c r="M6" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1658,7 +1658,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M7" s="54">
+      <c r="M7" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1756,7 +1756,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M8" s="54">
+      <c r="M8" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1854,7 +1854,7 @@
         <f t="shared" si="3"/>
         <v>625.29</v>
       </c>
-      <c r="M9" s="54">
+      <c r="M9" s="50">
         <f t="shared" si="4"/>
         <v>0.62698914057094723</v>
       </c>
@@ -1959,7 +1959,7 @@
         <f t="shared" si="3"/>
         <v>636.76499999999987</v>
       </c>
-      <c r="M10" s="54">
+      <c r="M10" s="50">
         <f t="shared" si="4"/>
         <v>0.67757896921038763</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>612.69679999999994</v>
       </c>
       <c r="W10" s="14">
-        <f>J10*(S10+T10)/100</f>
+        <f t="shared" ref="W10:W15" si="12">J10*(S10+T10)/100</f>
         <v>485.20669999999996</v>
       </c>
       <c r="X10" s="14">
@@ -2001,15 +2001,15 @@
         <v>481.13963399999989</v>
       </c>
       <c r="Y10" s="14">
-        <f t="shared" ref="Y10:Y11" si="12">W10+X10</f>
+        <f t="shared" ref="Y10:Y11" si="13">W10+X10</f>
         <v>966.34633399999984</v>
       </c>
       <c r="Z10" s="15">
-        <f t="shared" ref="Z10:Z11" si="13">J10*0.6</f>
+        <f t="shared" ref="Z10:Z11" si="14">J10*0.6</f>
         <v>1194.5999999999999</v>
       </c>
       <c r="AA10" s="14">
-        <f t="shared" ref="AA10:AA15" si="14">Z10+Y10</f>
+        <f t="shared" ref="AA10:AA15" si="15">Z10+Y10</f>
         <v>2160.9463339999998</v>
       </c>
       <c r="AB10" s="35">
@@ -2017,7 +2017,7 @@
         <v>0.82235144086324308</v>
       </c>
       <c r="AC10" s="35">
-        <f t="shared" ref="AC10:AC11" si="15">(P10+Q10+R10)/100</f>
+        <f t="shared" ref="AC10:AC12" si="16">(P10+Q10+R10)/100</f>
         <v>0.75560000000000005</v>
       </c>
       <c r="AD10" s="37">
@@ -2064,7 +2064,7 @@
         <f t="shared" si="3"/>
         <v>569.40700000000015</v>
       </c>
-      <c r="M11" s="54">
+      <c r="M11" s="50">
         <f t="shared" si="4"/>
         <v>0.62270630036734198</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>761.31799999999998</v>
       </c>
       <c r="W11" s="14">
-        <f>J11*(S11+T11)/100</f>
+        <f t="shared" si="12"/>
         <v>1083.0910000000001</v>
       </c>
       <c r="X11" s="15">
@@ -2106,15 +2106,15 @@
         <v>623.15902080000023</v>
       </c>
       <c r="Y11" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1706.2500208000004</v>
       </c>
       <c r="Z11" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1129.2</v>
       </c>
       <c r="AA11" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2835.4500208000004</v>
       </c>
       <c r="AB11" s="35">
@@ -2122,7 +2122,7 @@
         <v>1.1566622844758134</v>
       </c>
       <c r="AC11" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0944</v>
       </c>
       <c r="AD11" s="37">
@@ -2133,79 +2133,112 @@
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="56">
+      <c r="B12" s="52">
         <v>1649</v>
       </c>
       <c r="C12" s="3">
-        <v>0</v>
+        <v>963500</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>1021839</v>
       </c>
       <c r="E12" s="3">
-        <v>0</v>
+        <v>540904</v>
       </c>
       <c r="F12" s="3">
-        <v>0</v>
+        <v>422596</v>
       </c>
       <c r="G12" s="3">
-        <v>0</v>
+        <v>1444435</v>
       </c>
       <c r="H12" s="22">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="54"/>
+        <v>0.87594602789569431</v>
+      </c>
+      <c r="I12" s="7">
+        <v>541</v>
+      </c>
+      <c r="J12" s="7">
+        <v>1021</v>
+      </c>
+      <c r="K12" s="20">
+        <f t="shared" si="0"/>
+        <v>964.43499999999995</v>
+      </c>
+      <c r="L12" s="20">
+        <f t="shared" si="3"/>
+        <v>423.43499999999995</v>
+      </c>
+      <c r="M12" s="50">
+        <f t="shared" si="4"/>
+        <v>0.43904980636331115</v>
+      </c>
       <c r="N12" s="18">
         <v>0</v>
       </c>
       <c r="O12" s="18">
-        <v>0</v>
-      </c>
-      <c r="P12" s="19"/>
+        <v>383.75</v>
+      </c>
+      <c r="P12" s="19">
+        <v>49.69</v>
+      </c>
       <c r="Q12" s="19">
         <v>14.4</v>
       </c>
       <c r="R12" s="19">
         <v>44.13</v>
       </c>
-      <c r="S12" s="19"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
+      <c r="S12" s="19">
+        <v>48.24</v>
+      </c>
+      <c r="T12" s="18">
+        <v>2.92</v>
+      </c>
+      <c r="U12" s="14">
+        <f t="shared" si="5"/>
+        <v>1427.4615569999999</v>
+      </c>
+      <c r="V12" s="14">
+        <f>(I12*(P12+Q12+R12)/100)+N12+O12</f>
+        <v>969.22019999999998</v>
+      </c>
       <c r="W12" s="14">
-        <f>J12*(S12+T12)/100</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>522.34360000000004</v>
       </c>
       <c r="X12" s="15">
-        <f t="shared" ref="X12:X15" si="16">U12-V12</f>
-        <v>0</v>
+        <f t="shared" ref="X12:X15" si="17">U12-V12</f>
+        <v>458.24135699999988</v>
       </c>
       <c r="Y12" s="14">
-        <f t="shared" ref="Y12:Y15" si="17">W12+X12</f>
-        <v>0</v>
+        <f t="shared" ref="Y12:Y15" si="18">W12+X12</f>
+        <v>980.58495699999992</v>
       </c>
       <c r="Z12" s="15">
         <f>J12*0.6</f>
-        <v>0</v>
+        <v>612.6</v>
       </c>
       <c r="AA12" s="14">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="35"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="37"/>
+        <f t="shared" si="15"/>
+        <v>1593.1849569999999</v>
+      </c>
+      <c r="AB12" s="35">
+        <f>AA12/(G12/1000)</f>
+        <v>1.1029814128015452</v>
+      </c>
+      <c r="AC12" s="15">
+        <f t="shared" si="16"/>
+        <v>1.0822000000000001</v>
+      </c>
+      <c r="AD12" s="37">
+        <v>300</v>
+      </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="56">
+      <c r="B13" s="52">
         <v>785</v>
       </c>
       <c r="C13" s="3">
@@ -2231,7 +2264,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="54"/>
+      <c r="M13" s="50"/>
       <c r="N13" s="18">
         <v>0</v>
       </c>
@@ -2250,15 +2283,15 @@
       <c r="U13" s="14"/>
       <c r="V13" s="14"/>
       <c r="W13" s="14">
-        <f>J13*(S13+T13)/100</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X13" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Y13" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Z13" s="15">
@@ -2266,7 +2299,7 @@
         <v>0</v>
       </c>
       <c r="AA13" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB13" s="35"/>
@@ -2277,7 +2310,7 @@
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="56">
+      <c r="B14" s="52">
         <v>252</v>
       </c>
       <c r="C14" s="3">
@@ -2303,7 +2336,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
-      <c r="M14" s="54"/>
+      <c r="M14" s="50"/>
       <c r="N14" s="18">
         <v>0</v>
       </c>
@@ -2322,15 +2355,15 @@
       <c r="U14" s="14"/>
       <c r="V14" s="14"/>
       <c r="W14" s="14">
-        <f>J14*(S14+T14)/100</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X14" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Y14" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Z14" s="15">
@@ -2338,7 +2371,7 @@
         <v>0</v>
       </c>
       <c r="AA14" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB14" s="35"/>
@@ -2349,7 +2382,7 @@
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="56">
+      <c r="B15" s="52">
         <v>129</v>
       </c>
       <c r="C15" s="3">
@@ -2375,7 +2408,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
-      <c r="M15" s="54"/>
+      <c r="M15" s="50"/>
       <c r="N15" s="18">
         <v>0</v>
       </c>
@@ -2394,15 +2427,15 @@
       <c r="U15" s="14"/>
       <c r="V15" s="14"/>
       <c r="W15" s="14">
-        <f>J15*(S15+T15)/100</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X15" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Y15" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Z15" s="15">
@@ -2410,7 +2443,7 @@
         <v>0</v>
       </c>
       <c r="AA15" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB15" s="35"/>
@@ -2430,7 +2463,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
-      <c r="M16" s="54"/>
+      <c r="M16" s="50"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
       <c r="P16" s="19"/>
@@ -2546,56 +2579,56 @@
       </c>
       <c r="C18" s="42">
         <f>SUM(C4:C17)/1000</f>
-        <v>2854.7570000000001</v>
+        <v>3818.2570000000001</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D4:D17)/1000</f>
-        <v>5949.9350000000004</v>
+        <v>6971.7740000000003</v>
       </c>
       <c r="E18" s="42">
         <f>SUM(E4:E17)/1000</f>
-        <v>1226.723</v>
+        <v>1767.627</v>
       </c>
       <c r="F18" s="42">
         <f>SUM(F4:F17)/1000</f>
-        <v>1613.0050000000001</v>
+        <v>2035.6010000000001</v>
       </c>
       <c r="G18" s="42">
         <f>SUM(G4:G17)/1000</f>
-        <v>7569.4620000000004</v>
+        <v>9013.8970000000008</v>
       </c>
       <c r="H18" s="42"/>
       <c r="I18" s="43">
-        <f t="shared" ref="I18:O18" si="18">SUM(I4:I15)</f>
-        <v>11115</v>
+        <f t="shared" ref="I18:O18" si="19">SUM(I4:I15)</f>
+        <v>11656</v>
       </c>
       <c r="J18" s="43">
-        <f t="shared" si="18"/>
-        <v>5738</v>
+        <f t="shared" si="19"/>
+        <v>6759</v>
       </c>
       <c r="K18" s="43">
-        <f t="shared" si="18"/>
-        <v>12946.462</v>
+        <f t="shared" si="19"/>
+        <v>13910.896999999999</v>
       </c>
       <c r="L18" s="43">
-        <f t="shared" si="18"/>
-        <v>1831.462</v>
-      </c>
-      <c r="M18" s="55">
+        <f t="shared" si="19"/>
+        <v>2254.8969999999999</v>
+      </c>
+      <c r="M18" s="51">
         <f t="shared" si="4"/>
-        <v>0.14146428576394077</v>
+        <v>0.16209572970024866</v>
       </c>
       <c r="N18" s="43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="O18" s="44">
-        <f t="shared" si="18"/>
-        <v>3070</v>
+        <f t="shared" si="19"/>
+        <v>3453.75</v>
       </c>
       <c r="P18" s="44">
         <f>AVERAGE(P4:P15)</f>
-        <v>29.421250000000001</v>
+        <v>31.673333333333332</v>
       </c>
       <c r="Q18" s="44">
         <f>AVERAGE(Q4:Q15)</f>
@@ -2607,51 +2640,51 @@
       </c>
       <c r="S18" s="44">
         <f>AVERAGE(S4:S15)</f>
-        <v>40.580000000000005</v>
+        <v>42.495000000000005</v>
       </c>
       <c r="T18" s="44">
         <f>AVERAGE(T4:T15)</f>
         <v>2.92</v>
       </c>
       <c r="U18" s="44">
-        <f t="shared" ref="U18:AA18" si="19">SUM(U4:U15)</f>
-        <v>14378.514423799999</v>
+        <f t="shared" ref="U18:AA18" si="20">SUM(U4:U15)</f>
+        <v>15805.9759808</v>
       </c>
       <c r="V18" s="44">
-        <f t="shared" si="19"/>
-        <v>12676.375999999998</v>
+        <f t="shared" si="20"/>
+        <v>13645.596199999998</v>
       </c>
       <c r="W18" s="44">
-        <f t="shared" si="19"/>
-        <v>2474.3146999999999</v>
+        <f t="shared" si="20"/>
+        <v>2996.6583000000001</v>
       </c>
       <c r="X18" s="44">
-        <f t="shared" si="19"/>
-        <v>1702.1384238000001</v>
+        <f t="shared" si="20"/>
+        <v>2160.3797807999999</v>
       </c>
       <c r="Y18" s="44">
-        <f t="shared" si="19"/>
-        <v>4176.4531238</v>
+        <f t="shared" si="20"/>
+        <v>5157.0380808</v>
       </c>
       <c r="Z18" s="44">
-        <f t="shared" si="19"/>
-        <v>3442.8</v>
+        <f t="shared" si="20"/>
+        <v>4055.4</v>
       </c>
       <c r="AA18" s="44">
-        <f t="shared" si="19"/>
-        <v>7619.253123800001</v>
+        <f t="shared" si="20"/>
+        <v>9212.4380808000005</v>
       </c>
       <c r="AB18" s="45">
         <f>AVERAGE(AB4:AB15)</f>
-        <v>1.0107490639074965</v>
+        <v>1.0338071511310087</v>
       </c>
       <c r="AC18" s="45">
         <f>AVERAGE(AC4:AC15)</f>
-        <v>0.87951250000000014</v>
+        <v>0.90203333333333346</v>
       </c>
       <c r="AD18" s="44">
         <f>SUM(AD4:AD15)</f>
-        <v>1200</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
@@ -2708,10 +2741,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="50" t="s">
+      <c r="O21" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="P21" s="50"/>
+      <c r="P21" s="55"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -2721,23 +2754,23 @@
     <row r="22" spans="1:30" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="47">
         <f>G18</f>
-        <v>7569.4620000000004</v>
+        <v>9013.8970000000008</v>
       </c>
       <c r="D22" s="47">
         <f>J18</f>
-        <v>5738</v>
+        <v>6759</v>
       </c>
       <c r="E22" s="47">
         <f>I18</f>
-        <v>11115</v>
+        <v>11656</v>
       </c>
       <c r="F22" s="47">
         <f>K18</f>
-        <v>12946.462</v>
+        <v>13910.896999999999</v>
       </c>
       <c r="G22" s="47">
         <f>L18</f>
-        <v>1831.462</v>
+        <v>2254.8969999999999</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -2750,11 +2783,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="51">
+      <c r="O22" s="56">
         <f>G24/(G18)</f>
-        <v>1.0065778946773232</v>
-      </c>
-      <c r="P22" s="51"/>
+        <v>1.0220261093287397</v>
+      </c>
+      <c r="P22" s="56"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -2783,7 +2816,7 @@
       <c r="F24" s="27"/>
       <c r="G24" s="49">
         <f>AA18+K22</f>
-        <v>7619.253123800001</v>
+        <v>9212.4380808000005</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2809,7 +2842,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="48">
         <f>G24-AD18</f>
-        <v>6419.253123800001</v>
+        <v>7712.4380808000005</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2821,16 +2854,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="U1:AC1"/>
+    <mergeCell ref="U2:AC2"/>
+    <mergeCell ref="I2:J2"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="N1:T1"/>
     <mergeCell ref="N2:T2"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="U1:AC1"/>
-    <mergeCell ref="U2:AC2"/>
-    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated for October 2020
</commit_message>
<xml_diff>
--- a/PV_investment_electricity_cost.xlsx
+++ b/PV_investment_electricity_cost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devstuff\ElectricityCalculations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ElectricityCalculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0148763-4B2A-44B8-BEB9-F004A9CD03A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F036A3F3-CFB6-48A1-A551-7F32BF16F4E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
   </bookViews>
@@ -782,16 +782,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1129,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1623E28-38CC-4E14-8F03-C1FE1A23361C}">
   <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,75 +1163,75 @@
         <v>2020</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53" t="s">
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="53"/>
+      <c r="J1" s="55"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="53" t="s">
+      <c r="N1" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53" t="s">
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54" t="s">
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="J2" s="56"/>
+      <c r="N2" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54" t="s">
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="56"/>
     </row>
     <row r="3" spans="1:32" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -1357,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="20">
-        <f t="shared" ref="K4:K12" si="0">(G4/1000)+I4-J4</f>
+        <f t="shared" ref="K4:K13" si="0">(G4/1000)+I4-J4</f>
         <v>2451</v>
       </c>
       <c r="L4" s="20">
@@ -1459,7 +1459,7 @@
         <v>2291</v>
       </c>
       <c r="L5" s="20">
-        <f t="shared" ref="L5:L12" si="3">K5-I5</f>
+        <f t="shared" ref="L5:L13" si="3">K5-I5</f>
         <v>0</v>
       </c>
       <c r="M5" s="50">
@@ -1484,7 +1484,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
       <c r="U5" s="14">
-        <f t="shared" ref="U5:U12" si="5">(K5*(P5+Q5+R5)/100)+N5+O5</f>
+        <f t="shared" ref="U5:U13" si="5">(K5*(P5+Q5+R5)/100)+N5+O5</f>
         <v>2416.3252000000002</v>
       </c>
       <c r="V5" s="14">
@@ -2017,7 +2017,7 @@
         <v>0.82235144086324308</v>
       </c>
       <c r="AC10" s="35">
-        <f t="shared" ref="AC10:AC12" si="16">(P10+Q10+R10)/100</f>
+        <f t="shared" ref="AC10:AC13" si="16">(P10+Q10+R10)/100</f>
         <v>0.75560000000000005</v>
       </c>
       <c r="AD10" s="37">
@@ -2242,69 +2242,102 @@
         <v>785</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>1288599</v>
       </c>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>286301</v>
       </c>
       <c r="E13" s="3">
-        <v>0</v>
+        <v>950187</v>
       </c>
       <c r="F13" s="3">
-        <v>0</v>
+        <v>338412</v>
       </c>
       <c r="G13" s="3">
-        <v>0</v>
+        <v>624713</v>
       </c>
       <c r="H13" s="22">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="50"/>
+        <v>0.79581273885350312</v>
+      </c>
+      <c r="I13" s="7">
+        <v>953</v>
+      </c>
+      <c r="J13" s="7">
+        <v>286</v>
+      </c>
+      <c r="K13" s="20">
+        <f t="shared" si="0"/>
+        <v>1291.713</v>
+      </c>
+      <c r="L13" s="20">
+        <f t="shared" si="3"/>
+        <v>338.71299999999997</v>
+      </c>
+      <c r="M13" s="50">
+        <f t="shared" si="4"/>
+        <v>0.26222001326920141</v>
+      </c>
       <c r="N13" s="18">
         <v>0</v>
       </c>
       <c r="O13" s="18">
-        <v>0</v>
-      </c>
-      <c r="P13" s="19"/>
+        <v>383.75</v>
+      </c>
+      <c r="P13" s="19">
+        <v>35</v>
+      </c>
       <c r="Q13" s="19">
         <v>14.4</v>
       </c>
       <c r="R13" s="19">
         <v>44.13</v>
       </c>
-      <c r="S13" s="19"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
+      <c r="S13" s="19">
+        <v>42.49</v>
+      </c>
+      <c r="T13" s="18">
+        <v>2.92</v>
+      </c>
+      <c r="U13" s="14">
+        <f t="shared" si="5"/>
+        <v>1591.8891689</v>
+      </c>
+      <c r="V13" s="14">
+        <f>(I13*(P13+Q13+R13)/100)+N13+O13</f>
+        <v>1275.0908999999999</v>
+      </c>
       <c r="W13" s="14">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>129.87260000000001</v>
       </c>
       <c r="X13" s="15">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>316.79826890000004</v>
       </c>
       <c r="Y13" s="14">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>446.67086890000007</v>
       </c>
       <c r="Z13" s="15">
         <f>J13*0.6</f>
-        <v>0</v>
+        <v>171.6</v>
       </c>
       <c r="AA13" s="14">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="35"/>
-      <c r="AC13" s="15"/>
-      <c r="AD13" s="37"/>
+        <v>618.2708689000001</v>
+      </c>
+      <c r="AB13" s="35">
+        <f>AA13/(G13/1000)</f>
+        <v>0.98968785490297162</v>
+      </c>
+      <c r="AC13" s="15">
+        <f t="shared" si="16"/>
+        <v>0.93530000000000002</v>
+      </c>
+      <c r="AD13" s="37">
+        <v>300</v>
+      </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2579,44 +2612,44 @@
       </c>
       <c r="C18" s="42">
         <f>SUM(C4:C17)/1000</f>
-        <v>3818.2570000000001</v>
+        <v>5106.8559999999998</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D4:D17)/1000</f>
-        <v>6971.7740000000003</v>
+        <v>7258.0749999999998</v>
       </c>
       <c r="E18" s="42">
         <f>SUM(E4:E17)/1000</f>
-        <v>1767.627</v>
+        <v>2717.8139999999999</v>
       </c>
       <c r="F18" s="42">
         <f>SUM(F4:F17)/1000</f>
-        <v>2035.6010000000001</v>
+        <v>2374.0129999999999</v>
       </c>
       <c r="G18" s="42">
         <f>SUM(G4:G17)/1000</f>
-        <v>9013.8970000000008</v>
+        <v>9638.61</v>
       </c>
       <c r="H18" s="42"/>
       <c r="I18" s="43">
         <f t="shared" ref="I18:O18" si="19">SUM(I4:I15)</f>
-        <v>11656</v>
+        <v>12609</v>
       </c>
       <c r="J18" s="43">
         <f t="shared" si="19"/>
-        <v>6759</v>
+        <v>7045</v>
       </c>
       <c r="K18" s="43">
         <f t="shared" si="19"/>
-        <v>13910.896999999999</v>
+        <v>15202.609999999999</v>
       </c>
       <c r="L18" s="43">
         <f t="shared" si="19"/>
-        <v>2254.8969999999999</v>
+        <v>2593.6099999999997</v>
       </c>
       <c r="M18" s="51">
         <f t="shared" si="4"/>
-        <v>0.16209572970024866</v>
+        <v>0.17060294252105393</v>
       </c>
       <c r="N18" s="43">
         <f t="shared" si="19"/>
@@ -2624,11 +2657,11 @@
       </c>
       <c r="O18" s="44">
         <f t="shared" si="19"/>
-        <v>3453.75</v>
+        <v>3837.5</v>
       </c>
       <c r="P18" s="44">
         <f>AVERAGE(P4:P15)</f>
-        <v>31.673333333333332</v>
+        <v>32.006</v>
       </c>
       <c r="Q18" s="44">
         <f>AVERAGE(Q4:Q15)</f>
@@ -2640,7 +2673,7 @@
       </c>
       <c r="S18" s="44">
         <f>AVERAGE(S4:S15)</f>
-        <v>42.495000000000005</v>
+        <v>42.494000000000007</v>
       </c>
       <c r="T18" s="44">
         <f>AVERAGE(T4:T15)</f>
@@ -2648,43 +2681,43 @@
       </c>
       <c r="U18" s="44">
         <f t="shared" ref="U18:AA18" si="20">SUM(U4:U15)</f>
-        <v>15805.9759808</v>
+        <v>17397.865149699999</v>
       </c>
       <c r="V18" s="44">
         <f t="shared" si="20"/>
-        <v>13645.596199999998</v>
+        <v>14920.687099999997</v>
       </c>
       <c r="W18" s="44">
         <f t="shared" si="20"/>
-        <v>2996.6583000000001</v>
+        <v>3126.5309000000002</v>
       </c>
       <c r="X18" s="44">
         <f t="shared" si="20"/>
-        <v>2160.3797807999999</v>
+        <v>2477.1780497</v>
       </c>
       <c r="Y18" s="44">
         <f t="shared" si="20"/>
-        <v>5157.0380808</v>
+        <v>5603.7089496999997</v>
       </c>
       <c r="Z18" s="44">
         <f t="shared" si="20"/>
-        <v>4055.4</v>
+        <v>4227</v>
       </c>
       <c r="AA18" s="44">
         <f t="shared" si="20"/>
-        <v>9212.4380808000005</v>
+        <v>9830.7089497000015</v>
       </c>
       <c r="AB18" s="45">
         <f>AVERAGE(AB4:AB15)</f>
-        <v>1.0338071511310087</v>
+        <v>1.0249832918854014</v>
       </c>
       <c r="AC18" s="45">
         <f>AVERAGE(AC4:AC15)</f>
-        <v>0.90203333333333346</v>
+        <v>0.90536000000000016</v>
       </c>
       <c r="AD18" s="44">
         <f>SUM(AD4:AD15)</f>
-        <v>1500</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
@@ -2741,10 +2774,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="55" t="s">
+      <c r="O21" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="P21" s="55"/>
+      <c r="P21" s="53"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -2754,23 +2787,23 @@
     <row r="22" spans="1:30" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="47">
         <f>G18</f>
-        <v>9013.8970000000008</v>
+        <v>9638.61</v>
       </c>
       <c r="D22" s="47">
         <f>J18</f>
-        <v>6759</v>
+        <v>7045</v>
       </c>
       <c r="E22" s="47">
         <f>I18</f>
-        <v>11656</v>
+        <v>12609</v>
       </c>
       <c r="F22" s="47">
         <f>K18</f>
-        <v>13910.896999999999</v>
+        <v>15202.609999999999</v>
       </c>
       <c r="G22" s="47">
         <f>L18</f>
-        <v>2254.8969999999999</v>
+        <v>2593.6099999999997</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -2783,11 +2816,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="56">
+      <c r="O22" s="54">
         <f>G24/(G18)</f>
-        <v>1.0220261093287397</v>
-      </c>
-      <c r="P22" s="56"/>
+        <v>1.019930150685628</v>
+      </c>
+      <c r="P22" s="54"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -2816,7 +2849,7 @@
       <c r="F24" s="27"/>
       <c r="G24" s="49">
         <f>AA18+K22</f>
-        <v>9212.4380808000005</v>
+        <v>9830.7089497000015</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2842,7 +2875,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="48">
         <f>G24-AD18</f>
-        <v>7712.4380808000005</v>
+        <v>8030.7089497000015</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2854,16 +2887,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="N2:T2"/>
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="O22:P22"/>
     <mergeCell ref="U1:AC1"/>
     <mergeCell ref="U2:AC2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="N1:T1"/>
-    <mergeCell ref="N2:T2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Nov and Dec 2020
</commit_message>
<xml_diff>
--- a/PV_investment_electricity_cost.xlsx
+++ b/PV_investment_electricity_cost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ElectricityCalculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F036A3F3-CFB6-48A1-A551-7F32BF16F4E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DD1823-848F-4F61-B779-F74344557656}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
   </bookViews>
@@ -390,7 +390,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;????\ &quot;kr&quot;_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.000\ &quot;kr&quot;_-;\-* #,##0.000\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +500,12 @@
       <color rgb="FF21CC72"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -692,7 +698,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -782,18 +788,19 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1129,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1623E28-38CC-4E14-8F03-C1FE1A23361C}">
   <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,75 +1170,75 @@
         <v>2020</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55" t="s">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="55"/>
+      <c r="J1" s="53"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="55" t="s">
+      <c r="N1" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55" t="s">
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="N2" s="56" t="s">
+      <c r="J2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
     </row>
     <row r="3" spans="1:32" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -1357,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="20">
-        <f t="shared" ref="K4:K13" si="0">(G4/1000)+I4-J4</f>
+        <f t="shared" ref="K4:K15" si="0">(G4/1000)+I4-J4</f>
         <v>2451</v>
       </c>
       <c r="L4" s="20">
@@ -1459,7 +1466,7 @@
         <v>2291</v>
       </c>
       <c r="L5" s="20">
-        <f t="shared" ref="L5:L13" si="3">K5-I5</f>
+        <f t="shared" ref="L5:L15" si="3">K5-I5</f>
         <v>0</v>
       </c>
       <c r="M5" s="50">
@@ -1484,7 +1491,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
       <c r="U5" s="14">
-        <f t="shared" ref="U5:U13" si="5">(K5*(P5+Q5+R5)/100)+N5+O5</f>
+        <f t="shared" ref="U5:U15" si="5">(K5*(P5+Q5+R5)/100)+N5+O5</f>
         <v>2416.3252000000002</v>
       </c>
       <c r="V5" s="14">
@@ -2017,7 +2024,7 @@
         <v>0.82235144086324308</v>
       </c>
       <c r="AC10" s="35">
-        <f t="shared" ref="AC10:AC13" si="16">(P10+Q10+R10)/100</f>
+        <f t="shared" ref="AC10:AC15" si="16">(P10+Q10+R10)/100</f>
         <v>0.75560000000000005</v>
       </c>
       <c r="AD10" s="37">
@@ -2346,70 +2353,103 @@
       <c r="B14" s="52">
         <v>252</v>
       </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
+      <c r="C14" s="57">
+        <v>1639463</v>
+      </c>
+      <c r="D14" s="57">
+        <v>39270</v>
+      </c>
+      <c r="E14" s="57">
+        <v>1511986</v>
+      </c>
+      <c r="F14" s="57">
+        <v>127477</v>
+      </c>
+      <c r="G14" s="57">
+        <v>166747</v>
       </c>
       <c r="H14" s="22">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="50"/>
+        <v>0.66169444444444447</v>
+      </c>
+      <c r="I14" s="7">
+        <v>1512</v>
+      </c>
+      <c r="J14" s="7">
+        <v>39</v>
+      </c>
+      <c r="K14" s="20">
+        <f t="shared" si="0"/>
+        <v>1639.7470000000001</v>
+      </c>
+      <c r="L14" s="20">
+        <f t="shared" si="3"/>
+        <v>127.74700000000007</v>
+      </c>
+      <c r="M14" s="50">
+        <f t="shared" si="4"/>
+        <v>7.7906530702602325E-2</v>
+      </c>
       <c r="N14" s="18">
         <v>0</v>
       </c>
       <c r="O14" s="18">
-        <v>0</v>
-      </c>
-      <c r="P14" s="19"/>
+        <v>383.75</v>
+      </c>
+      <c r="P14" s="19">
+        <v>39.33</v>
+      </c>
       <c r="Q14" s="19">
         <v>14.4</v>
       </c>
       <c r="R14" s="19">
         <v>44.13</v>
       </c>
-      <c r="S14" s="19"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
+      <c r="S14" s="19">
+        <v>34.31</v>
+      </c>
+      <c r="T14" s="18">
+        <v>2.92</v>
+      </c>
+      <c r="U14" s="14">
+        <f t="shared" si="5"/>
+        <v>1988.4064142</v>
+      </c>
+      <c r="V14" s="14">
+        <f>(I14*(P14+Q14+R14)/100)+N14+O14</f>
+        <v>1863.3932</v>
+      </c>
       <c r="W14" s="14">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>14.519700000000002</v>
       </c>
       <c r="X14" s="15">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>125.01321419999999</v>
       </c>
       <c r="Y14" s="14">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>139.53291419999999</v>
       </c>
       <c r="Z14" s="15">
         <f>J14*0.6</f>
-        <v>0</v>
+        <v>23.4</v>
       </c>
       <c r="AA14" s="14">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AB14" s="35"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="37"/>
+        <v>162.9329142</v>
+      </c>
+      <c r="AB14" s="35">
+        <f t="shared" ref="AB14:AB15" si="19">AA14/(G14/1000)</f>
+        <v>0.97712651022207286</v>
+      </c>
+      <c r="AC14" s="15">
+        <f t="shared" si="16"/>
+        <v>0.97860000000000003</v>
+      </c>
+      <c r="AD14" s="37">
+        <v>300</v>
+      </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -2418,70 +2458,103 @@
       <c r="B15" s="52">
         <v>129</v>
       </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
+      <c r="C15" s="57">
+        <v>1968326</v>
+      </c>
+      <c r="D15" s="57">
+        <v>440</v>
+      </c>
+      <c r="E15" s="57">
+        <v>1943394</v>
+      </c>
+      <c r="F15" s="57">
+        <v>24932</v>
+      </c>
+      <c r="G15" s="57">
+        <v>25372</v>
       </c>
       <c r="H15" s="22">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="50"/>
+        <v>0.19668217054263565</v>
+      </c>
+      <c r="I15" s="7">
+        <v>1943</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="K15" s="20">
+        <f t="shared" si="0"/>
+        <v>1968.2080000000001</v>
+      </c>
+      <c r="L15" s="20">
+        <f t="shared" si="3"/>
+        <v>25.208000000000084</v>
+      </c>
+      <c r="M15" s="50">
+        <f t="shared" si="4"/>
+        <v>1.2807589441766359E-2</v>
+      </c>
       <c r="N15" s="18">
         <v>0</v>
       </c>
       <c r="O15" s="18">
-        <v>0</v>
-      </c>
-      <c r="P15" s="19"/>
+        <v>383.75</v>
+      </c>
+      <c r="P15" s="19">
+        <v>46.06</v>
+      </c>
       <c r="Q15" s="19">
         <v>14.4</v>
       </c>
       <c r="R15" s="19">
         <v>44.13</v>
       </c>
-      <c r="S15" s="19"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
+      <c r="S15" s="19">
+        <v>30.45</v>
+      </c>
+      <c r="T15" s="18">
+        <v>2.92</v>
+      </c>
+      <c r="U15" s="14">
+        <f t="shared" si="5"/>
+        <v>2442.2987472000004</v>
+      </c>
+      <c r="V15" s="14">
+        <f>(I15*(P15+Q15+R15)/100)+N15+O15</f>
+        <v>2415.9337</v>
+      </c>
       <c r="W15" s="14">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5.4726799999999992E-2</v>
       </c>
       <c r="X15" s="15">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>26.36504720000039</v>
       </c>
       <c r="Y15" s="14">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>26.419774000000391</v>
       </c>
       <c r="Z15" s="15">
         <f>J15*0.6</f>
-        <v>0</v>
+        <v>9.8400000000000001E-2</v>
       </c>
       <c r="AA15" s="14">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AB15" s="35"/>
-      <c r="AC15" s="15"/>
-      <c r="AD15" s="37"/>
+        <v>26.518174000000393</v>
+      </c>
+      <c r="AB15" s="35">
+        <f t="shared" si="19"/>
+        <v>1.0451747595775025</v>
+      </c>
+      <c r="AC15" s="15">
+        <f t="shared" si="16"/>
+        <v>1.0459000000000001</v>
+      </c>
+      <c r="AD15" s="37">
+        <v>300</v>
+      </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -2612,56 +2685,56 @@
       </c>
       <c r="C18" s="42">
         <f>SUM(C4:C17)/1000</f>
-        <v>5106.8559999999998</v>
+        <v>8714.6450000000004</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D4:D17)/1000</f>
-        <v>7258.0749999999998</v>
+        <v>7297.7849999999999</v>
       </c>
       <c r="E18" s="42">
         <f>SUM(E4:E17)/1000</f>
-        <v>2717.8139999999999</v>
+        <v>6173.1940000000004</v>
       </c>
       <c r="F18" s="42">
         <f>SUM(F4:F17)/1000</f>
-        <v>2374.0129999999999</v>
+        <v>2526.422</v>
       </c>
       <c r="G18" s="42">
         <f>SUM(G4:G17)/1000</f>
-        <v>9638.61</v>
+        <v>9830.7289999999994</v>
       </c>
       <c r="H18" s="42"/>
       <c r="I18" s="43">
-        <f t="shared" ref="I18:O18" si="19">SUM(I4:I15)</f>
-        <v>12609</v>
+        <f t="shared" ref="I18:O18" si="20">SUM(I4:I15)</f>
+        <v>16064</v>
       </c>
       <c r="J18" s="43">
-        <f t="shared" si="19"/>
-        <v>7045</v>
+        <f t="shared" si="20"/>
+        <v>7084.1639999999998</v>
       </c>
       <c r="K18" s="43">
-        <f t="shared" si="19"/>
-        <v>15202.609999999999</v>
+        <f t="shared" si="20"/>
+        <v>18810.564999999999</v>
       </c>
       <c r="L18" s="43">
-        <f t="shared" si="19"/>
-        <v>2593.6099999999997</v>
+        <f t="shared" si="20"/>
+        <v>2746.5650000000001</v>
       </c>
       <c r="M18" s="51">
         <f t="shared" si="4"/>
-        <v>0.17060294252105393</v>
+        <v>0.14601182899078258</v>
       </c>
       <c r="N18" s="43">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O18" s="44">
-        <f t="shared" si="19"/>
-        <v>3837.5</v>
+        <f t="shared" si="20"/>
+        <v>4605</v>
       </c>
       <c r="P18" s="44">
         <f>AVERAGE(P4:P15)</f>
-        <v>32.006</v>
+        <v>33.787500000000001</v>
       </c>
       <c r="Q18" s="44">
         <f>AVERAGE(Q4:Q15)</f>
@@ -2673,51 +2746,51 @@
       </c>
       <c r="S18" s="44">
         <f>AVERAGE(S4:S15)</f>
-        <v>42.494000000000007</v>
+        <v>39.604285714285716</v>
       </c>
       <c r="T18" s="44">
         <f>AVERAGE(T4:T15)</f>
-        <v>2.92</v>
+        <v>2.9199999999999995</v>
       </c>
       <c r="U18" s="44">
-        <f t="shared" ref="U18:AA18" si="20">SUM(U4:U15)</f>
-        <v>17397.865149699999</v>
+        <f t="shared" ref="U18:AA18" si="21">SUM(U4:U15)</f>
+        <v>21828.570311099997</v>
       </c>
       <c r="V18" s="44">
-        <f t="shared" si="20"/>
-        <v>14920.687099999997</v>
+        <f t="shared" si="21"/>
+        <v>19200.013999999999</v>
       </c>
       <c r="W18" s="44">
-        <f t="shared" si="20"/>
-        <v>3126.5309000000002</v>
+        <f t="shared" si="21"/>
+        <v>3141.1053268000001</v>
       </c>
       <c r="X18" s="44">
-        <f t="shared" si="20"/>
-        <v>2477.1780497</v>
+        <f t="shared" si="21"/>
+        <v>2628.5563111000006</v>
       </c>
       <c r="Y18" s="44">
-        <f t="shared" si="20"/>
-        <v>5603.7089496999997</v>
+        <f t="shared" si="21"/>
+        <v>5769.6616378999997</v>
       </c>
       <c r="Z18" s="44">
-        <f t="shared" si="20"/>
-        <v>4227</v>
+        <f t="shared" si="21"/>
+        <v>4250.4983999999995</v>
       </c>
       <c r="AA18" s="44">
-        <f t="shared" si="20"/>
-        <v>9830.7089497000015</v>
+        <f t="shared" si="21"/>
+        <v>10020.160037900003</v>
       </c>
       <c r="AB18" s="45">
         <f>AVERAGE(AB4:AB15)</f>
-        <v>1.0249832918854014</v>
+        <v>1.021031104175226</v>
       </c>
       <c r="AC18" s="45">
         <f>AVERAGE(AC4:AC15)</f>
-        <v>0.90536000000000016</v>
+        <v>0.92317500000000008</v>
       </c>
       <c r="AD18" s="44">
         <f>SUM(AD4:AD15)</f>
-        <v>1800</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
@@ -2774,10 +2847,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="53" t="s">
+      <c r="O21" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="P21" s="53"/>
+      <c r="P21" s="55"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -2787,23 +2860,23 @@
     <row r="22" spans="1:30" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="47">
         <f>G18</f>
-        <v>9638.61</v>
+        <v>9830.7289999999994</v>
       </c>
       <c r="D22" s="47">
         <f>J18</f>
-        <v>7045</v>
+        <v>7084.1639999999998</v>
       </c>
       <c r="E22" s="47">
         <f>I18</f>
-        <v>12609</v>
+        <v>16064</v>
       </c>
       <c r="F22" s="47">
         <f>K18</f>
-        <v>15202.609999999999</v>
+        <v>18810.564999999999</v>
       </c>
       <c r="G22" s="47">
         <f>L18</f>
-        <v>2593.6099999999997</v>
+        <v>2746.5650000000001</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -2816,11 +2889,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="54">
+      <c r="O22" s="56">
         <f>G24/(G18)</f>
-        <v>1.019930150685628</v>
-      </c>
-      <c r="P22" s="54"/>
+        <v>1.0192692767647245</v>
+      </c>
+      <c r="P22" s="56"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -2849,7 +2922,7 @@
       <c r="F24" s="27"/>
       <c r="G24" s="49">
         <f>AA18+K22</f>
-        <v>9830.7089497000015</v>
+        <v>10020.160037900003</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2875,7 +2948,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="48">
         <f>G24-AD18</f>
-        <v>8030.7089497000015</v>
+        <v>7620.1600379000029</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2887,16 +2960,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="U1:AC1"/>
+    <mergeCell ref="U2:AC2"/>
+    <mergeCell ref="I2:J2"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="N1:T1"/>
     <mergeCell ref="N2:T2"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="U1:AC1"/>
-    <mergeCell ref="U2:AC2"/>
-    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding actual energy cost
</commit_message>
<xml_diff>
--- a/PV_investment_electricity_cost.xlsx
+++ b/PV_investment_electricity_cost.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ElectricityCalculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DD1823-848F-4F61-B779-F74344557656}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126A2383-F0AD-490E-9F75-3F0CE18723A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity 2020" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -114,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB3" authorId="0" shapeId="0" xr:uid="{B02FA356-B083-43AD-ABF5-E9CEB24B2DF3}">
+    <comment ref="AC3" authorId="0" shapeId="0" xr:uid="{B02FA356-B083-43AD-ABF5-E9CEB24B2DF3}">
       <text>
         <r>
           <rPr>
@@ -138,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD3" authorId="0" shapeId="0" xr:uid="{2971E639-60A4-4DF2-84FB-60FBFF742701}">
+    <comment ref="AE3" authorId="0" shapeId="0" xr:uid="{2971E639-60A4-4DF2-84FB-60FBFF742701}">
       <text>
         <r>
           <rPr>
@@ -183,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>kWh</t>
   </si>
@@ -297,12 +298,6 @@
     <t>Tax return</t>
   </si>
   <si>
-    <t>Virtual electricity cost (SEK)</t>
-  </si>
-  <si>
-    <t>Actual Electricity Cost (SEK)</t>
-  </si>
-  <si>
     <t>SEK</t>
   </si>
   <si>
@@ -377,6 +372,15 @@
   </si>
   <si>
     <t>Percentage of selfconsumption (%)</t>
+  </si>
+  <si>
+    <t>Virtual electricity bill (SEK)</t>
+  </si>
+  <si>
+    <t>Actual Electricity bill (SEK)</t>
+  </si>
+  <si>
+    <t>Net Cost of electricity (SEK)</t>
   </si>
 </sst>
 </file>
@@ -698,7 +702,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -794,13 +798,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1134,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1623E28-38CC-4E14-8F03-C1FE1A23361C}">
-  <dimension ref="A1:AF28"/>
+  <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,94 +1167,97 @@
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" customWidth="1"/>
-    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="15.85546875" customWidth="1"/>
-    <col min="30" max="30" width="11.85546875" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" customWidth="1"/>
+    <col min="24" max="24" width="11" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" customWidth="1"/>
+    <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="15.85546875" customWidth="1"/>
+    <col min="31" max="31" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="10">
         <v>2020</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="53"/>
+      <c r="J1" s="58"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="53" t="s">
+      <c r="N1" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53" t="s">
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C2" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C2" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="J2" s="59"/>
+      <c r="N2" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-    </row>
-    <row r="3" spans="1:32" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+    </row>
+    <row r="3" spans="1:33" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>3</v>
@@ -1260,10 +1275,10 @@
         <v>7</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>21</v>
@@ -1272,10 +1287,10 @@
         <v>22</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N3" s="16" t="s">
         <v>25</v>
@@ -1299,39 +1314,42 @@
         <v>31</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="V3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="X3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="Y3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="Z3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Z3" s="13" t="s">
+      <c r="AA3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AA3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB3" s="12" t="s">
-        <v>44</v>
+      <c r="AB3" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD3" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE3" s="11"/>
+        <v>42</v>
+      </c>
+      <c r="AD3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE3" s="36" t="s">
+        <v>51</v>
+      </c>
       <c r="AF3" s="11"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG3" s="11"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1393,43 +1411,47 @@
       <c r="S4" s="19"/>
       <c r="T4" s="19"/>
       <c r="U4" s="14">
+        <f>P4*I4/100</f>
+        <v>894.61500000000001</v>
+      </c>
+      <c r="V4" s="14">
         <f>(K4*(P4+Q4+R4)/100)+N4+O4</f>
         <v>2712.9353000000001</v>
       </c>
-      <c r="V4" s="14">
-        <f t="shared" ref="V4:V8" si="1">(I4*(P4+Q4+R4)/100)+N4+O4</f>
+      <c r="W4" s="14">
+        <f t="shared" ref="W4:W8" si="1">(I4*(P4+Q4+R4)/100)+N4+O4</f>
         <v>2712.9353000000001</v>
       </c>
-      <c r="W4" s="14">
+      <c r="X4" s="14">
         <f>J4*(S4+T4)/100</f>
         <v>0</v>
       </c>
-      <c r="X4" s="14">
-        <f t="shared" ref="X4:X8" si="2">U4-V4</f>
-        <v>0</v>
-      </c>
       <c r="Y4" s="14">
-        <f>W4+X4</f>
-        <v>0</v>
-      </c>
-      <c r="Z4" s="15">
+        <f t="shared" ref="Y4:Y8" si="2">V4-W4</f>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="14">
+        <f>X4+Y4</f>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="15">
         <f>J4*0.6</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="14">
-        <f>Z4+Y4</f>
-        <v>0</v>
-      </c>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="35">
+      <c r="AB4" s="14">
+        <f>AA4+Z4</f>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="35">
         <f>(P4+Q4+R4)/100</f>
         <v>0.95030000000000003</v>
       </c>
-      <c r="AD4" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE4" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1491,43 +1513,47 @@
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
       <c r="U5" s="14">
-        <f t="shared" ref="U5:U15" si="5">(K5*(P5+Q5+R5)/100)+N5+O5</f>
+        <f t="shared" ref="U5:U15" si="5">P5*I5/100</f>
+        <v>691.65290000000005</v>
+      </c>
+      <c r="V5" s="14">
+        <f t="shared" ref="V5:V15" si="6">(K5*(P5+Q5+R5)/100)+N5+O5</f>
         <v>2416.3252000000002</v>
       </c>
-      <c r="V5" s="14">
+      <c r="W5" s="14">
         <f t="shared" si="1"/>
         <v>2416.3252000000002</v>
       </c>
-      <c r="W5" s="14">
-        <f t="shared" ref="W5:W9" si="6">J5*(S5+T5)/100</f>
-        <v>0</v>
-      </c>
       <c r="X5" s="14">
+        <f t="shared" ref="X5:X9" si="7">J5*(S5+T5)/100</f>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y5" s="14">
-        <f t="shared" ref="Y5:Y9" si="7">W5+X5</f>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="15">
-        <f t="shared" ref="Z5:Z9" si="8">J5*0.6</f>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="14">
-        <f t="shared" ref="AA5:AA9" si="9">Z5+Y5</f>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="35">
-        <f t="shared" ref="AC5:AC9" si="10">(P5+Q5+R5)/100</f>
+      <c r="Z5" s="14">
+        <f t="shared" ref="Z5:Z9" si="8">X5+Y5</f>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="15">
+        <f t="shared" ref="AA5:AA9" si="9">J5*0.6</f>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="14">
+        <f t="shared" ref="AB5:AB9" si="10">AA5+Z5</f>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="35">
+        <f t="shared" ref="AD5:AD9" si="11">(P5+Q5+R5)/100</f>
         <v>0.88719999999999999</v>
       </c>
-      <c r="AD5" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE5" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1590,42 +1616,46 @@
       <c r="T6" s="19"/>
       <c r="U6" s="14">
         <f t="shared" si="5"/>
+        <v>537.25979999999993</v>
+      </c>
+      <c r="V6" s="14">
+        <f t="shared" si="6"/>
         <v>2227.9847</v>
       </c>
-      <c r="V6" s="14">
+      <c r="W6" s="14">
         <f t="shared" si="1"/>
         <v>2227.9847</v>
       </c>
-      <c r="W6" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="X6" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y6" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z6" s="15">
+      <c r="Z6" s="14">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="14">
+      <c r="AA6" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="35">
+      <c r="AB6" s="14">
         <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="35">
+        <f t="shared" si="11"/>
         <v>0.82590000000000008</v>
       </c>
-      <c r="AD6" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE6" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1688,42 +1718,46 @@
       <c r="T7" s="19"/>
       <c r="U7" s="14">
         <f t="shared" si="5"/>
+        <v>283.87839999999994</v>
+      </c>
+      <c r="V7" s="14">
+        <f t="shared" si="6"/>
         <v>1641.5676000000001</v>
       </c>
-      <c r="V7" s="14">
+      <c r="W7" s="14">
         <f t="shared" si="1"/>
         <v>1641.5676000000001</v>
       </c>
-      <c r="W7" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="X7" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y7" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z7" s="15">
+      <c r="Z7" s="14">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AA7" s="14">
+      <c r="AA7" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AB7" s="15"/>
-      <c r="AC7" s="35">
+      <c r="AB7" s="14">
         <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="35">
+        <f t="shared" si="11"/>
         <v>0.75590000000000002</v>
       </c>
-      <c r="AD7" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE7" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1786,42 +1820,46 @@
       <c r="T8" s="19"/>
       <c r="U8" s="14">
         <f t="shared" si="5"/>
+        <v>328.18239999999997</v>
+      </c>
+      <c r="V8" s="14">
+        <f t="shared" si="6"/>
         <v>1564.1291999999999</v>
       </c>
-      <c r="V8" s="14">
+      <c r="W8" s="14">
         <f t="shared" si="1"/>
         <v>1564.1291999999999</v>
       </c>
-      <c r="W8" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="X8" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y8" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z8" s="15">
+      <c r="Z8" s="14">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AA8" s="14">
+      <c r="AA8" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AB8" s="15"/>
-      <c r="AC8" s="35">
+      <c r="AB8" s="14">
         <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="35">
+        <f t="shared" si="11"/>
         <v>0.81069999999999998</v>
       </c>
-      <c r="AD8" s="37">
+      <c r="AE8" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1888,45 +1926,49 @@
       </c>
       <c r="U9" s="14">
         <f t="shared" si="5"/>
+        <v>137.9376</v>
+      </c>
+      <c r="V9" s="14">
+        <f t="shared" si="6"/>
         <v>1337.258969</v>
       </c>
-      <c r="V9" s="14">
-        <f>(I9*(P9+Q9+R9)/100)+N9+O9</f>
+      <c r="W9" s="14">
+        <f t="shared" ref="W9:W15" si="12">(I9*(P9+Q9+R9)/100)+N9+O9</f>
         <v>739.41920000000005</v>
       </c>
-      <c r="W9" s="14">
-        <f t="shared" si="6"/>
+      <c r="X9" s="14">
+        <f t="shared" si="7"/>
         <v>906.01699999999994</v>
       </c>
-      <c r="X9" s="14">
-        <f>U9-V9</f>
+      <c r="Y9" s="14">
+        <f>V9-W9</f>
         <v>597.83976899999993</v>
       </c>
-      <c r="Y9" s="14">
-        <f t="shared" si="7"/>
+      <c r="Z9" s="14">
+        <f t="shared" si="8"/>
         <v>1503.856769</v>
       </c>
-      <c r="Z9" s="15">
-        <f t="shared" si="8"/>
+      <c r="AA9" s="15">
+        <f t="shared" si="9"/>
         <v>1119</v>
       </c>
-      <c r="AA9" s="14">
-        <f t="shared" si="9"/>
+      <c r="AB9" s="14">
+        <f t="shared" si="10"/>
         <v>2622.856769</v>
       </c>
-      <c r="AB9" s="35">
-        <f>AA9/(G9/1000)</f>
+      <c r="AC9" s="35">
+        <f>AB9/(G9/1000)</f>
         <v>1.0532334663834333</v>
       </c>
-      <c r="AC9" s="35">
-        <f t="shared" si="10"/>
+      <c r="AD9" s="35">
+        <f t="shared" si="11"/>
         <v>0.95609999999999995</v>
       </c>
-      <c r="AD9" s="37">
+      <c r="AE9" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1949,7 +1991,7 @@
         <v>2627765</v>
       </c>
       <c r="H10" s="22">
-        <f t="shared" ref="H10:H15" si="11">(G10/1000)/B10</f>
+        <f t="shared" ref="H10:H15" si="13">(G10/1000)/B10</f>
         <v>1.0091263440860214</v>
       </c>
       <c r="I10" s="7">
@@ -1993,45 +2035,49 @@
       </c>
       <c r="U10" s="14">
         <f t="shared" si="5"/>
+        <v>51.600900000000003</v>
+      </c>
+      <c r="V10" s="14">
+        <f t="shared" si="6"/>
         <v>1093.8364339999998</v>
       </c>
-      <c r="V10" s="14">
-        <f>(I10*(P10+Q10+R10)/100)+N10+O10</f>
+      <c r="W10" s="14">
+        <f t="shared" si="12"/>
         <v>612.69679999999994</v>
       </c>
-      <c r="W10" s="14">
-        <f t="shared" ref="W10:W15" si="12">J10*(S10+T10)/100</f>
+      <c r="X10" s="14">
+        <f t="shared" ref="X10:X15" si="14">J10*(S10+T10)/100</f>
         <v>485.20669999999996</v>
       </c>
-      <c r="X10" s="14">
-        <f>U10-V10</f>
+      <c r="Y10" s="14">
+        <f>V10-W10</f>
         <v>481.13963399999989</v>
       </c>
-      <c r="Y10" s="14">
-        <f t="shared" ref="Y10:Y11" si="13">W10+X10</f>
+      <c r="Z10" s="14">
+        <f t="shared" ref="Z10:Z11" si="15">X10+Y10</f>
         <v>966.34633399999984</v>
       </c>
-      <c r="Z10" s="15">
-        <f t="shared" ref="Z10:Z11" si="14">J10*0.6</f>
+      <c r="AA10" s="15">
+        <f t="shared" ref="AA10:AA11" si="16">J10*0.6</f>
         <v>1194.5999999999999</v>
       </c>
-      <c r="AA10" s="14">
-        <f t="shared" ref="AA10:AA15" si="15">Z10+Y10</f>
+      <c r="AB10" s="14">
+        <f t="shared" ref="AB10:AB15" si="17">AA10+Z10</f>
         <v>2160.9463339999998</v>
       </c>
-      <c r="AB10" s="35">
-        <f>AA10/(G10/1000)</f>
+      <c r="AC10" s="35">
+        <f>AB10/(G10/1000)</f>
         <v>0.82235144086324308</v>
       </c>
-      <c r="AC10" s="35">
-        <f t="shared" ref="AC10:AC15" si="16">(P10+Q10+R10)/100</f>
+      <c r="AD10" s="35">
+        <f t="shared" ref="AD10:AD15" si="18">(P10+Q10+R10)/100</f>
         <v>0.75560000000000005</v>
       </c>
-      <c r="AD10" s="37">
+      <c r="AE10" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -2054,7 +2100,7 @@
         <v>2451407</v>
       </c>
       <c r="H11" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.1281210308329499</v>
       </c>
       <c r="I11" s="7">
@@ -2098,45 +2144,49 @@
       </c>
       <c r="U11" s="14">
         <f t="shared" si="5"/>
+        <v>175.63949999999997</v>
+      </c>
+      <c r="V11" s="14">
+        <f t="shared" si="6"/>
         <v>1384.4770208000002</v>
-      </c>
-      <c r="V11" s="14">
-        <f>(I11*(P11+Q11+R11)/100)+N11+O11</f>
-        <v>761.31799999999998</v>
       </c>
       <c r="W11" s="14">
         <f t="shared" si="12"/>
+        <v>761.31799999999998</v>
+      </c>
+      <c r="X11" s="14">
+        <f t="shared" si="14"/>
         <v>1083.0910000000001</v>
       </c>
-      <c r="X11" s="15">
-        <f>U11-V11</f>
+      <c r="Y11" s="15">
+        <f>V11-W11</f>
         <v>623.15902080000023</v>
       </c>
-      <c r="Y11" s="14">
-        <f t="shared" si="13"/>
+      <c r="Z11" s="14">
+        <f t="shared" si="15"/>
         <v>1706.2500208000004</v>
       </c>
-      <c r="Z11" s="15">
-        <f t="shared" si="14"/>
+      <c r="AA11" s="15">
+        <f t="shared" si="16"/>
         <v>1129.2</v>
       </c>
-      <c r="AA11" s="14">
-        <f t="shared" si="15"/>
+      <c r="AB11" s="14">
+        <f t="shared" si="17"/>
         <v>2835.4500208000004</v>
       </c>
-      <c r="AB11" s="35">
-        <f>AA11/(G11/1000)</f>
+      <c r="AC11" s="35">
+        <f>AB11/(G11/1000)</f>
         <v>1.1566622844758134</v>
       </c>
-      <c r="AC11" s="15">
-        <f t="shared" si="16"/>
+      <c r="AD11" s="15">
+        <f t="shared" si="18"/>
         <v>1.0944</v>
       </c>
-      <c r="AD11" s="37">
+      <c r="AE11" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -2159,7 +2209,7 @@
         <v>1444435</v>
       </c>
       <c r="H12" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.87594602789569431</v>
       </c>
       <c r="I12" s="7">
@@ -2203,45 +2253,49 @@
       </c>
       <c r="U12" s="14">
         <f t="shared" si="5"/>
+        <v>268.82289999999995</v>
+      </c>
+      <c r="V12" s="14">
+        <f t="shared" si="6"/>
         <v>1427.4615569999999</v>
-      </c>
-      <c r="V12" s="14">
-        <f>(I12*(P12+Q12+R12)/100)+N12+O12</f>
-        <v>969.22019999999998</v>
       </c>
       <c r="W12" s="14">
         <f t="shared" si="12"/>
+        <v>969.22019999999998</v>
+      </c>
+      <c r="X12" s="14">
+        <f t="shared" si="14"/>
         <v>522.34360000000004</v>
       </c>
-      <c r="X12" s="15">
-        <f t="shared" ref="X12:X15" si="17">U12-V12</f>
+      <c r="Y12" s="15">
+        <f t="shared" ref="Y12:Y15" si="19">V12-W12</f>
         <v>458.24135699999988</v>
       </c>
-      <c r="Y12" s="14">
-        <f t="shared" ref="Y12:Y15" si="18">W12+X12</f>
+      <c r="Z12" s="14">
+        <f t="shared" ref="Z12:Z15" si="20">X12+Y12</f>
         <v>980.58495699999992</v>
       </c>
-      <c r="Z12" s="15">
+      <c r="AA12" s="15">
         <f>J12*0.6</f>
         <v>612.6</v>
       </c>
-      <c r="AA12" s="14">
-        <f t="shared" si="15"/>
+      <c r="AB12" s="14">
+        <f t="shared" si="17"/>
         <v>1593.1849569999999</v>
       </c>
-      <c r="AB12" s="35">
-        <f>AA12/(G12/1000)</f>
+      <c r="AC12" s="35">
+        <f>AB12/(G12/1000)</f>
         <v>1.1029814128015452</v>
       </c>
-      <c r="AC12" s="15">
-        <f t="shared" si="16"/>
+      <c r="AD12" s="15">
+        <f t="shared" si="18"/>
         <v>1.0822000000000001</v>
       </c>
-      <c r="AD12" s="37">
+      <c r="AE12" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -2264,7 +2318,7 @@
         <v>624713</v>
       </c>
       <c r="H13" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.79581273885350312</v>
       </c>
       <c r="I13" s="7">
@@ -2308,68 +2362,72 @@
       </c>
       <c r="U13" s="14">
         <f t="shared" si="5"/>
+        <v>333.55</v>
+      </c>
+      <c r="V13" s="14">
+        <f t="shared" si="6"/>
         <v>1591.8891689</v>
-      </c>
-      <c r="V13" s="14">
-        <f>(I13*(P13+Q13+R13)/100)+N13+O13</f>
-        <v>1275.0908999999999</v>
       </c>
       <c r="W13" s="14">
         <f t="shared" si="12"/>
+        <v>1275.0908999999999</v>
+      </c>
+      <c r="X13" s="14">
+        <f t="shared" si="14"/>
         <v>129.87260000000001</v>
       </c>
-      <c r="X13" s="15">
-        <f t="shared" si="17"/>
+      <c r="Y13" s="15">
+        <f t="shared" si="19"/>
         <v>316.79826890000004</v>
       </c>
-      <c r="Y13" s="14">
-        <f t="shared" si="18"/>
+      <c r="Z13" s="14">
+        <f t="shared" si="20"/>
         <v>446.67086890000007</v>
       </c>
-      <c r="Z13" s="15">
+      <c r="AA13" s="15">
         <f>J13*0.6</f>
         <v>171.6</v>
       </c>
-      <c r="AA13" s="14">
-        <f t="shared" si="15"/>
+      <c r="AB13" s="14">
+        <f t="shared" si="17"/>
         <v>618.2708689000001</v>
       </c>
-      <c r="AB13" s="35">
-        <f>AA13/(G13/1000)</f>
+      <c r="AC13" s="35">
+        <f>AB13/(G13/1000)</f>
         <v>0.98968785490297162</v>
       </c>
-      <c r="AC13" s="15">
-        <f t="shared" si="16"/>
+      <c r="AD13" s="15">
+        <f t="shared" si="18"/>
         <v>0.93530000000000002</v>
       </c>
-      <c r="AD13" s="37">
+      <c r="AE13" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="52">
         <v>252</v>
       </c>
-      <c r="C14" s="57">
+      <c r="C14" s="55">
         <v>1639463</v>
       </c>
-      <c r="D14" s="57">
+      <c r="D14" s="55">
         <v>39270</v>
       </c>
-      <c r="E14" s="57">
+      <c r="E14" s="55">
         <v>1511986</v>
       </c>
-      <c r="F14" s="57">
+      <c r="F14" s="55">
         <v>127477</v>
       </c>
-      <c r="G14" s="57">
+      <c r="G14" s="55">
         <v>166747</v>
       </c>
       <c r="H14" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.66169444444444447</v>
       </c>
       <c r="I14" s="7">
@@ -2413,68 +2471,72 @@
       </c>
       <c r="U14" s="14">
         <f t="shared" si="5"/>
+        <v>594.66959999999995</v>
+      </c>
+      <c r="V14" s="14">
+        <f t="shared" si="6"/>
         <v>1988.4064142</v>
-      </c>
-      <c r="V14" s="14">
-        <f>(I14*(P14+Q14+R14)/100)+N14+O14</f>
-        <v>1863.3932</v>
       </c>
       <c r="W14" s="14">
         <f t="shared" si="12"/>
+        <v>1863.3932</v>
+      </c>
+      <c r="X14" s="14">
+        <f t="shared" si="14"/>
         <v>14.519700000000002</v>
       </c>
-      <c r="X14" s="15">
-        <f t="shared" si="17"/>
+      <c r="Y14" s="15">
+        <f t="shared" si="19"/>
         <v>125.01321419999999</v>
       </c>
-      <c r="Y14" s="14">
-        <f t="shared" si="18"/>
+      <c r="Z14" s="14">
+        <f t="shared" si="20"/>
         <v>139.53291419999999</v>
       </c>
-      <c r="Z14" s="15">
+      <c r="AA14" s="15">
         <f>J14*0.6</f>
         <v>23.4</v>
       </c>
-      <c r="AA14" s="14">
-        <f t="shared" si="15"/>
+      <c r="AB14" s="14">
+        <f t="shared" si="17"/>
         <v>162.9329142</v>
       </c>
-      <c r="AB14" s="35">
-        <f t="shared" ref="AB14:AB15" si="19">AA14/(G14/1000)</f>
+      <c r="AC14" s="35">
+        <f t="shared" ref="AC14:AC15" si="21">AB14/(G14/1000)</f>
         <v>0.97712651022207286</v>
       </c>
-      <c r="AC14" s="15">
-        <f t="shared" si="16"/>
+      <c r="AD14" s="15">
+        <f t="shared" si="18"/>
         <v>0.97860000000000003</v>
       </c>
-      <c r="AD14" s="37">
+      <c r="AE14" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="52">
         <v>129</v>
       </c>
-      <c r="C15" s="57">
+      <c r="C15" s="55">
         <v>1968326</v>
       </c>
-      <c r="D15" s="57">
+      <c r="D15" s="55">
         <v>440</v>
       </c>
-      <c r="E15" s="57">
+      <c r="E15" s="55">
         <v>1943394</v>
       </c>
-      <c r="F15" s="57">
+      <c r="F15" s="55">
         <v>24932</v>
       </c>
-      <c r="G15" s="57">
+      <c r="G15" s="55">
         <v>25372</v>
       </c>
       <c r="H15" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.19668217054263565</v>
       </c>
       <c r="I15" s="7">
@@ -2518,45 +2580,49 @@
       </c>
       <c r="U15" s="14">
         <f t="shared" si="5"/>
+        <v>894.94579999999996</v>
+      </c>
+      <c r="V15" s="14">
+        <f t="shared" si="6"/>
         <v>2442.2987472000004</v>
-      </c>
-      <c r="V15" s="14">
-        <f>(I15*(P15+Q15+R15)/100)+N15+O15</f>
-        <v>2415.9337</v>
       </c>
       <c r="W15" s="14">
         <f t="shared" si="12"/>
+        <v>2415.9337</v>
+      </c>
+      <c r="X15" s="14">
+        <f t="shared" si="14"/>
         <v>5.4726799999999992E-2</v>
       </c>
-      <c r="X15" s="15">
-        <f t="shared" si="17"/>
+      <c r="Y15" s="15">
+        <f t="shared" si="19"/>
         <v>26.36504720000039</v>
       </c>
-      <c r="Y15" s="14">
-        <f t="shared" si="18"/>
+      <c r="Z15" s="14">
+        <f t="shared" si="20"/>
         <v>26.419774000000391</v>
       </c>
-      <c r="Z15" s="15">
+      <c r="AA15" s="15">
         <f>J15*0.6</f>
         <v>9.8400000000000001E-2</v>
       </c>
-      <c r="AA15" s="14">
-        <f t="shared" si="15"/>
+      <c r="AB15" s="14">
+        <f t="shared" si="17"/>
         <v>26.518174000000393</v>
       </c>
-      <c r="AB15" s="35">
-        <f t="shared" si="19"/>
+      <c r="AC15" s="35">
+        <f t="shared" si="21"/>
         <v>1.0451747595775025</v>
       </c>
-      <c r="AC15" s="15">
-        <f t="shared" si="16"/>
+      <c r="AD15" s="15">
+        <f t="shared" si="18"/>
         <v>1.0459000000000001</v>
       </c>
-      <c r="AD15" s="37">
+      <c r="AE15" s="37">
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="21"/>
       <c r="C16" s="3"/>
@@ -2577,18 +2643,19 @@
       <c r="R16" s="19"/>
       <c r="S16" s="19"/>
       <c r="T16" s="18"/>
-      <c r="U16" s="14"/>
+      <c r="U16" s="15"/>
       <c r="V16" s="14"/>
       <c r="W16" s="14"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="35"/>
-      <c r="AC16" s="15"/>
-      <c r="AD16" s="37"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="X16" s="14"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="35"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="37"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
         <v>0</v>
       </c>
@@ -2624,58 +2691,59 @@
         <v>0</v>
       </c>
       <c r="N17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="P17" s="39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q17" s="39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R17" s="39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="S17" s="39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T17" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="U17" s="39" t="s">
-        <v>39</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="U17" s="39"/>
       <c r="V17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="W17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="X17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Y17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Z17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AA17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AB17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AC17" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AD17" s="39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="AE17" s="39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
         <v>23</v>
       </c>
@@ -2705,19 +2773,19 @@
       </c>
       <c r="H18" s="42"/>
       <c r="I18" s="43">
-        <f t="shared" ref="I18:O18" si="20">SUM(I4:I15)</f>
+        <f t="shared" ref="I18:O18" si="22">SUM(I4:I15)</f>
         <v>16064</v>
       </c>
       <c r="J18" s="43">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>7084.1639999999998</v>
       </c>
       <c r="K18" s="43">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>18810.564999999999</v>
       </c>
       <c r="L18" s="43">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2746.5650000000001</v>
       </c>
       <c r="M18" s="51">
@@ -2725,11 +2793,11 @@
         <v>0.14601182899078258</v>
       </c>
       <c r="N18" s="43">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O18" s="44">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>4605</v>
       </c>
       <c r="P18" s="44">
@@ -2753,47 +2821,51 @@
         <v>2.9199999999999995</v>
       </c>
       <c r="U18" s="44">
-        <f t="shared" ref="U18:AA18" si="21">SUM(U4:U15)</f>
+        <f>SUM(U4:U15)</f>
+        <v>5192.7548000000006</v>
+      </c>
+      <c r="V18" s="44">
+        <f t="shared" ref="V18:AB18" si="23">SUM(V4:V15)</f>
         <v>21828.570311099997</v>
       </c>
-      <c r="V18" s="44">
-        <f t="shared" si="21"/>
+      <c r="W18" s="44">
+        <f t="shared" si="23"/>
         <v>19200.013999999999</v>
       </c>
-      <c r="W18" s="44">
-        <f t="shared" si="21"/>
+      <c r="X18" s="44">
+        <f t="shared" si="23"/>
         <v>3141.1053268000001</v>
       </c>
-      <c r="X18" s="44">
-        <f t="shared" si="21"/>
+      <c r="Y18" s="44">
+        <f t="shared" si="23"/>
         <v>2628.5563111000006</v>
       </c>
-      <c r="Y18" s="44">
-        <f t="shared" si="21"/>
+      <c r="Z18" s="44">
+        <f t="shared" si="23"/>
         <v>5769.6616378999997</v>
       </c>
-      <c r="Z18" s="44">
-        <f t="shared" si="21"/>
+      <c r="AA18" s="44">
+        <f t="shared" si="23"/>
         <v>4250.4983999999995</v>
       </c>
-      <c r="AA18" s="44">
-        <f t="shared" si="21"/>
+      <c r="AB18" s="44">
+        <f t="shared" si="23"/>
         <v>10020.160037900003</v>
-      </c>
-      <c r="AB18" s="45">
-        <f>AVERAGE(AB4:AB15)</f>
-        <v>1.021031104175226</v>
       </c>
       <c r="AC18" s="45">
         <f>AVERAGE(AC4:AC15)</f>
+        <v>1.021031104175226</v>
+      </c>
+      <c r="AD18" s="45">
+        <f>AVERAGE(AD4:AD15)</f>
         <v>0.92317500000000008</v>
       </c>
-      <c r="AD18" s="44">
-        <f>SUM(AD4:AD15)</f>
+      <c r="AE18" s="44">
+        <f>SUM(AE4:AE15)</f>
         <v>2400</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -2807,8 +2879,9 @@
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
-    </row>
-    <row r="20" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V19" s="6"/>
+    </row>
+    <row r="20" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -2822,42 +2895,44 @@
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
-    </row>
-    <row r="21" spans="1:30" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V20" s="6"/>
+    </row>
+    <row r="21" spans="1:31" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="F21" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="46" t="s">
-        <v>48</v>
-      </c>
       <c r="G21" s="46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="P21" s="55"/>
+      <c r="O21" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="P21" s="56"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
-    </row>
-    <row r="22" spans="1:30" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V21" s="6"/>
+    </row>
+    <row r="22" spans="1:31" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="47">
         <f>G18</f>
         <v>9830.7289999999994</v>
@@ -2889,69 +2964,71 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="56">
+      <c r="O22" s="57">
         <f>G24/(G18)</f>
         <v>1.0192692767647245</v>
       </c>
-      <c r="P22" s="56"/>
+      <c r="P22" s="57"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="V22" s="61"/>
+      <c r="W22" s="60"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C23" s="23"/>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="25"/>
       <c r="K23" s="33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" ht="21" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="21" x14ac:dyDescent="0.35">
       <c r="C24" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
       <c r="G24" s="49">
-        <f>AA18+K22</f>
+        <f>AB18+K22</f>
         <v>10020.160037900003</v>
       </c>
     </row>
-    <row r="25" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="28"/>
       <c r="D25" s="29"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
       <c r="G25" s="31"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C26" s="23"/>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="25"/>
     </row>
-    <row r="27" spans="1:30" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" ht="21" x14ac:dyDescent="0.35">
       <c r="C27" s="32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="48">
-        <f>G24-AD18</f>
+        <f>G24-AE18</f>
         <v>7620.1600379000029</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="28"/>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
@@ -2960,16 +3037,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="U1:AC1"/>
-    <mergeCell ref="U2:AC2"/>
-    <mergeCell ref="I2:J2"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="N1:T1"/>
     <mergeCell ref="N2:T2"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="V1:AD1"/>
+    <mergeCell ref="V2:AD2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2979,4 +3056,148 @@
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EF3DC6-BC91-401A-8695-9FDC77CDF10D}">
+  <dimension ref="D5:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="19">
+        <v>45.66</v>
+      </c>
+      <c r="H5">
+        <f>E5*I5</f>
+        <v>85155.9</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="19">
+        <v>21.45</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H11" si="0">E6*I6</f>
+        <v>42706.95</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="19">
+        <v>54.63</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>102813.66</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="19">
+        <v>48.24</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>49253.04</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="19">
+        <v>42.49</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>12152.140000000001</v>
+      </c>
+      <c r="I9" s="7">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="19">
+        <v>34.31</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1338.0900000000001</v>
+      </c>
+      <c r="I10" s="7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="19">
+        <v>30.45</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>4.9938000000000002</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="60">
+        <f>AVERAGE(E5:E12)</f>
+        <v>39.604285714285716</v>
+      </c>
+      <c r="H13">
+        <f>SUM(H5:H12)</f>
+        <v>293424.77380000002</v>
+      </c>
+      <c r="I13">
+        <f>SUM(I5:I12)</f>
+        <v>7084.1639999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f>H13/I13</f>
+        <v>41.419816621975443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: Internal</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated numbers for August 2022
</commit_message>
<xml_diff>
--- a/PV_investment_electricity_cost.xlsx
+++ b/PV_investment_electricity_cost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeveloperArea\ElectricityCalculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F769996-34EA-4372-8424-B36D86C9F669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A11D441-1234-4FBA-BA77-656FEB3549F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8325" yWindow="2685" windowWidth="24735" windowHeight="12630" activeTab="2" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity 2020" sheetId="2" r:id="rId1"/>
@@ -1096,11 +1096,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1108,11 +1108,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1547,7 +1547,7 @@
       <c r="R2" s="63"/>
       <c r="S2" s="63"/>
       <c r="T2" s="63"/>
-      <c r="U2" s="64" t="s">
+      <c r="U2" s="60" t="s">
         <v>67</v>
       </c>
       <c r="V2" s="59"/>
@@ -2096,43 +2096,43 @@
         <v>37.08</v>
       </c>
       <c r="V9" s="14">
-        <f>P9*I9/100</f>
+        <f t="shared" ref="V9:V15" si="3">P9*I9/100</f>
         <v>137.9376</v>
       </c>
       <c r="W9" s="14">
-        <f t="shared" ref="W5:W15" si="3">U9*I9/100</f>
+        <f t="shared" ref="W9:W15" si="4">U9*I9/100</f>
         <v>137.9376</v>
       </c>
       <c r="X9" s="14">
-        <f t="shared" ref="X4:X14" si="4">(K9*(U9+Q9+R9)/100)+N9+O9</f>
+        <f t="shared" ref="X9:X14" si="5">(K9*(U9+Q9+R9)/100)+N9+O9</f>
         <v>1337.258969</v>
       </c>
       <c r="Y9" s="14">
-        <f>(O9+((Q9+R9)*I9/100)+V9)-Z9</f>
+        <f t="shared" ref="Y9:Y15" si="6">(O9+((Q9+R9)*I9/100)+V9)-Z9</f>
         <v>-166.59780000000001</v>
       </c>
       <c r="Z9" s="14">
-        <f>J9*(S9+T9)/100</f>
+        <f t="shared" ref="Z9:Z15" si="7">J9*(S9+T9)/100</f>
         <v>906.01699999999994</v>
       </c>
       <c r="AA9" s="14">
-        <f t="shared" ref="AA4:AA15" si="5">X9-Y9</f>
+        <f t="shared" ref="AA9:AA15" si="8">X9-Y9</f>
         <v>1503.856769</v>
       </c>
       <c r="AB9" s="15">
-        <f>J9*0.6</f>
+        <f t="shared" ref="AB9:AB15" si="9">J9*0.6</f>
         <v>1119</v>
       </c>
       <c r="AC9" s="14">
-        <f t="shared" ref="AC8:AC14" si="6">AA9+AB9</f>
+        <f t="shared" ref="AC9:AC14" si="10">AA9+AB9</f>
         <v>2622.856769</v>
       </c>
       <c r="AD9" s="35">
-        <f>AC9/(G9/1000)</f>
+        <f t="shared" ref="AD9:AD15" si="11">AC9/(G9/1000)</f>
         <v>1.0532334663834333</v>
       </c>
       <c r="AE9" s="35">
-        <f>(P9+Q9+R9)/100</f>
+        <f t="shared" ref="AE9:AE15" si="12">(P9+Q9+R9)/100</f>
         <v>0.95609999999999995</v>
       </c>
       <c r="AF9" s="37">
@@ -2162,7 +2162,7 @@
         <v>2627765</v>
       </c>
       <c r="H10" s="22">
-        <f t="shared" ref="H10:H15" si="7">(G10/1000)/B10</f>
+        <f t="shared" ref="H10:H15" si="13">(G10/1000)/B10</f>
         <v>1.0091263440860214</v>
       </c>
       <c r="I10" s="7">
@@ -2208,43 +2208,43 @@
         <v>17.03</v>
       </c>
       <c r="V10" s="14">
-        <f>P10*I10/100</f>
-        <v>51.600900000000003</v>
-      </c>
-      <c r="W10" s="14">
         <f t="shared" si="3"/>
         <v>51.600900000000003</v>
       </c>
+      <c r="W10" s="14">
+        <f t="shared" si="4"/>
+        <v>51.600900000000003</v>
+      </c>
       <c r="X10" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1093.8364339999998</v>
       </c>
       <c r="Y10" s="14">
-        <f>(O10+((Q10+R10)*I10/100)+V10)-Z10</f>
+        <f t="shared" si="6"/>
         <v>127.4901000000001</v>
       </c>
       <c r="Z10" s="14">
-        <f>J10*(S10+T10)/100</f>
+        <f t="shared" si="7"/>
         <v>485.20669999999996</v>
       </c>
       <c r="AA10" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>966.34633399999973</v>
       </c>
       <c r="AB10" s="15">
-        <f>J10*0.6</f>
+        <f t="shared" si="9"/>
         <v>1194.5999999999999</v>
       </c>
       <c r="AC10" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2160.9463339999998</v>
       </c>
       <c r="AD10" s="35">
-        <f>AC10/(G10/1000)</f>
+        <f t="shared" si="11"/>
         <v>0.82235144086324308</v>
       </c>
       <c r="AE10" s="35">
-        <f>(P10+Q10+R10)/100</f>
+        <f t="shared" si="12"/>
         <v>0.75560000000000005</v>
       </c>
       <c r="AF10" s="37">
@@ -2274,7 +2274,7 @@
         <v>2451407</v>
       </c>
       <c r="H11" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>1.1281210308329499</v>
       </c>
       <c r="I11" s="7">
@@ -2320,43 +2320,43 @@
         <v>50.91</v>
       </c>
       <c r="V11" s="14">
-        <f>P11*I11/100</f>
-        <v>175.63949999999997</v>
-      </c>
-      <c r="W11" s="14">
         <f t="shared" si="3"/>
         <v>175.63949999999997</v>
       </c>
+      <c r="W11" s="14">
+        <f t="shared" si="4"/>
+        <v>175.63949999999997</v>
+      </c>
       <c r="X11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1384.4770208000002</v>
       </c>
       <c r="Y11" s="14">
-        <f>(O11+((Q11+R11)*I11/100)+V11)-Z11</f>
+        <f t="shared" si="6"/>
         <v>-321.77300000000014</v>
       </c>
       <c r="Z11" s="14">
-        <f>J11*(S11+T11)/100</f>
+        <f t="shared" si="7"/>
         <v>1083.0910000000001</v>
       </c>
       <c r="AA11" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1706.2500208000004</v>
       </c>
       <c r="AB11" s="15">
-        <f>J11*0.6</f>
+        <f t="shared" si="9"/>
         <v>1129.2</v>
       </c>
       <c r="AC11" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2835.4500208000004</v>
       </c>
       <c r="AD11" s="35">
-        <f>AC11/(G11/1000)</f>
+        <f t="shared" si="11"/>
         <v>1.1566622844758134</v>
       </c>
       <c r="AE11" s="35">
-        <f>(P11+Q11+R11)/100</f>
+        <f t="shared" si="12"/>
         <v>1.0944</v>
       </c>
       <c r="AF11" s="37">
@@ -2386,7 +2386,7 @@
         <v>1444435</v>
       </c>
       <c r="H12" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.87594602789569431</v>
       </c>
       <c r="I12" s="7">
@@ -2432,43 +2432,43 @@
         <v>49.69</v>
       </c>
       <c r="V12" s="14">
-        <f>P12*I12/100</f>
-        <v>268.82289999999995</v>
-      </c>
-      <c r="W12" s="14">
         <f t="shared" si="3"/>
         <v>268.82289999999995</v>
       </c>
+      <c r="W12" s="14">
+        <f t="shared" si="4"/>
+        <v>268.82289999999995</v>
+      </c>
       <c r="X12" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1427.4615569999999</v>
       </c>
       <c r="Y12" s="14">
-        <f>(O12+((Q12+R12)*I12/100)+V12)-Z12</f>
+        <f t="shared" si="6"/>
         <v>446.87659999999994</v>
       </c>
       <c r="Z12" s="14">
-        <f>J12*(S12+T12)/100</f>
+        <f t="shared" si="7"/>
         <v>522.34360000000004</v>
       </c>
       <c r="AA12" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>980.58495699999992</v>
       </c>
       <c r="AB12" s="15">
-        <f>J12*0.6</f>
+        <f t="shared" si="9"/>
         <v>612.6</v>
       </c>
       <c r="AC12" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1593.1849569999999</v>
       </c>
       <c r="AD12" s="35">
-        <f>AC12/(G12/1000)</f>
+        <f t="shared" si="11"/>
         <v>1.1029814128015452</v>
       </c>
       <c r="AE12" s="35">
-        <f>(P12+Q12+R12)/100</f>
+        <f t="shared" si="12"/>
         <v>1.0822000000000001</v>
       </c>
       <c r="AF12" s="37">
@@ -2498,7 +2498,7 @@
         <v>624713</v>
       </c>
       <c r="H13" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.79581273885350312</v>
       </c>
       <c r="I13" s="7">
@@ -2544,43 +2544,43 @@
         <v>35</v>
       </c>
       <c r="V13" s="14">
-        <f>P13*I13/100</f>
-        <v>333.55</v>
-      </c>
-      <c r="W13" s="14">
         <f t="shared" si="3"/>
         <v>333.55</v>
       </c>
+      <c r="W13" s="14">
+        <f t="shared" si="4"/>
+        <v>333.55</v>
+      </c>
       <c r="X13" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1591.8891689</v>
       </c>
       <c r="Y13" s="14">
-        <f>(O13+((Q13+R13)*I13/100)+V13)-Z13</f>
+        <f t="shared" si="6"/>
         <v>1145.2183000000002</v>
       </c>
       <c r="Z13" s="14">
-        <f>J13*(S13+T13)/100</f>
+        <f t="shared" si="7"/>
         <v>129.87260000000001</v>
       </c>
       <c r="AA13" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>446.67086889999973</v>
       </c>
       <c r="AB13" s="15">
-        <f>J13*0.6</f>
+        <f t="shared" si="9"/>
         <v>171.6</v>
       </c>
       <c r="AC13" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>618.27086889999975</v>
       </c>
       <c r="AD13" s="35">
-        <f>AC13/(G13/1000)</f>
+        <f t="shared" si="11"/>
         <v>0.98968785490297106</v>
       </c>
       <c r="AE13" s="35">
-        <f>(P13+Q13+R13)/100</f>
+        <f t="shared" si="12"/>
         <v>0.93530000000000002</v>
       </c>
       <c r="AF13" s="37">
@@ -2610,7 +2610,7 @@
         <v>166747</v>
       </c>
       <c r="H14" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.66169444444444447</v>
       </c>
       <c r="I14" s="7">
@@ -2656,43 +2656,43 @@
         <v>39.33</v>
       </c>
       <c r="V14" s="14">
-        <f>P14*I14/100</f>
-        <v>594.66959999999995</v>
-      </c>
-      <c r="W14" s="14">
         <f t="shared" si="3"/>
         <v>594.66959999999995</v>
       </c>
+      <c r="W14" s="14">
+        <f t="shared" si="4"/>
+        <v>594.66959999999995</v>
+      </c>
       <c r="X14" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1988.4064142</v>
       </c>
       <c r="Y14" s="14">
-        <f>(O14+((Q14+R14)*I14/100)+V14)-Z14</f>
+        <f t="shared" si="6"/>
         <v>1848.8734999999999</v>
       </c>
       <c r="Z14" s="14">
-        <f>J14*(S14+T14)/100</f>
+        <f t="shared" si="7"/>
         <v>14.519700000000002</v>
       </c>
       <c r="AA14" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>139.53291420000005</v>
       </c>
       <c r="AB14" s="15">
-        <f>J14*0.6</f>
+        <f t="shared" si="9"/>
         <v>23.4</v>
       </c>
       <c r="AC14" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>162.93291420000006</v>
       </c>
       <c r="AD14" s="35">
-        <f>AC14/(G14/1000)</f>
+        <f t="shared" si="11"/>
         <v>0.9771265102220732</v>
       </c>
       <c r="AE14" s="35">
-        <f>(P14+Q14+R14)/100</f>
+        <f t="shared" si="12"/>
         <v>0.97860000000000003</v>
       </c>
       <c r="AF14" s="37">
@@ -2722,7 +2722,7 @@
         <v>25372</v>
       </c>
       <c r="H15" s="22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.19668217054263565</v>
       </c>
       <c r="I15" s="7">
@@ -2768,11 +2768,11 @@
         <v>46.06</v>
       </c>
       <c r="V15" s="14">
-        <f>P15*I15/100</f>
+        <f t="shared" si="3"/>
         <v>894.94579999999996</v>
       </c>
       <c r="W15" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>894.94579999999996</v>
       </c>
       <c r="X15" s="14">
@@ -2780,19 +2780,19 @@
         <v>2442.2987472000004</v>
       </c>
       <c r="Y15" s="14">
-        <f>(O15+((Q15+R15)*I15/100)+V15)-Z15</f>
+        <f t="shared" si="6"/>
         <v>2415.8789732</v>
       </c>
       <c r="Z15" s="14">
-        <f>J15*(S15+T15)/100</f>
+        <f t="shared" si="7"/>
         <v>5.4726799999999992E-2</v>
       </c>
       <c r="AA15" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>26.419774000000416</v>
       </c>
       <c r="AB15" s="15">
-        <f>J15*0.6</f>
+        <f t="shared" si="9"/>
         <v>9.8400000000000001E-2</v>
       </c>
       <c r="AC15" s="14">
@@ -2800,11 +2800,11 @@
         <v>26.518174000000418</v>
       </c>
       <c r="AD15" s="35">
-        <f>AC15/(G15/1000)</f>
+        <f t="shared" si="11"/>
         <v>1.0451747595775034</v>
       </c>
       <c r="AE15" s="35">
-        <f>(P15+Q15+R15)/100</f>
+        <f t="shared" si="12"/>
         <v>1.0459000000000001</v>
       </c>
       <c r="AF15" s="37">
@@ -2964,19 +2964,19 @@
       </c>
       <c r="H18" s="42"/>
       <c r="I18" s="43">
-        <f t="shared" ref="I18:O18" si="8">SUM(I4:I15)</f>
+        <f t="shared" ref="I18:O18" si="14">SUM(I4:I15)</f>
         <v>16064</v>
       </c>
       <c r="J18" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>7084.1639999999998</v>
       </c>
       <c r="K18" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>18810.564999999999</v>
       </c>
       <c r="L18" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>2746.5650000000001</v>
       </c>
       <c r="M18" s="51">
@@ -2984,11 +2984,11 @@
         <v>0.14601182899078258</v>
       </c>
       <c r="N18" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O18" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>4605</v>
       </c>
       <c r="P18" s="44">
@@ -3013,35 +3013,35 @@
       </c>
       <c r="U18" s="44"/>
       <c r="V18" s="44">
-        <f t="shared" ref="V18:AC18" si="9">SUM(V4:V15)</f>
+        <f t="shared" ref="V18:AC18" si="15">SUM(V4:V15)</f>
         <v>2457.1662999999999</v>
       </c>
       <c r="W18" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>2457.1662999999999</v>
       </c>
       <c r="X18" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>11265.628311100001</v>
       </c>
       <c r="Y18" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>5495.9666732000005</v>
       </c>
       <c r="Z18" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>3141.1053268000001</v>
       </c>
       <c r="AA18" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>5769.6616379000006</v>
       </c>
       <c r="AB18" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4250.4983999999995</v>
       </c>
       <c r="AC18" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>10020.160037900001</v>
       </c>
       <c r="AD18" s="45"/>
@@ -3115,10 +3115,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="60" t="s">
+      <c r="O21" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="P21" s="60"/>
+      <c r="P21" s="64"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -3158,11 +3158,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="61">
+      <c r="O22" s="65">
         <f>G24/(G18)</f>
         <v>1.0192692767647242</v>
       </c>
-      <c r="P22" s="61"/>
+      <c r="P22" s="65"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -3231,16 +3231,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="X1:AE1"/>
+    <mergeCell ref="X2:AE2"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="N1:T1"/>
     <mergeCell ref="N2:T2"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="X1:AE1"/>
-    <mergeCell ref="X2:AE2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3350,7 +3350,7 @@
       <c r="R2" s="63"/>
       <c r="S2" s="63"/>
       <c r="T2" s="63"/>
-      <c r="U2" s="64" t="s">
+      <c r="U2" s="60" t="s">
         <v>67</v>
       </c>
       <c r="V2" s="55"/>
@@ -3530,7 +3530,7 @@
         <v>68.3</v>
       </c>
       <c r="V4" s="14">
-        <f>P4*I4/100</f>
+        <f t="shared" ref="V4:V15" si="1">P4*I4/100</f>
         <v>1396.0519999999999</v>
       </c>
       <c r="W4" s="14">
@@ -3538,35 +3538,35 @@
         <v>1396.0519999999999</v>
       </c>
       <c r="X4" s="14">
-        <f t="shared" ref="X4:X14" si="1">(K4*(U4+Q4+R4)/100)+N4+O4</f>
+        <f t="shared" ref="X4:X14" si="2">(K4*(U4+Q4+R4)/100)+N4+O4</f>
         <v>3035.6410400000004</v>
       </c>
       <c r="Y4" s="14">
-        <f>(O4+((Q4+R4)*I4/100)+V4)-Z4</f>
+        <f t="shared" ref="Y4:Y15" si="3">(O4+((Q4+R4)*I4/100)+V4)-Z4</f>
         <v>2982.4094</v>
       </c>
       <c r="Z4" s="14">
-        <f>J4*(S4+T4)/100</f>
+        <f t="shared" ref="Z4:Z15" si="4">J4*(S4+T4)/100</f>
         <v>1.3086000000000002</v>
       </c>
       <c r="AA4" s="14">
-        <f t="shared" ref="AA4" si="2">X4-Y4</f>
+        <f t="shared" ref="AA4" si="5">X4-Y4</f>
         <v>53.231640000000425</v>
       </c>
       <c r="AB4" s="15">
-        <f>J4*0.6</f>
+        <f t="shared" ref="AB4:AB15" si="6">J4*0.6</f>
         <v>1.7999999999999998</v>
       </c>
       <c r="AC4" s="14">
-        <f t="shared" ref="AC4:AC6" si="3">AA4+AB4</f>
+        <f t="shared" ref="AC4:AC6" si="7">AA4+AB4</f>
         <v>55.031640000000422</v>
       </c>
       <c r="AD4" s="35">
-        <f>AC4/(G4/1000)</f>
+        <f t="shared" ref="AD4:AD15" si="8">AC4/(G4/1000)</f>
         <v>1.2558566864445555</v>
       </c>
       <c r="AE4" s="35">
-        <f>(P4+Q4+R4)/100</f>
+        <f t="shared" ref="AE4:AE15" si="9">(P4+Q4+R4)/100</f>
         <v>1.272</v>
       </c>
       <c r="AF4" s="37">
@@ -3596,7 +3596,7 @@
         <v>431693</v>
       </c>
       <c r="H5" s="22">
-        <f t="shared" ref="H5:H15" si="4">(G5/1000)/B5</f>
+        <f t="shared" ref="H5:H15" si="10">(G5/1000)/B5</f>
         <v>0.75207839721254355</v>
       </c>
       <c r="I5" s="7">
@@ -3642,43 +3642,43 @@
         <v>76.540000000000006</v>
       </c>
       <c r="V5" s="14">
-        <f>P5*I5/100</f>
+        <f t="shared" si="1"/>
         <v>805.20080000000007</v>
       </c>
       <c r="W5" s="14">
-        <f t="shared" ref="W5:W15" si="5">U5*I5/100</f>
+        <f t="shared" ref="W5:W15" si="11">U5*I5/100</f>
         <v>805.20080000000007</v>
       </c>
       <c r="X5" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2343.1509992000001</v>
       </c>
       <c r="Y5" s="14">
-        <f>(O5+((Q5+R5)*I5/100)+V5)-Z5</f>
+        <f t="shared" si="3"/>
         <v>1781.5096000000001</v>
       </c>
       <c r="Z5" s="14">
-        <f>J5*(S5+T5)/100</f>
+        <f t="shared" si="4"/>
         <v>27.069200000000002</v>
       </c>
       <c r="AA5" s="14">
-        <f t="shared" ref="AA5" si="6">X5-Y5</f>
+        <f t="shared" ref="AA5" si="12">X5-Y5</f>
         <v>561.64139920000002</v>
       </c>
       <c r="AB5" s="15">
-        <f>J5*0.6</f>
+        <f t="shared" si="6"/>
         <v>22.2</v>
       </c>
       <c r="AC5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>583.84139920000007</v>
       </c>
       <c r="AD5" s="35">
-        <f>AC5/(G5/1000)</f>
+        <f t="shared" si="8"/>
         <v>1.3524458334974161</v>
       </c>
       <c r="AE5" s="35">
-        <f>(P5+Q5+R5)/100</f>
+        <f t="shared" si="9"/>
         <v>1.3544</v>
       </c>
       <c r="AF5" s="37">
@@ -3708,7 +3708,7 @@
         <v>1290145</v>
       </c>
       <c r="H6" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.92949927953890488</v>
       </c>
       <c r="I6" s="7">
@@ -3718,7 +3718,7 @@
         <v>282</v>
       </c>
       <c r="K6" s="20">
-        <f t="shared" ref="K6" si="7">(G6/1000)+I6-J6</f>
+        <f t="shared" ref="K6" si="13">(G6/1000)+I6-J6</f>
         <v>1219.145</v>
       </c>
       <c r="L6" s="20">
@@ -3754,43 +3754,43 @@
         <v>52.71</v>
       </c>
       <c r="V6" s="14">
-        <f>P6*I6/100</f>
+        <f t="shared" si="1"/>
         <v>111.21809999999999</v>
       </c>
       <c r="W6" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>111.21809999999999</v>
       </c>
       <c r="X6" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1744.4377345</v>
       </c>
       <c r="Y6" s="14">
-        <f>(O6+((Q6+R6)*I6/100)+V6)-Z6</f>
+        <f t="shared" si="3"/>
         <v>476.30130000000003</v>
       </c>
       <c r="Z6" s="14">
-        <f>J6*(S6+T6)/100</f>
+        <f t="shared" si="4"/>
         <v>142.94580000000002</v>
       </c>
       <c r="AA6" s="14">
-        <f t="shared" ref="AA6" si="8">X6-Y6</f>
+        <f t="shared" ref="AA6" si="14">X6-Y6</f>
         <v>1268.1364345</v>
       </c>
       <c r="AB6" s="15">
-        <f>J6*0.6</f>
+        <f t="shared" si="6"/>
         <v>169.2</v>
       </c>
       <c r="AC6" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1437.3364345</v>
       </c>
       <c r="AD6" s="35">
-        <f>AC6/(G6/1000)</f>
+        <f t="shared" si="8"/>
         <v>1.114089063244829</v>
       </c>
       <c r="AE6" s="35">
-        <f>(P6+Q6+R6)/100</f>
+        <f t="shared" si="9"/>
         <v>1.1161000000000001</v>
       </c>
       <c r="AF6" s="37">
@@ -3820,7 +3820,7 @@
         <v>2352377</v>
       </c>
       <c r="H7" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1.0376607851786501</v>
       </c>
       <c r="I7" s="7">
@@ -3830,15 +3830,15 @@
         <v>1044</v>
       </c>
       <c r="K7" s="20">
-        <f t="shared" ref="K7:K15" si="9">(G7/1000)+I7-J7</f>
+        <f t="shared" ref="K7:K15" si="15">(G7/1000)+I7-J7</f>
         <v>1319.0769999999998</v>
       </c>
       <c r="L7" s="20">
-        <f t="shared" ref="L7:L15" si="10">K7-I7</f>
+        <f t="shared" ref="L7:L15" si="16">K7-I7</f>
         <v>1308.3769999999997</v>
       </c>
       <c r="M7" s="50">
-        <f t="shared" ref="M7:M15" si="11">L7/K7</f>
+        <f t="shared" ref="M7:M15" si="17">L7/K7</f>
         <v>0.99188826732631985</v>
       </c>
       <c r="N7" s="18">
@@ -3866,31 +3866,31 @@
         <v>47.24</v>
       </c>
       <c r="V7" s="14">
-        <f>P7*I7/100</f>
+        <f t="shared" si="1"/>
         <v>5.0546799999999994</v>
       </c>
       <c r="W7" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>5.0546799999999994</v>
       </c>
       <c r="X7" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1783.8183277999997</v>
       </c>
       <c r="Y7" s="14">
-        <f>(O7+((Q7+R7)*I7/100)+V7)-Z7</f>
+        <f t="shared" si="3"/>
         <v>-128.98102000000006</v>
       </c>
       <c r="Z7" s="14">
-        <f>J7*(S7+T7)/100</f>
+        <f t="shared" si="4"/>
         <v>524.08800000000008</v>
       </c>
       <c r="AA7" s="14">
-        <f t="shared" ref="AA7:AA15" si="12">X7-Y7</f>
+        <f t="shared" ref="AA7:AA15" si="18">X7-Y7</f>
         <v>1912.7993477999999</v>
       </c>
       <c r="AB7" s="15">
-        <f>J7*0.6</f>
+        <f t="shared" si="6"/>
         <v>626.4</v>
       </c>
       <c r="AC7" s="14">
@@ -3898,11 +3898,11 @@
         <v>2539.1993477999999</v>
       </c>
       <c r="AD7" s="35">
-        <f>AC7/(G7/1000)</f>
+        <f t="shared" si="8"/>
         <v>1.0794185403955234</v>
       </c>
       <c r="AE7" s="35">
-        <f>(P7+Q7+R7)/100</f>
+        <f t="shared" si="9"/>
         <v>1.0613999999999999</v>
       </c>
       <c r="AF7" s="37">
@@ -3932,7 +3932,7 @@
         <v>2534976</v>
       </c>
       <c r="H8" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.79566101694915259</v>
       </c>
       <c r="I8" s="7">
@@ -3942,15 +3942,15 @@
         <v>1426</v>
       </c>
       <c r="K8" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1189.576</v>
       </c>
       <c r="L8" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1108.9760000000001</v>
       </c>
       <c r="M8" s="50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.9322447662024117</v>
       </c>
       <c r="N8" s="18">
@@ -3978,43 +3978,43 @@
         <v>62.99</v>
       </c>
       <c r="V8" s="14">
-        <f>P8*I8/100</f>
+        <f t="shared" si="1"/>
         <v>41.879759999999997</v>
       </c>
       <c r="W8" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>50.769939999999998</v>
       </c>
       <c r="X8" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1833.7241863999998</v>
       </c>
       <c r="Y8" s="14">
-        <f>(O8+((Q8+R8)*I8/100)+V8)-Z8</f>
+        <f t="shared" si="3"/>
         <v>-343.99484000000012</v>
       </c>
       <c r="Z8" s="14">
-        <f>J8*(S8+T8)/100</f>
+        <f t="shared" si="4"/>
         <v>817.09800000000007</v>
       </c>
       <c r="AA8" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2177.7190264000001</v>
       </c>
       <c r="AB8" s="15">
-        <f>J8*0.6</f>
+        <f t="shared" si="6"/>
         <v>855.6</v>
       </c>
       <c r="AC8" s="14">
-        <f t="shared" ref="AC8:AC15" si="13">AA8+AB8</f>
+        <f t="shared" ref="AC8:AC14" si="19">AA8+AB8</f>
         <v>3033.3190264</v>
       </c>
       <c r="AD8" s="35">
-        <f>AC8/(G8/1000)</f>
+        <f t="shared" si="8"/>
         <v>1.1965868814537099</v>
       </c>
       <c r="AE8" s="35">
-        <f>(P8+Q8+R8)/100</f>
+        <f t="shared" si="9"/>
         <v>1.1086</v>
       </c>
       <c r="AF8" s="37">
@@ -4044,7 +4044,7 @@
         <v>3304243</v>
       </c>
       <c r="H9" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1.0641684380032206</v>
       </c>
       <c r="I9" s="7">
@@ -4054,15 +4054,15 @@
         <v>2095</v>
       </c>
       <c r="K9" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1218.5430000000001</v>
       </c>
       <c r="L9" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1209.2430000000002</v>
       </c>
       <c r="M9" s="50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.99236793449225846</v>
       </c>
       <c r="N9" s="18">
@@ -4090,43 +4090,43 @@
         <v>58.5</v>
       </c>
       <c r="V9" s="14">
-        <f>P9*I9/100</f>
+        <f t="shared" si="1"/>
         <v>4.8704099999999997</v>
       </c>
       <c r="W9" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>5.440500000000001</v>
       </c>
       <c r="X9" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1814.3194820000001</v>
       </c>
       <c r="Y9" s="14">
-        <f>(O9+((Q9+R9)*I9/100)+V9)-Z9</f>
+        <f t="shared" si="3"/>
         <v>-853.26489000000004</v>
       </c>
       <c r="Z9" s="14">
-        <f>J9*(S9+T9)/100</f>
+        <f t="shared" si="4"/>
         <v>1247.3630000000001</v>
       </c>
       <c r="AA9" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2667.5843720000003</v>
       </c>
       <c r="AB9" s="15">
-        <f>J9*0.6</f>
+        <f t="shared" si="6"/>
         <v>1257</v>
       </c>
       <c r="AC9" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>3924.5843720000003</v>
       </c>
       <c r="AD9" s="35">
-        <f>AC9/(G9/1000)</f>
+        <f t="shared" si="8"/>
         <v>1.1877408447260085</v>
       </c>
       <c r="AE9" s="35">
-        <f>(P9+Q9+R9)/100</f>
+        <f t="shared" si="9"/>
         <v>1.1127</v>
       </c>
       <c r="AF9" s="37">
@@ -4156,7 +4156,7 @@
         <v>3235776</v>
       </c>
       <c r="H10" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1.0782325891369542</v>
       </c>
       <c r="I10" s="7">
@@ -4166,15 +4166,15 @@
         <v>2008</v>
       </c>
       <c r="K10" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1238.3759999999997</v>
       </c>
       <c r="L10" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1227.7759999999998</v>
       </c>
       <c r="M10" s="50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.99144040259178157</v>
       </c>
       <c r="N10" s="18">
@@ -4202,43 +4202,43 @@
         <v>82.1</v>
       </c>
       <c r="V10" s="14">
-        <f>P10*I10/100</f>
+        <f t="shared" si="1"/>
         <v>8.5213400000000004</v>
       </c>
       <c r="W10" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>8.7025999999999986</v>
       </c>
       <c r="X10" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2129.8601599999997</v>
       </c>
       <c r="Y10" s="14">
-        <f>(O10+((Q10+R10)*I10/100)+V10)-Z10</f>
+        <f t="shared" si="3"/>
         <v>-1163.7092599999999</v>
       </c>
       <c r="Z10" s="14">
-        <f>J10*(S10+T10)/100</f>
+        <f t="shared" si="4"/>
         <v>1562.2239999999999</v>
       </c>
       <c r="AA10" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>3293.5694199999998</v>
       </c>
       <c r="AB10" s="15">
-        <f>J10*0.6</f>
+        <f t="shared" si="6"/>
         <v>1204.8</v>
       </c>
       <c r="AC10" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>4498.36942</v>
       </c>
       <c r="AD10" s="35">
-        <f>AC10/(G10/1000)</f>
+        <f t="shared" si="8"/>
         <v>1.3901980297770922</v>
       </c>
       <c r="AE10" s="35">
-        <f>(P10+Q10+R10)/100</f>
+        <f t="shared" si="9"/>
         <v>1.3929000000000002</v>
       </c>
       <c r="AF10" s="37">
@@ -4268,7 +4268,7 @@
         <v>1996099</v>
       </c>
       <c r="H11" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.80390616190092623</v>
       </c>
       <c r="I11" s="7">
@@ -4278,15 +4278,15 @@
         <v>974</v>
       </c>
       <c r="K11" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1105.1990000000001</v>
       </c>
       <c r="L11" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1022.099</v>
       </c>
       <c r="M11" s="50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.9248099211092301</v>
       </c>
       <c r="N11" s="18">
@@ -4314,43 +4314,43 @@
         <v>92.79</v>
       </c>
       <c r="V11" s="14">
-        <f>P11*I11/100</f>
+        <f t="shared" si="1"/>
         <v>60.023130000000002</v>
       </c>
       <c r="W11" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>77.108490000000003</v>
       </c>
       <c r="X11" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2078.2523581</v>
       </c>
       <c r="Y11" s="14">
-        <f>(O11+((Q11+R11)*I11/100)+V11)-Z11</f>
+        <f t="shared" si="3"/>
         <v>-351.87507000000011</v>
       </c>
       <c r="Z11" s="14">
-        <f>J11*(S11+T11)/100</f>
+        <f t="shared" si="4"/>
         <v>857.50960000000009</v>
       </c>
       <c r="AA11" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2430.1274281000001</v>
       </c>
       <c r="AB11" s="15">
-        <f>J11*0.6</f>
+        <f t="shared" si="6"/>
         <v>584.4</v>
       </c>
       <c r="AC11" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>3014.5274281000002</v>
       </c>
       <c r="AD11" s="35">
-        <f>AC11/(G11/1000)</f>
+        <f t="shared" si="8"/>
         <v>1.5102093774406982</v>
       </c>
       <c r="AE11" s="35">
-        <f>(P11+Q11+R11)/100</f>
+        <f t="shared" si="9"/>
         <v>1.3163</v>
       </c>
       <c r="AF11" s="37">
@@ -4380,7 +4380,7 @@
         <v>1377694</v>
       </c>
       <c r="H12" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.83547240751970886</v>
       </c>
       <c r="I12" s="7">
@@ -4390,15 +4390,15 @@
         <v>544</v>
       </c>
       <c r="K12" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1081.694</v>
       </c>
       <c r="L12" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>833.69399999999996</v>
       </c>
       <c r="M12" s="50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.77072998463521103</v>
       </c>
       <c r="N12" s="18">
@@ -4426,43 +4426,43 @@
         <v>125.71</v>
       </c>
       <c r="V12" s="14">
-        <f>P12*I12/100</f>
+        <f t="shared" si="1"/>
         <v>193.81200000000001</v>
       </c>
       <c r="W12" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>311.76079999999996</v>
       </c>
       <c r="X12" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2398.5737633999997</v>
       </c>
       <c r="Y12" s="14">
-        <f>(O12+((Q12+R12)*I12/100)+V12)-Z12</f>
+        <f t="shared" si="3"/>
         <v>78.86200000000008</v>
       </c>
       <c r="Z12" s="14">
-        <f>J12*(S12+T12)/100</f>
+        <f t="shared" si="4"/>
         <v>658.51199999999994</v>
       </c>
       <c r="AA12" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2319.7117633999997</v>
       </c>
       <c r="AB12" s="15">
-        <f>J12*0.6</f>
+        <f t="shared" si="6"/>
         <v>326.39999999999998</v>
       </c>
       <c r="AC12" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2646.1117633999997</v>
       </c>
       <c r="AD12" s="35">
-        <f>AC12/(G12/1000)</f>
+        <f t="shared" si="8"/>
         <v>1.9206817794081994</v>
       </c>
       <c r="AE12" s="35">
-        <f>(P12+Q12+R12)/100</f>
+        <f t="shared" si="9"/>
         <v>1.3755000000000002</v>
       </c>
       <c r="AF12" s="37">
@@ -4492,7 +4492,7 @@
         <v>616306</v>
       </c>
       <c r="H13" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.78510318471337581</v>
       </c>
       <c r="I13" s="7">
@@ -4502,15 +4502,15 @@
         <v>139</v>
       </c>
       <c r="K13" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1727.306</v>
       </c>
       <c r="L13" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>477.30600000000004</v>
       </c>
       <c r="M13" s="50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.27632972964836572</v>
       </c>
       <c r="N13" s="18">
@@ -4538,43 +4538,43 @@
         <v>93.71</v>
       </c>
       <c r="V13" s="14">
-        <f>P13*I13/100</f>
+        <f t="shared" si="1"/>
         <v>440.75</v>
       </c>
       <c r="W13" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1171.3749999999998</v>
       </c>
       <c r="X13" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3040.9282166000003</v>
       </c>
       <c r="Y13" s="14">
-        <f>(O13+((Q13+R13)*I13/100)+V13)-Z13</f>
+        <f t="shared" si="3"/>
         <v>1419.7751000000001</v>
       </c>
       <c r="Z13" s="14">
-        <f>J13*(S13+T13)/100</f>
+        <f t="shared" si="4"/>
         <v>159.72489999999999</v>
       </c>
       <c r="AA13" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1621.1531166000002</v>
       </c>
       <c r="AB13" s="15">
-        <f>J13*0.6</f>
+        <f t="shared" si="6"/>
         <v>83.399999999999991</v>
       </c>
       <c r="AC13" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1704.5531166000003</v>
       </c>
       <c r="AD13" s="35">
-        <f>AC13/(G13/1000)</f>
+        <f t="shared" si="8"/>
         <v>2.7657577836334553</v>
       </c>
       <c r="AE13" s="35">
-        <f>(P13+Q13+R13)/100</f>
+        <f t="shared" si="9"/>
         <v>0.9466</v>
       </c>
       <c r="AF13" s="37">
@@ -4604,7 +4604,7 @@
         <v>198605</v>
       </c>
       <c r="H14" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.7881150793650793</v>
       </c>
       <c r="I14" s="7">
@@ -4614,15 +4614,15 @@
         <v>15.1</v>
       </c>
       <c r="K14" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1924.5050000000001</v>
       </c>
       <c r="L14" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>183.50500000000011</v>
       </c>
       <c r="M14" s="50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>9.5351791759439489E-2</v>
       </c>
       <c r="N14" s="18">
@@ -4650,43 +4650,43 @@
         <v>125.79</v>
       </c>
       <c r="V14" s="14">
-        <f>P14*I14/100</f>
+        <f t="shared" si="1"/>
         <v>1217.8295000000001</v>
       </c>
       <c r="W14" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>2190.0039000000002</v>
       </c>
       <c r="X14" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3960.2408095000005</v>
       </c>
       <c r="Y14" s="14">
-        <f>(O14+((Q14+R14)*I14/100)+V14)-Z14</f>
+        <f t="shared" si="3"/>
         <v>2636.3830200000002</v>
       </c>
       <c r="Z14" s="14">
-        <f>J14*(S14+T14)/100</f>
+        <f t="shared" si="4"/>
         <v>11.850479999999999</v>
       </c>
       <c r="AA14" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1323.8577895000003</v>
       </c>
       <c r="AB14" s="15">
-        <f>J14*0.6</f>
+        <f t="shared" si="6"/>
         <v>9.0599999999999987</v>
       </c>
       <c r="AC14" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1332.9177895000003</v>
       </c>
       <c r="AD14" s="35">
-        <f>AC14/(G14/1000)</f>
+        <f t="shared" si="8"/>
         <v>6.7114009692605938</v>
       </c>
       <c r="AE14" s="35">
-        <f>(P14+Q14+R14)/100</f>
+        <f t="shared" si="9"/>
         <v>1.2935000000000003</v>
       </c>
       <c r="AF14" s="37">
@@ -4716,7 +4716,7 @@
         <v>34869</v>
       </c>
       <c r="H15" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.27030232558139533</v>
       </c>
       <c r="I15" s="7">
@@ -4726,15 +4726,15 @@
         <v>7</v>
       </c>
       <c r="K15" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>2255.8690000000001</v>
       </c>
       <c r="L15" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>27.869000000000142</v>
       </c>
       <c r="M15" s="50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.2353997506060919E-2</v>
       </c>
       <c r="N15" s="18">
@@ -4763,11 +4763,11 @@
         <v>246.2</v>
       </c>
       <c r="V15" s="14">
-        <f>P15*I15/100</f>
+        <f t="shared" si="1"/>
         <v>3279.1704000000004</v>
       </c>
       <c r="W15" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>5485.3359999999993</v>
       </c>
       <c r="X15" s="14">
@@ -4775,19 +4775,19 @@
         <v>5290.1856640000005</v>
       </c>
       <c r="Y15" s="14">
-        <f>(O15+((Q15+R15)*I15/100)+V15)-Z15</f>
+        <f t="shared" si="3"/>
         <v>2980.7980000000002</v>
       </c>
       <c r="Z15" s="14">
-        <f>J15*(S15+T15)/100</f>
+        <f t="shared" si="4"/>
         <v>18.054400000000001</v>
       </c>
       <c r="AA15" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2309.3876640000003</v>
       </c>
       <c r="AB15" s="15">
-        <f>J15*0.6</f>
+        <f t="shared" si="6"/>
         <v>4.2</v>
       </c>
       <c r="AC15" s="14">
@@ -4795,11 +4795,11 @@
         <v>2313.5876640000001</v>
       </c>
       <c r="AD15" s="35">
-        <f>AC15/(G15/1000)</f>
+        <f t="shared" si="8"/>
         <v>66.350846425191435</v>
       </c>
       <c r="AE15" s="35">
-        <f>(P15+Q15+R15)/100</f>
+        <f t="shared" si="9"/>
         <v>2.0658000000000003</v>
       </c>
       <c r="AF15" s="37">
@@ -4959,31 +4959,31 @@
       </c>
       <c r="H18" s="42"/>
       <c r="I18" s="43">
-        <f t="shared" ref="I18:O18" si="14">SUM(I4:I15)</f>
+        <f t="shared" ref="I18:O18" si="20">SUM(I4:I15)</f>
         <v>8968.2999999999993</v>
       </c>
       <c r="J18" s="43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>8574.1</v>
       </c>
       <c r="K18" s="43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>17810.803</v>
       </c>
       <c r="L18" s="43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>8842.5030000000024</v>
       </c>
       <c r="M18" s="51">
-        <f t="shared" ref="M18" si="15">L18/K18</f>
+        <f t="shared" ref="M18" si="21">L18/K18</f>
         <v>0.49646851969560285</v>
       </c>
       <c r="N18" s="43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O18" s="44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>2667.5</v>
       </c>
       <c r="P18" s="44">
@@ -5008,35 +5008,35 @@
       </c>
       <c r="U18" s="44"/>
       <c r="V18" s="44">
-        <f t="shared" ref="V18:W18" si="16">SUM(V4:V15)</f>
+        <f t="shared" ref="V18:W18" si="22">SUM(V4:V15)</f>
         <v>7564.3821200000002</v>
       </c>
       <c r="W18" s="44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>11618.02281</v>
       </c>
       <c r="X18" s="44">
-        <f t="shared" ref="X18:AC18" si="17">SUM(X4:X15)</f>
+        <f t="shared" ref="X18:AC18" si="23">SUM(X4:X15)</f>
         <v>31453.132741500001</v>
       </c>
       <c r="Y18" s="44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>9514.2133400000002</v>
       </c>
       <c r="Z18" s="44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>6027.747980000001</v>
       </c>
       <c r="AA18" s="44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>21938.919401500003</v>
       </c>
       <c r="AB18" s="44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>5144.4599999999991</v>
       </c>
       <c r="AC18" s="44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>27083.379401500002</v>
       </c>
       <c r="AD18" s="45"/>
@@ -5113,10 +5113,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="60" t="s">
+      <c r="O21" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="P21" s="60"/>
+      <c r="P21" s="64"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -5158,11 +5158,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="61">
+      <c r="O22" s="65">
         <f>G24/(G18)</f>
         <v>1.5550322529312981</v>
       </c>
-      <c r="P22" s="61"/>
+      <c r="P22" s="65"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -5233,16 +5233,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="N1:T1"/>
     <mergeCell ref="X1:AE1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="N2:T2"/>
     <mergeCell ref="X2:AE2"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="N1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5254,7 +5254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973158C2-652A-42A8-8176-9FD76258C4A0}">
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
@@ -5351,7 +5351,7 @@
       <c r="R2" s="63"/>
       <c r="S2" s="63"/>
       <c r="T2" s="63"/>
-      <c r="U2" s="64" t="s">
+      <c r="U2" s="60" t="s">
         <v>67</v>
       </c>
       <c r="V2" s="59"/>
@@ -5425,7 +5425,7 @@
       <c r="T3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="65" t="s">
+      <c r="U3" s="61" t="s">
         <v>67</v>
       </c>
       <c r="V3" s="12" t="s">
@@ -5497,7 +5497,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="K4" s="20">
-        <f t="shared" ref="K4:K15" si="0">(G4/1000)+I4-J4</f>
+        <f t="shared" ref="K4:K10" si="0">(G4/1000)+I4-J4</f>
         <v>2204.1499999999996</v>
       </c>
       <c r="L4" s="20">
@@ -5534,7 +5534,7 @@
         <v>147.54</v>
       </c>
       <c r="V4" s="14">
-        <f>P4*I4/100</f>
+        <f t="shared" ref="V4:V11" si="1">P4*I4/100</f>
         <v>1896.8992000000001</v>
       </c>
       <c r="W4" s="14">
@@ -5542,35 +5542,35 @@
         <v>3139.6511999999998</v>
       </c>
       <c r="X4" s="14">
-        <f t="shared" ref="X4:X14" si="1">(K4*(U4+Q4+R4)/100)+N4+O4</f>
+        <f t="shared" ref="X4:X11" si="2">(K4*(U4+Q4+R4)/100)+N4+O4</f>
         <v>2968.5387599999995</v>
       </c>
       <c r="Y4" s="14">
-        <f>(O4+((Q4+R4)*I4/100)+V4)-Z4</f>
+        <f t="shared" ref="Y4:Y11" si="3">(O4+((Q4+R4)*I4/100)+V4)-Z4</f>
         <v>1554.05448</v>
       </c>
       <c r="Z4" s="14">
-        <f>J4*(S4+T4)/100</f>
+        <f t="shared" ref="Z4:Z11" si="4">J4*(S4+T4)/100</f>
         <v>13.766719999999999</v>
       </c>
       <c r="AA4" s="14">
-        <f t="shared" ref="AA4:AA15" si="2">X4-Y4</f>
+        <f t="shared" ref="AA4:AA11" si="5">X4-Y4</f>
         <v>1414.4842799999994</v>
       </c>
       <c r="AB4" s="15">
-        <f>J4*0.6</f>
+        <f t="shared" ref="AB4:AB11" si="6">J4*0.6</f>
         <v>5.28</v>
       </c>
       <c r="AC4" s="14">
-        <f t="shared" ref="AC4:AC6" si="3">AA4+AB4</f>
+        <f t="shared" ref="AC4:AC6" si="7">AA4+AB4</f>
         <v>1419.7642799999994</v>
       </c>
       <c r="AD4" s="35">
-        <f>AC4/(G4/1000)</f>
+        <f t="shared" ref="AD4:AD11" si="8">AC4/(G4/1000)</f>
         <v>16.712940317834011</v>
       </c>
       <c r="AE4" s="35">
-        <f>(P4+Q4+R4)/100</f>
+        <f t="shared" ref="AE4:AE11" si="9">(P4+Q4+R4)/100</f>
         <v>1.4904000000000002</v>
       </c>
       <c r="AF4" s="37">
@@ -5600,7 +5600,7 @@
         <v>473722</v>
       </c>
       <c r="H5" s="22">
-        <f t="shared" ref="H5:H15" si="4">(G5/1000)/B5</f>
+        <f t="shared" ref="H5:H11" si="10">(G5/1000)/B5</f>
         <v>0.82529965156794427</v>
       </c>
       <c r="I5" s="7">
@@ -5647,43 +5647,43 @@
         <v>110.28</v>
       </c>
       <c r="V5" s="14">
-        <f>P5*I5/100</f>
+        <f t="shared" si="1"/>
         <v>918.13959999999997</v>
       </c>
       <c r="W5" s="14">
-        <f t="shared" ref="W5:W15" si="5">U5*I5/100</f>
+        <f t="shared" ref="W5:W11" si="11">U5*I5/100</f>
         <v>1873.6572000000001</v>
       </c>
       <c r="X5" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2643.0088195999997</v>
       </c>
       <c r="Y5" s="14">
-        <f>(O5+((Q5+R5)*I5/100)+V5)-Z5</f>
+        <f t="shared" si="3"/>
         <v>927.87041999999997</v>
       </c>
       <c r="Z5" s="14">
-        <f>J5*(S5+T5)/100</f>
+        <f t="shared" si="4"/>
         <v>104.22017999999998</v>
       </c>
       <c r="AA5" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1715.1383995999997</v>
       </c>
       <c r="AB5" s="15">
-        <f>J5*0.6</f>
+        <f t="shared" si="6"/>
         <v>53.16</v>
       </c>
       <c r="AC5" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1768.2983995999998</v>
       </c>
       <c r="AD5" s="35">
-        <f>AC5/(G5/1000)</f>
+        <f t="shared" si="8"/>
         <v>3.7327766065329451</v>
       </c>
       <c r="AE5" s="35">
-        <f>(P5+Q5+R5)/100</f>
+        <f t="shared" si="9"/>
         <v>1.1394</v>
       </c>
       <c r="AF5" s="37">
@@ -5713,7 +5713,7 @@
         <v>1848604</v>
       </c>
       <c r="H6" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1.3318472622478386</v>
       </c>
       <c r="I6" s="7">
@@ -5760,43 +5760,43 @@
         <v>179.43</v>
       </c>
       <c r="V6" s="14">
-        <f>P6*I6/100</f>
+        <f t="shared" si="1"/>
         <v>862.10599999999988</v>
       </c>
       <c r="W6" s="14">
+        <f t="shared" si="11"/>
+        <v>1670.4933000000001</v>
+      </c>
+      <c r="X6" s="14">
+        <f t="shared" si="2"/>
+        <v>5788.4443532000005</v>
+      </c>
+      <c r="Y6" s="14">
+        <f t="shared" si="3"/>
+        <v>636.59629999999993</v>
+      </c>
+      <c r="Z6" s="14">
+        <f t="shared" si="4"/>
+        <v>979.42869999999994</v>
+      </c>
+      <c r="AA6" s="14">
         <f t="shared" si="5"/>
-        <v>1670.4933000000001</v>
-      </c>
-      <c r="X6" s="14">
-        <f t="shared" si="1"/>
-        <v>5788.4443532000005</v>
-      </c>
-      <c r="Y6" s="14">
-        <f>(O6+((Q6+R6)*I6/100)+V6)-Z6</f>
-        <v>636.59629999999993</v>
-      </c>
-      <c r="Z6" s="14">
-        <f>J6*(S6+T6)/100</f>
-        <v>979.42869999999994</v>
-      </c>
-      <c r="AA6" s="14">
-        <f t="shared" si="2"/>
         <v>5151.8480532000003</v>
       </c>
       <c r="AB6" s="15">
-        <f>J6*0.6</f>
+        <f t="shared" si="6"/>
         <v>265.8</v>
       </c>
       <c r="AC6" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>5417.6480532000005</v>
       </c>
       <c r="AD6" s="35">
-        <f>AC6/(G6/1000)</f>
+        <f t="shared" si="8"/>
         <v>2.9306698747811866</v>
       </c>
       <c r="AE6" s="35">
-        <f>(P6+Q6+R6)/100</f>
+        <f t="shared" si="9"/>
         <v>1.5249999999999999</v>
       </c>
       <c r="AF6" s="37">
@@ -5826,7 +5826,7 @@
         <v>2327419</v>
       </c>
       <c r="H7" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1.0266515218350243</v>
       </c>
       <c r="I7" s="7">
@@ -5840,11 +5840,11 @@
         <v>2354.4189999999999</v>
       </c>
       <c r="L7" s="20">
-        <f t="shared" ref="L7:L15" si="6">K7-I7</f>
+        <f t="shared" ref="L7:L10" si="12">K7-I7</f>
         <v>1701.4189999999999</v>
       </c>
       <c r="M7" s="50">
-        <f t="shared" ref="M7:M15" si="7">L7/K7</f>
+        <f t="shared" ref="M7:M10" si="13">L7/K7</f>
         <v>0.72264919710552789</v>
       </c>
       <c r="N7" s="18">
@@ -5872,31 +5872,31 @@
         <v>120.39</v>
       </c>
       <c r="V7" s="14">
-        <f>P7*I7/100</f>
+        <f t="shared" si="1"/>
         <v>488.05219999999991</v>
       </c>
       <c r="W7" s="14">
+        <f t="shared" si="11"/>
+        <v>786.14670000000001</v>
+      </c>
+      <c r="X7" s="14">
+        <f t="shared" si="2"/>
+        <v>4641.0320150999996</v>
+      </c>
+      <c r="Y7" s="14">
+        <f t="shared" si="3"/>
+        <v>533.70179999999993</v>
+      </c>
+      <c r="Z7" s="14">
+        <f t="shared" si="4"/>
+        <v>741.74739999999986</v>
+      </c>
+      <c r="AA7" s="14">
         <f t="shared" si="5"/>
-        <v>786.14670000000001</v>
-      </c>
-      <c r="X7" s="14">
-        <f t="shared" si="1"/>
-        <v>4641.0320150999996</v>
-      </c>
-      <c r="Y7" s="14">
-        <f>(O7+((Q7+R7)*I7/100)+V7)-Z7</f>
-        <v>533.70179999999993</v>
-      </c>
-      <c r="Z7" s="14">
-        <f>J7*(S7+T7)/100</f>
-        <v>741.74739999999986</v>
-      </c>
-      <c r="AA7" s="14">
-        <f t="shared" si="2"/>
         <v>4107.3302150999998</v>
       </c>
       <c r="AB7" s="15">
-        <f>J7*0.6</f>
+        <f t="shared" si="6"/>
         <v>375.59999999999997</v>
       </c>
       <c r="AC7" s="14">
@@ -5904,11 +5904,11 @@
         <v>4482.9302151000002</v>
       </c>
       <c r="AD7" s="35">
-        <f>AC7/(G7/1000)</f>
+        <f t="shared" si="8"/>
         <v>1.9261380160168842</v>
       </c>
       <c r="AE7" s="35">
-        <f>(P7+Q7+R7)/100</f>
+        <f t="shared" si="9"/>
         <v>1.3463999999999998</v>
       </c>
       <c r="AF7" s="37">
@@ -5938,7 +5938,7 @@
         <v>2977130</v>
       </c>
       <c r="H8" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.93444130571249218</v>
       </c>
       <c r="I8" s="7">
@@ -5952,11 +5952,11 @@
         <v>2158.13</v>
       </c>
       <c r="L8" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>1946.13</v>
       </c>
       <c r="M8" s="50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.90176680737490322</v>
       </c>
       <c r="N8" s="18">
@@ -5984,43 +5984,43 @@
         <v>139.09</v>
       </c>
       <c r="V8" s="14">
-        <f>P8*I8/100</f>
+        <f t="shared" si="1"/>
         <v>134.38679999999999</v>
       </c>
       <c r="W8" s="14">
+        <f t="shared" si="11"/>
+        <v>294.87080000000003</v>
+      </c>
+      <c r="X8" s="14">
+        <f t="shared" si="2"/>
+        <v>4736.033617</v>
+      </c>
+      <c r="Y8" s="14">
+        <f t="shared" si="3"/>
+        <v>-695.95640000000003</v>
+      </c>
+      <c r="Z8" s="14">
+        <f t="shared" si="4"/>
+        <v>1358.0332000000001</v>
+      </c>
+      <c r="AA8" s="14">
         <f t="shared" si="5"/>
-        <v>294.87080000000003</v>
-      </c>
-      <c r="X8" s="14">
-        <f t="shared" si="1"/>
-        <v>4736.033617</v>
-      </c>
-      <c r="Y8" s="14">
-        <f>(O8+((Q8+R8)*I8/100)+V8)-Z8</f>
-        <v>-695.95640000000003</v>
-      </c>
-      <c r="Z8" s="14">
-        <f>J8*(S8+T8)/100</f>
-        <v>1358.0332000000001</v>
-      </c>
-      <c r="AA8" s="14">
-        <f t="shared" si="2"/>
         <v>5431.9900170000001</v>
       </c>
       <c r="AB8" s="15">
-        <f>J8*0.6</f>
+        <f t="shared" si="6"/>
         <v>618.6</v>
       </c>
       <c r="AC8" s="14">
-        <f t="shared" ref="AC8:AC14" si="8">AA8+AB8</f>
+        <f t="shared" ref="AC8:AC11" si="14">AA8+AB8</f>
         <v>6050.5900170000004</v>
       </c>
       <c r="AD8" s="35">
-        <f>AC8/(G8/1000)</f>
+        <f t="shared" si="8"/>
         <v>2.0323566713579857</v>
       </c>
       <c r="AE8" s="35">
-        <f>(P8+Q8+R8)/100</f>
+        <f t="shared" si="9"/>
         <v>1.2539</v>
       </c>
       <c r="AF8" s="37">
@@ -6050,7 +6050,7 @@
         <v>3193807</v>
       </c>
       <c r="H9" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1.0286012882447664</v>
       </c>
       <c r="I9" s="7">
@@ -6064,11 +6064,11 @@
         <v>2054.8069999999998</v>
       </c>
       <c r="L9" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>1805.8069999999998</v>
       </c>
       <c r="M9" s="50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.87882073596206356</v>
       </c>
       <c r="N9" s="18">
@@ -6096,43 +6096,43 @@
         <v>171.86</v>
       </c>
       <c r="V9" s="14">
-        <f>P9*I9/100</f>
+        <f t="shared" si="1"/>
         <v>143.22480000000002</v>
       </c>
       <c r="W9" s="14">
+        <f t="shared" si="11"/>
+        <v>427.93140000000005</v>
+      </c>
+      <c r="X9" s="14">
+        <f t="shared" si="2"/>
+        <v>5201.6216501999997</v>
+      </c>
+      <c r="Y9" s="14">
+        <f t="shared" si="3"/>
+        <v>-1566.0868</v>
+      </c>
+      <c r="Z9" s="14">
+        <f t="shared" si="4"/>
+        <v>2259.9416000000001</v>
+      </c>
+      <c r="AA9" s="14">
         <f t="shared" si="5"/>
-        <v>427.93140000000005</v>
-      </c>
-      <c r="X9" s="14">
-        <f t="shared" si="1"/>
-        <v>5201.6216501999997</v>
-      </c>
-      <c r="Y9" s="14">
-        <f>(O9+((Q9+R9)*I9/100)+V9)-Z9</f>
-        <v>-1566.0868</v>
-      </c>
-      <c r="Z9" s="14">
-        <f>J9*(S9+T9)/100</f>
-        <v>2259.9416000000001</v>
-      </c>
-      <c r="AA9" s="14">
-        <f t="shared" si="2"/>
         <v>6767.7084501999998</v>
       </c>
       <c r="AB9" s="15">
-        <f>J9*0.6</f>
+        <f t="shared" si="6"/>
         <v>832.8</v>
       </c>
       <c r="AC9" s="14">
+        <f t="shared" si="14"/>
+        <v>7600.5084502</v>
+      </c>
+      <c r="AD9" s="35">
         <f t="shared" si="8"/>
-        <v>7600.5084502</v>
-      </c>
-      <c r="AD9" s="35">
-        <f>AC9/(G9/1000)</f>
         <v>2.3797644786300487</v>
       </c>
       <c r="AE9" s="35">
-        <f>(P9+Q9+R9)/100</f>
+        <f t="shared" si="9"/>
         <v>1.1952</v>
       </c>
       <c r="AF9" s="37">
@@ -6162,7 +6162,7 @@
         <v>2874754</v>
       </c>
       <c r="H10" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.95793202265911359</v>
       </c>
       <c r="I10" s="7">
@@ -6176,11 +6176,11 @@
         <v>2020.7539999999999</v>
       </c>
       <c r="L10" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>1627.7539999999999</v>
       </c>
       <c r="M10" s="50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0.80551813827907803</v>
       </c>
       <c r="N10" s="18">
@@ -6208,43 +6208,43 @@
         <v>124.38</v>
       </c>
       <c r="V10" s="14">
-        <f>P10*I10/100</f>
+        <f t="shared" si="1"/>
         <v>131.2227</v>
       </c>
       <c r="W10" s="14">
+        <f t="shared" si="11"/>
+        <v>488.81339999999994</v>
+      </c>
+      <c r="X10" s="14">
+        <f t="shared" si="2"/>
+        <v>4162.5313052000001</v>
+      </c>
+      <c r="Y10" s="14">
+        <f t="shared" si="3"/>
+        <v>-1005.2188000000002</v>
+      </c>
+      <c r="Z10" s="14">
+        <f t="shared" si="4"/>
+        <v>1776.3515000000002</v>
+      </c>
+      <c r="AA10" s="14">
         <f t="shared" si="5"/>
-        <v>488.81339999999994</v>
-      </c>
-      <c r="X10" s="14">
-        <f t="shared" si="1"/>
-        <v>4162.5313052000001</v>
-      </c>
-      <c r="Y10" s="14">
-        <f>(O10+((Q10+R10)*I10/100)+V10)-Z10</f>
-        <v>-1005.2188000000002</v>
-      </c>
-      <c r="Z10" s="14">
-        <f>J10*(S10+T10)/100</f>
-        <v>1776.3515000000002</v>
-      </c>
-      <c r="AA10" s="14">
-        <f t="shared" si="2"/>
         <v>5167.7501052000007</v>
       </c>
       <c r="AB10" s="15">
-        <f>J10*0.6</f>
+        <f t="shared" si="6"/>
         <v>748.19999999999993</v>
       </c>
       <c r="AC10" s="14">
+        <f t="shared" si="14"/>
+        <v>5915.9501052000005</v>
+      </c>
+      <c r="AD10" s="35">
         <f t="shared" si="8"/>
-        <v>5915.9501052000005</v>
-      </c>
-      <c r="AD10" s="35">
-        <f>AC10/(G10/1000)</f>
         <v>2.0578978601995166</v>
       </c>
       <c r="AE10" s="35">
-        <f>(P10+Q10+R10)/100</f>
+        <f t="shared" si="9"/>
         <v>0.95389999999999997</v>
       </c>
       <c r="AF10" s="37">
@@ -6258,36 +6258,110 @@
       <c r="B11" s="21">
         <v>2483</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="35"/>
-      <c r="AE11" s="35"/>
-      <c r="AF11" s="37"/>
+      <c r="C11" s="3">
+        <v>1753395</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1435472</v>
+      </c>
+      <c r="E11" s="3">
+        <v>708530</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1044865</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2480337</v>
+      </c>
+      <c r="H11" s="22">
+        <f t="shared" si="10"/>
+        <v>0.99892750704792588</v>
+      </c>
+      <c r="I11" s="7">
+        <v>703</v>
+      </c>
+      <c r="J11" s="7">
+        <v>1429</v>
+      </c>
+      <c r="K11" s="20">
+        <f t="shared" ref="K11" si="15">(G11/1000)+I11-J11</f>
+        <v>1754.337</v>
+      </c>
+      <c r="L11" s="20">
+        <f t="shared" ref="L11" si="16">K11-I11</f>
+        <v>1051.337</v>
+      </c>
+      <c r="M11" s="50">
+        <f t="shared" ref="M11" si="17">L11/K11</f>
+        <v>0.59927881587175102</v>
+      </c>
+      <c r="N11" s="18">
+        <v>0</v>
+      </c>
+      <c r="O11" s="18">
+        <v>452.5</v>
+      </c>
+      <c r="P11" s="19">
+        <v>43.37</v>
+      </c>
+      <c r="Q11" s="19">
+        <v>17</v>
+      </c>
+      <c r="R11" s="19">
+        <v>45</v>
+      </c>
+      <c r="S11" s="19">
+        <v>397.76</v>
+      </c>
+      <c r="T11" s="19">
+        <v>6.9</v>
+      </c>
+      <c r="U11" s="19">
+        <v>308.86</v>
+      </c>
+      <c r="V11" s="14">
+        <f t="shared" si="1"/>
+        <v>304.89109999999999</v>
+      </c>
+      <c r="W11" s="14">
+        <f t="shared" si="11"/>
+        <v>2171.2858000000001</v>
+      </c>
+      <c r="X11" s="14">
+        <f t="shared" si="2"/>
+        <v>6958.6341982000004</v>
+      </c>
+      <c r="Y11" s="14">
+        <f t="shared" si="3"/>
+        <v>-4589.3402999999998</v>
+      </c>
+      <c r="Z11" s="14">
+        <f t="shared" si="4"/>
+        <v>5782.5913999999993</v>
+      </c>
+      <c r="AA11" s="14">
+        <f t="shared" si="5"/>
+        <v>11547.974498200001</v>
+      </c>
+      <c r="AB11" s="15">
+        <f t="shared" si="6"/>
+        <v>857.4</v>
+      </c>
+      <c r="AC11" s="14">
+        <f t="shared" si="14"/>
+        <v>12405.374498200001</v>
+      </c>
+      <c r="AD11" s="35">
+        <f t="shared" si="8"/>
+        <v>5.0014874987552096</v>
+      </c>
+      <c r="AE11" s="35">
+        <f t="shared" si="9"/>
+        <v>1.0537000000000001</v>
+      </c>
+      <c r="AF11" s="37">
+        <v>300</v>
+      </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -6574,60 +6648,60 @@
       </c>
       <c r="C18" s="42">
         <f>SUM(C4:C17)/1000</f>
-        <v>15202.548000000001</v>
+        <v>16955.942999999999</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D4:D17)/1000</f>
-        <v>4871.45</v>
+        <v>6306.9219999999996</v>
       </c>
       <c r="E18" s="42">
         <f>SUM(E4:E17)/1000</f>
-        <v>6293.6120000000001</v>
+        <v>7002.1419999999998</v>
       </c>
       <c r="F18" s="42">
         <f>SUM(F4:F17)/1000</f>
-        <v>8911.6229999999996</v>
+        <v>9956.4879999999994</v>
       </c>
       <c r="G18" s="42">
         <f>SUM(G4:G17)/1000</f>
-        <v>13780.386</v>
+        <v>16260.723</v>
       </c>
       <c r="H18" s="42"/>
       <c r="I18" s="43">
-        <f t="shared" ref="I18:O18" si="9">SUM(I4:I15)</f>
-        <v>6265</v>
+        <f t="shared" ref="I18:O18" si="18">SUM(I4:I15)</f>
+        <v>6968</v>
       </c>
       <c r="J18" s="43">
-        <f t="shared" si="9"/>
-        <v>4832.3999999999996</v>
+        <f t="shared" si="18"/>
+        <v>6261.4</v>
       </c>
       <c r="K18" s="43">
-        <f t="shared" si="9"/>
-        <v>15212.986000000001</v>
+        <f t="shared" si="18"/>
+        <v>16967.323</v>
       </c>
       <c r="L18" s="43">
-        <f t="shared" si="9"/>
-        <v>8947.985999999999</v>
+        <f t="shared" si="18"/>
+        <v>9999.3229999999985</v>
       </c>
       <c r="M18" s="51">
-        <f t="shared" ref="M18" si="10">L18/K18</f>
-        <v>0.58818078186622924</v>
+        <f t="shared" ref="M18" si="19">L18/K18</f>
+        <v>0.58932826350980638</v>
       </c>
       <c r="N18" s="43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="O18" s="44">
-        <f t="shared" si="9"/>
-        <v>-726.25</v>
+        <f t="shared" si="18"/>
+        <v>-273.75</v>
       </c>
       <c r="P18" s="44">
         <f>AVERAGE(P4:P14)</f>
-        <v>66.40285714285713</v>
+        <v>63.523749999999993</v>
       </c>
       <c r="Q18" s="44">
         <f>AVERAGE(Q4:Q15)</f>
-        <v>15.799999999999999</v>
+        <v>15.95</v>
       </c>
       <c r="R18" s="44">
         <f>AVERAGE(R4:R15)</f>
@@ -6635,53 +6709,53 @@
       </c>
       <c r="S18" s="44">
         <f>AVERAGE(S4:S14)</f>
-        <v>145.46571428571428</v>
+        <v>177.0025</v>
       </c>
       <c r="T18" s="44">
         <f>AVERAGE(T4:T15)</f>
-        <v>4.6257142857142854</v>
+        <v>4.9099999999999993</v>
       </c>
       <c r="U18" s="44"/>
       <c r="V18" s="44">
-        <f t="shared" ref="V18:AC18" si="11">SUM(V4:V15)</f>
-        <v>4574.0313000000006</v>
+        <f t="shared" ref="V18:AC18" si="20">SUM(V4:V15)</f>
+        <v>4878.9224000000004</v>
       </c>
       <c r="W18" s="44">
-        <f t="shared" si="11"/>
-        <v>8681.5639999999985</v>
+        <f t="shared" si="20"/>
+        <v>10852.849799999998</v>
       </c>
       <c r="X18" s="44">
-        <f t="shared" si="11"/>
-        <v>30141.210520299996</v>
+        <f t="shared" si="20"/>
+        <v>37099.844718499997</v>
       </c>
       <c r="Y18" s="44">
-        <f t="shared" si="11"/>
-        <v>384.96099999999967</v>
+        <f t="shared" si="20"/>
+        <v>-4204.3793000000005</v>
       </c>
       <c r="Z18" s="44">
-        <f t="shared" si="11"/>
-        <v>7233.4892999999993</v>
+        <f t="shared" si="20"/>
+        <v>13016.080699999999</v>
       </c>
       <c r="AA18" s="44">
-        <f t="shared" si="11"/>
-        <v>29756.2495203</v>
+        <f t="shared" si="20"/>
+        <v>41304.224018499997</v>
       </c>
       <c r="AB18" s="44">
-        <f t="shared" si="11"/>
-        <v>2899.4399999999996</v>
+        <f t="shared" si="20"/>
+        <v>3756.8399999999997</v>
       </c>
       <c r="AC18" s="44">
-        <f t="shared" si="11"/>
-        <v>32655.689520300002</v>
+        <f t="shared" si="20"/>
+        <v>45061.064018500001</v>
       </c>
       <c r="AD18" s="45"/>
       <c r="AE18" s="45">
         <f>AVERAGE(AE4:AE15)</f>
-        <v>1.2720285714285713</v>
+        <v>1.2447374999999998</v>
       </c>
       <c r="AF18" s="44">
         <f>SUM(AF4:AF15)</f>
-        <v>2100</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
@@ -6721,7 +6795,7 @@
       <c r="X20" s="57"/>
       <c r="Y20" s="56">
         <f>Y18-AB18</f>
-        <v>-2514.4789999999998</v>
+        <v>-7961.2193000000007</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6748,10 +6822,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="60" t="s">
+      <c r="O21" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="P21" s="60"/>
+      <c r="P21" s="64"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -6764,23 +6838,23 @@
     <row r="22" spans="1:32" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="47">
         <f>G18</f>
-        <v>13780.386</v>
+        <v>16260.723</v>
       </c>
       <c r="D22" s="47">
         <f>J18</f>
-        <v>4832.3999999999996</v>
+        <v>6261.4</v>
       </c>
       <c r="E22" s="47">
         <f>I18</f>
-        <v>6265</v>
+        <v>6968</v>
       </c>
       <c r="F22" s="47">
         <f>K18</f>
-        <v>15212.986000000001</v>
+        <v>16967.323</v>
       </c>
       <c r="G22" s="47">
         <f>L18</f>
-        <v>8947.985999999999</v>
+        <v>9999.3229999999985</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -6793,11 +6867,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="61">
+      <c r="O22" s="65">
         <f>G24/(G18)</f>
-        <v>2.3697224098294489</v>
-      </c>
-      <c r="P22" s="61"/>
+        <v>2.7711599304963257</v>
+      </c>
+      <c r="P22" s="65"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -6830,7 +6904,7 @@
       <c r="F24" s="27"/>
       <c r="G24" s="49">
         <f>AC18+K22</f>
-        <v>32655.689520300002</v>
+        <v>45061.064018500001</v>
       </c>
     </row>
     <row r="25" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6856,7 +6930,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="48">
         <f>G24-AF18</f>
-        <v>30555.689520300002</v>
+        <v>42661.064018500001</v>
       </c>
     </row>
     <row r="28" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6868,16 +6942,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="X1:AE1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="X2:AE2"/>
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="O22:P22"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="N1:T1"/>
-    <mergeCell ref="X1:AE1"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="N2:T2"/>
-    <mergeCell ref="X2:AE2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to December 2022
</commit_message>
<xml_diff>
--- a/PV_investment_electricity_cost.xlsx
+++ b/PV_investment_electricity_cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeveloperArea\ElectricityCalculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A11D441-1234-4FBA-BA77-656FEB3549F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1F1736-B4F9-4EAB-B30D-7A3CEBCFED20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity 2020" sheetId="2" r:id="rId1"/>
@@ -449,7 +449,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="73">
   <si>
     <t>kWh</t>
   </si>
@@ -664,6 +664,12 @@
   </si>
   <si>
     <t>(enter this value into SolarEdge Dashboard per 2022-01-01)</t>
+  </si>
+  <si>
+    <t>Total value of solar cell production 2022</t>
+  </si>
+  <si>
+    <t>Total value of solar cells after intrest 2022</t>
   </si>
 </sst>
 </file>
@@ -991,7 +997,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1102,16 +1108,19 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1428,7 +1437,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1485,83 +1494,83 @@
         <v>2020</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62" t="s">
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="62"/>
+      <c r="J1" s="65"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="62" t="s">
+      <c r="N1" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
       <c r="U1" s="58" t="s">
         <v>68</v>
       </c>
       <c r="V1" s="58"/>
       <c r="W1" s="58"/>
-      <c r="X1" s="62" t="s">
+      <c r="X1" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="N2" s="63" t="s">
+      <c r="J2" s="64"/>
+      <c r="N2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="64"/>
       <c r="U2" s="60" t="s">
         <v>67</v>
       </c>
       <c r="V2" s="59"/>
       <c r="W2" s="59"/>
-      <c r="X2" s="63" t="s">
+      <c r="X2" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="63"/>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64"/>
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
     </row>
     <row r="3" spans="1:33" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -3115,10 +3124,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="64" t="s">
+      <c r="O21" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="P21" s="64"/>
+      <c r="P21" s="62"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -3158,11 +3167,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="65">
+      <c r="O22" s="63">
         <f>G24/(G18)</f>
         <v>1.0192692767647242</v>
       </c>
-      <c r="P22" s="65"/>
+      <c r="P22" s="63"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -3231,16 +3240,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="N2:T2"/>
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="O22:P22"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="X1:AE1"/>
     <mergeCell ref="X2:AE2"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="N1:T1"/>
-    <mergeCell ref="N2:T2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3253,7 +3262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D10279-7320-4E8B-8CBE-9D26D6E82614}">
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
@@ -3288,83 +3297,83 @@
         <v>2021</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62" t="s">
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="62"/>
+      <c r="J1" s="65"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="62" t="s">
+      <c r="N1" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
       <c r="U1" s="58" t="s">
         <v>68</v>
       </c>
       <c r="V1" s="54"/>
       <c r="W1" s="58"/>
-      <c r="X1" s="62" t="s">
+      <c r="X1" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="N2" s="63" t="s">
+      <c r="J2" s="64"/>
+      <c r="N2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="64"/>
       <c r="U2" s="60" t="s">
         <v>67</v>
       </c>
       <c r="V2" s="55"/>
       <c r="W2" s="59"/>
-      <c r="X2" s="63" t="s">
+      <c r="X2" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="63"/>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64"/>
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
     </row>
     <row r="3" spans="1:34" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -5113,10 +5122,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="64" t="s">
+      <c r="O21" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="P21" s="64"/>
+      <c r="P21" s="62"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -5158,11 +5167,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="65">
+      <c r="O22" s="63">
         <f>G24/(G18)</f>
         <v>1.5550322529312981</v>
       </c>
-      <c r="P22" s="65"/>
+      <c r="P22" s="63"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -5233,16 +5242,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="X1:AE1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="X2:AE2"/>
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="O22:P22"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="N1:T1"/>
-    <mergeCell ref="X1:AE1"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="N2:T2"/>
-    <mergeCell ref="X2:AE2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5254,8 +5263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973158C2-652A-42A8-8176-9FD76258C4A0}">
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5289,83 +5298,83 @@
         <v>2022</v>
       </c>
       <c r="B1" s="10"/>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62" t="s">
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="62"/>
+      <c r="J1" s="65"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="62" t="s">
+      <c r="N1" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
       <c r="U1" s="58" t="s">
         <v>68</v>
       </c>
       <c r="V1" s="58"/>
       <c r="W1" s="58"/>
-      <c r="X1" s="62" t="s">
+      <c r="X1" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="N2" s="63" t="s">
+      <c r="J2" s="64"/>
+      <c r="N2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="64"/>
       <c r="U2" s="60" t="s">
         <v>67</v>
       </c>
       <c r="V2" s="59"/>
       <c r="W2" s="59"/>
-      <c r="X2" s="63" t="s">
+      <c r="X2" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="63"/>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64"/>
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
     </row>
     <row r="3" spans="1:34" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -5534,7 +5543,7 @@
         <v>147.54</v>
       </c>
       <c r="V4" s="14">
-        <f t="shared" ref="V4:V11" si="1">P4*I4/100</f>
+        <f t="shared" ref="V4:V12" si="1">P4*I4/100</f>
         <v>1896.8992000000001</v>
       </c>
       <c r="W4" s="14">
@@ -5546,11 +5555,11 @@
         <v>2968.5387599999995</v>
       </c>
       <c r="Y4" s="14">
-        <f t="shared" ref="Y4:Y11" si="3">(O4+((Q4+R4)*I4/100)+V4)-Z4</f>
+        <f t="shared" ref="Y4:Y12" si="3">(O4+((Q4+R4)*I4/100)+V4)-Z4</f>
         <v>1554.05448</v>
       </c>
       <c r="Z4" s="14">
-        <f t="shared" ref="Z4:Z11" si="4">J4*(S4+T4)/100</f>
+        <f t="shared" ref="Z4:Z12" si="4">J4*(S4+T4)/100</f>
         <v>13.766719999999999</v>
       </c>
       <c r="AA4" s="14">
@@ -5558,7 +5567,7 @@
         <v>1414.4842799999994</v>
       </c>
       <c r="AB4" s="15">
-        <f t="shared" ref="AB4:AB11" si="6">J4*0.6</f>
+        <f t="shared" ref="AB4:AB15" si="6">J4*0.6</f>
         <v>5.28</v>
       </c>
       <c r="AC4" s="14">
@@ -5570,7 +5579,7 @@
         <v>16.712940317834011</v>
       </c>
       <c r="AE4" s="35">
-        <f t="shared" ref="AE4:AE11" si="9">(P4+Q4+R4)/100</f>
+        <f t="shared" ref="AE4:AE12" si="9">(P4+Q4+R4)/100</f>
         <v>1.4904000000000002</v>
       </c>
       <c r="AF4" s="37">
@@ -5600,7 +5609,7 @@
         <v>473722</v>
       </c>
       <c r="H5" s="22">
-        <f t="shared" ref="H5:H11" si="10">(G5/1000)/B5</f>
+        <f t="shared" ref="H5:H18" si="10">(G5/1000)/B5</f>
         <v>0.82529965156794427</v>
       </c>
       <c r="I5" s="7">
@@ -6284,15 +6293,15 @@
         <v>1429</v>
       </c>
       <c r="K11" s="20">
-        <f t="shared" ref="K11" si="15">(G11/1000)+I11-J11</f>
+        <f t="shared" ref="K11:K15" si="15">(G11/1000)+I11-J11</f>
         <v>1754.337</v>
       </c>
       <c r="L11" s="20">
-        <f t="shared" ref="L11" si="16">K11-I11</f>
+        <f t="shared" ref="L11:L15" si="16">K11-I11</f>
         <v>1051.337</v>
       </c>
       <c r="M11" s="50">
-        <f t="shared" ref="M11" si="17">L11/K11</f>
+        <f t="shared" ref="M11:M15" si="17">L11/K11</f>
         <v>0.59927881587175102</v>
       </c>
       <c r="N11" s="18">
@@ -6370,36 +6379,110 @@
       <c r="B12" s="52">
         <v>1649</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="14"/>
-      <c r="AD12" s="35"/>
-      <c r="AE12" s="35"/>
-      <c r="AF12" s="37"/>
+      <c r="C12" s="3">
+        <v>1219556</v>
+      </c>
+      <c r="D12" s="3">
+        <v>765749</v>
+      </c>
+      <c r="E12" s="3">
+        <v>602849</v>
+      </c>
+      <c r="F12" s="3">
+        <v>616707</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1382456</v>
+      </c>
+      <c r="H12" s="22">
+        <f t="shared" si="10"/>
+        <v>0.83836021831412977</v>
+      </c>
+      <c r="I12" s="7">
+        <v>598</v>
+      </c>
+      <c r="J12" s="7">
+        <v>763</v>
+      </c>
+      <c r="K12" s="20">
+        <f t="shared" si="15"/>
+        <v>1217.4559999999999</v>
+      </c>
+      <c r="L12" s="20">
+        <f t="shared" si="16"/>
+        <v>619.4559999999999</v>
+      </c>
+      <c r="M12" s="50">
+        <f t="shared" si="17"/>
+        <v>0.50881181742913084</v>
+      </c>
+      <c r="N12" s="18">
+        <v>0</v>
+      </c>
+      <c r="O12" s="18">
+        <v>452.5</v>
+      </c>
+      <c r="P12" s="19">
+        <v>82.29</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>17</v>
+      </c>
+      <c r="R12" s="19">
+        <v>45</v>
+      </c>
+      <c r="S12" s="19">
+        <v>346.05</v>
+      </c>
+      <c r="T12" s="19">
+        <v>6.9</v>
+      </c>
+      <c r="U12" s="19">
+        <v>306.43</v>
+      </c>
+      <c r="V12" s="14">
+        <f t="shared" ref="V12:V15" si="18">P12*I12/100</f>
+        <v>492.09420000000006</v>
+      </c>
+      <c r="W12" s="14">
+        <f t="shared" ref="W12:W15" si="19">U12*I12/100</f>
+        <v>1832.4514000000001</v>
+      </c>
+      <c r="X12" s="14">
+        <f t="shared" ref="X12:X15" si="20">(K12*(U12+Q12+R12)/100)+N12+O12</f>
+        <v>4937.9731407999998</v>
+      </c>
+      <c r="Y12" s="14">
+        <f t="shared" ref="Y12:Y15" si="21">(O12+((Q12+R12)*I12/100)+V12)-Z12</f>
+        <v>-1377.6542999999999</v>
+      </c>
+      <c r="Z12" s="14">
+        <f t="shared" ref="Z12:Z15" si="22">J12*(S12+T12)/100</f>
+        <v>2693.0084999999999</v>
+      </c>
+      <c r="AA12" s="14">
+        <f t="shared" ref="AA12:AA15" si="23">X12-Y12</f>
+        <v>6315.6274407999999</v>
+      </c>
+      <c r="AB12" s="15">
+        <f t="shared" ref="AB12:AB15" si="24">J12*0.6</f>
+        <v>457.8</v>
+      </c>
+      <c r="AC12" s="14">
+        <f t="shared" ref="AC12:AC15" si="25">AA12+AB12</f>
+        <v>6773.4274408000001</v>
+      </c>
+      <c r="AD12" s="35">
+        <f t="shared" ref="AD12:AD15" si="26">AC12/(G12/1000)</f>
+        <v>4.8995609558640565</v>
+      </c>
+      <c r="AE12" s="35">
+        <f t="shared" ref="AE12:AE15" si="27">(P12+Q12+R12)/100</f>
+        <v>1.4429000000000003</v>
+      </c>
+      <c r="AF12" s="37">
+        <v>300</v>
+      </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -6408,36 +6491,110 @@
       <c r="B13" s="52">
         <v>785</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="15"/>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="35"/>
-      <c r="AE13" s="35"/>
-      <c r="AF13" s="37"/>
+      <c r="C13" s="3">
+        <v>1304831</v>
+      </c>
+      <c r="D13" s="3">
+        <v>273151</v>
+      </c>
+      <c r="E13" s="3">
+        <v>789423</v>
+      </c>
+      <c r="F13" s="3">
+        <v>515408</v>
+      </c>
+      <c r="G13" s="3">
+        <v>788559</v>
+      </c>
+      <c r="H13" s="22">
+        <f t="shared" si="10"/>
+        <v>1.0045337579617835</v>
+      </c>
+      <c r="I13" s="7">
+        <v>784</v>
+      </c>
+      <c r="J13" s="7">
+        <v>270</v>
+      </c>
+      <c r="K13" s="20">
+        <f t="shared" si="15"/>
+        <v>1302.559</v>
+      </c>
+      <c r="L13" s="20">
+        <f t="shared" si="16"/>
+        <v>518.55899999999997</v>
+      </c>
+      <c r="M13" s="50">
+        <f t="shared" si="17"/>
+        <v>0.39810787841472056</v>
+      </c>
+      <c r="N13" s="18">
+        <v>0</v>
+      </c>
+      <c r="O13" s="18">
+        <v>452.5</v>
+      </c>
+      <c r="P13" s="19">
+        <v>45.35</v>
+      </c>
+      <c r="Q13" s="19">
+        <v>17</v>
+      </c>
+      <c r="R13" s="19">
+        <v>45</v>
+      </c>
+      <c r="S13" s="19">
+        <v>146.47</v>
+      </c>
+      <c r="T13" s="19">
+        <v>6.9</v>
+      </c>
+      <c r="U13" s="19">
+        <v>114.91</v>
+      </c>
+      <c r="V13" s="14">
+        <f t="shared" si="18"/>
+        <v>355.54400000000004</v>
+      </c>
+      <c r="W13" s="14">
+        <f t="shared" si="19"/>
+        <v>900.89440000000002</v>
+      </c>
+      <c r="X13" s="14">
+        <f t="shared" si="20"/>
+        <v>2756.8571268999999</v>
+      </c>
+      <c r="Y13" s="14">
+        <f t="shared" si="21"/>
+        <v>880.02500000000009</v>
+      </c>
+      <c r="Z13" s="14">
+        <f t="shared" si="22"/>
+        <v>414.09899999999999</v>
+      </c>
+      <c r="AA13" s="14">
+        <f t="shared" si="23"/>
+        <v>1876.8321268999998</v>
+      </c>
+      <c r="AB13" s="15">
+        <f t="shared" si="24"/>
+        <v>162</v>
+      </c>
+      <c r="AC13" s="14">
+        <f t="shared" si="25"/>
+        <v>2038.8321268999998</v>
+      </c>
+      <c r="AD13" s="35">
+        <f t="shared" si="26"/>
+        <v>2.5855162732274946</v>
+      </c>
+      <c r="AE13" s="35">
+        <f t="shared" si="27"/>
+        <v>1.0734999999999999</v>
+      </c>
+      <c r="AF13" s="37">
+        <v>300</v>
+      </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -6446,36 +6603,110 @@
       <c r="B14" s="52">
         <v>252</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="14"/>
-      <c r="AD14" s="35"/>
-      <c r="AE14" s="35"/>
-      <c r="AF14" s="37"/>
+      <c r="C14" s="3">
+        <v>1410228</v>
+      </c>
+      <c r="D14" s="3">
+        <v>29350</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1281077</v>
+      </c>
+      <c r="F14" s="3">
+        <v>131674</v>
+      </c>
+      <c r="G14" s="3">
+        <v>158501</v>
+      </c>
+      <c r="H14" s="22">
+        <f t="shared" si="10"/>
+        <v>0.62897222222222227</v>
+      </c>
+      <c r="I14" s="7">
+        <v>1276</v>
+      </c>
+      <c r="J14" s="7">
+        <v>26</v>
+      </c>
+      <c r="K14" s="20">
+        <f t="shared" si="15"/>
+        <v>1408.501</v>
+      </c>
+      <c r="L14" s="20">
+        <f t="shared" si="16"/>
+        <v>132.50099999999998</v>
+      </c>
+      <c r="M14" s="50">
+        <f t="shared" si="17"/>
+        <v>9.407235067635733E-2</v>
+      </c>
+      <c r="N14" s="18">
+        <v>0</v>
+      </c>
+      <c r="O14" s="18">
+        <v>452.5</v>
+      </c>
+      <c r="P14" s="19">
+        <v>124.53</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>17</v>
+      </c>
+      <c r="R14" s="19">
+        <v>45</v>
+      </c>
+      <c r="S14" s="19">
+        <v>102.21</v>
+      </c>
+      <c r="T14" s="19">
+        <v>6.9</v>
+      </c>
+      <c r="U14" s="19">
+        <v>197.51</v>
+      </c>
+      <c r="V14" s="14">
+        <f t="shared" si="18"/>
+        <v>1589.0028</v>
+      </c>
+      <c r="W14" s="14">
+        <f t="shared" si="19"/>
+        <v>2520.2275999999997</v>
+      </c>
+      <c r="X14" s="14">
+        <f t="shared" si="20"/>
+        <v>4107.7009450999994</v>
+      </c>
+      <c r="Y14" s="14">
+        <f t="shared" si="21"/>
+        <v>2804.2542000000003</v>
+      </c>
+      <c r="Z14" s="14">
+        <f t="shared" si="22"/>
+        <v>28.368600000000001</v>
+      </c>
+      <c r="AA14" s="14">
+        <f t="shared" si="23"/>
+        <v>1303.4467450999991</v>
+      </c>
+      <c r="AB14" s="15">
+        <f t="shared" si="24"/>
+        <v>15.6</v>
+      </c>
+      <c r="AC14" s="14">
+        <f t="shared" si="25"/>
+        <v>1319.046745099999</v>
+      </c>
+      <c r="AD14" s="35">
+        <f t="shared" si="26"/>
+        <v>8.3220089784922422</v>
+      </c>
+      <c r="AE14" s="35">
+        <f t="shared" si="27"/>
+        <v>1.8653</v>
+      </c>
+      <c r="AF14" s="37">
+        <v>300</v>
+      </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -6484,36 +6715,110 @@
       <c r="B15" s="52">
         <v>129</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="15"/>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="35"/>
-      <c r="AE15" s="35"/>
-      <c r="AF15" s="37"/>
+      <c r="C15" s="3">
+        <v>1687518</v>
+      </c>
+      <c r="D15" s="3">
+        <v>13500</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1668805</v>
+      </c>
+      <c r="F15" s="3">
+        <v>23707</v>
+      </c>
+      <c r="G15" s="3">
+        <v>32213</v>
+      </c>
+      <c r="H15" s="22">
+        <f t="shared" si="10"/>
+        <v>0.24971317829457365</v>
+      </c>
+      <c r="I15" s="7">
+        <v>1666</v>
+      </c>
+      <c r="J15" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="K15" s="20">
+        <f t="shared" si="15"/>
+        <v>1692.8129999999999</v>
+      </c>
+      <c r="L15" s="20">
+        <f t="shared" si="16"/>
+        <v>26.812999999999874</v>
+      </c>
+      <c r="M15" s="50">
+        <f t="shared" si="17"/>
+        <v>1.5839315978787898E-2</v>
+      </c>
+      <c r="N15" s="18">
+        <v>0</v>
+      </c>
+      <c r="O15" s="18">
+        <v>452.5</v>
+      </c>
+      <c r="P15" s="19">
+        <v>258.41000000000003</v>
+      </c>
+      <c r="Q15" s="19">
+        <v>17</v>
+      </c>
+      <c r="R15" s="19">
+        <v>45</v>
+      </c>
+      <c r="S15" s="19">
+        <v>235.83</v>
+      </c>
+      <c r="T15" s="19">
+        <v>6.9</v>
+      </c>
+      <c r="U15" s="19">
+        <v>371.36</v>
+      </c>
+      <c r="V15" s="14">
+        <f t="shared" si="18"/>
+        <v>4305.1106000000009</v>
+      </c>
+      <c r="W15" s="14">
+        <f t="shared" si="19"/>
+        <v>6186.8576000000003</v>
+      </c>
+      <c r="X15" s="14">
+        <f t="shared" si="20"/>
+        <v>7788.4744167999997</v>
+      </c>
+      <c r="Y15" s="14">
+        <f t="shared" si="21"/>
+        <v>5777.4231800000007</v>
+      </c>
+      <c r="Z15" s="14">
+        <f t="shared" si="22"/>
+        <v>13.107420000000001</v>
+      </c>
+      <c r="AA15" s="14">
+        <f t="shared" si="23"/>
+        <v>2011.0512367999991</v>
+      </c>
+      <c r="AB15" s="15">
+        <f t="shared" si="24"/>
+        <v>3.24</v>
+      </c>
+      <c r="AC15" s="14">
+        <f t="shared" si="25"/>
+        <v>2014.2912367999991</v>
+      </c>
+      <c r="AD15" s="35">
+        <f t="shared" si="26"/>
+        <v>62.53038328625086</v>
+      </c>
+      <c r="AE15" s="35">
+        <f t="shared" si="27"/>
+        <v>3.2041000000000004</v>
+      </c>
+      <c r="AF15" s="37">
+        <v>300</v>
+      </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -6648,60 +6953,63 @@
       </c>
       <c r="C18" s="42">
         <f>SUM(C4:C17)/1000</f>
-        <v>16955.942999999999</v>
+        <v>22578.076000000001</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D4:D17)/1000</f>
-        <v>6306.9219999999996</v>
+        <v>7388.6719999999996</v>
       </c>
       <c r="E18" s="42">
         <f>SUM(E4:E17)/1000</f>
-        <v>7002.1419999999998</v>
+        <v>11344.296</v>
       </c>
       <c r="F18" s="42">
         <f>SUM(F4:F17)/1000</f>
-        <v>9956.4879999999994</v>
+        <v>11243.984</v>
       </c>
       <c r="G18" s="42">
         <f>SUM(G4:G17)/1000</f>
-        <v>16260.723</v>
-      </c>
-      <c r="H18" s="42"/>
+        <v>18622.452000000001</v>
+      </c>
+      <c r="H18" s="66">
+        <f>G18/B18</f>
+        <v>0.97755653543307097</v>
+      </c>
       <c r="I18" s="43">
-        <f t="shared" ref="I18:O18" si="18">SUM(I4:I15)</f>
-        <v>6968</v>
+        <f t="shared" ref="I18:O18" si="28">SUM(I4:I15)</f>
+        <v>11292</v>
       </c>
       <c r="J18" s="43">
-        <f t="shared" si="18"/>
-        <v>6261.4</v>
+        <f t="shared" si="28"/>
+        <v>7325.7999999999993</v>
       </c>
       <c r="K18" s="43">
-        <f t="shared" si="18"/>
-        <v>16967.323</v>
+        <f t="shared" si="28"/>
+        <v>22588.651999999998</v>
       </c>
       <c r="L18" s="43">
-        <f t="shared" si="18"/>
-        <v>9999.3229999999985</v>
+        <f t="shared" si="28"/>
+        <v>11296.651999999998</v>
       </c>
       <c r="M18" s="51">
-        <f t="shared" ref="M18" si="19">L18/K18</f>
-        <v>0.58932826350980638</v>
+        <f t="shared" ref="M18" si="29">L18/K18</f>
+        <v>0.50010297205871335</v>
       </c>
       <c r="N18" s="43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O18" s="44">
-        <f t="shared" si="18"/>
-        <v>-273.75</v>
+        <f t="shared" si="28"/>
+        <v>1536.25</v>
       </c>
       <c r="P18" s="44">
         <f>AVERAGE(P4:P14)</f>
-        <v>63.523749999999993</v>
+        <v>69.123636363636351</v>
       </c>
       <c r="Q18" s="44">
         <f>AVERAGE(Q4:Q15)</f>
-        <v>15.95</v>
+        <v>16.3</v>
       </c>
       <c r="R18" s="44">
         <f>AVERAGE(R4:R15)</f>
@@ -6709,53 +7017,53 @@
       </c>
       <c r="S18" s="44">
         <f>AVERAGE(S4:S14)</f>
-        <v>177.0025</v>
+        <v>182.79545454545453</v>
       </c>
       <c r="T18" s="44">
         <f>AVERAGE(T4:T15)</f>
-        <v>4.9099999999999993</v>
+        <v>5.5733333333333333</v>
       </c>
       <c r="U18" s="44"/>
       <c r="V18" s="44">
-        <f t="shared" ref="V18:AC18" si="20">SUM(V4:V15)</f>
-        <v>4878.9224000000004</v>
+        <f t="shared" ref="V18:AC18" si="30">SUM(V4:V15)</f>
+        <v>11620.674000000003</v>
       </c>
       <c r="W18" s="44">
-        <f t="shared" si="20"/>
-        <v>10852.849799999998</v>
+        <f t="shared" si="30"/>
+        <v>22293.280799999997</v>
       </c>
       <c r="X18" s="44">
-        <f t="shared" si="20"/>
-        <v>37099.844718499997</v>
+        <f t="shared" si="30"/>
+        <v>56690.850348099993</v>
       </c>
       <c r="Y18" s="44">
-        <f t="shared" si="20"/>
-        <v>-4204.3793000000005</v>
+        <f t="shared" si="30"/>
+        <v>3879.66878</v>
       </c>
       <c r="Z18" s="44">
-        <f t="shared" si="20"/>
-        <v>13016.080699999999</v>
+        <f t="shared" si="30"/>
+        <v>16164.664219999999</v>
       </c>
       <c r="AA18" s="44">
-        <f t="shared" si="20"/>
-        <v>41304.224018499997</v>
+        <f t="shared" si="30"/>
+        <v>52811.181568100001</v>
       </c>
       <c r="AB18" s="44">
-        <f t="shared" si="20"/>
-        <v>3756.8399999999997</v>
+        <f t="shared" si="30"/>
+        <v>4395.4799999999996</v>
       </c>
       <c r="AC18" s="44">
-        <f t="shared" si="20"/>
-        <v>45061.064018500001</v>
+        <f t="shared" si="30"/>
+        <v>57206.661568099997</v>
       </c>
       <c r="AD18" s="45"/>
       <c r="AE18" s="45">
         <f>AVERAGE(AE4:AE15)</f>
-        <v>1.2447374999999998</v>
+        <v>1.4619749999999998</v>
       </c>
       <c r="AF18" s="44">
         <f>SUM(AF4:AF15)</f>
-        <v>2400</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
@@ -6793,10 +7101,7 @@
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
       <c r="X20" s="57"/>
-      <c r="Y20" s="56">
-        <f>Y18-AB18</f>
-        <v>-7961.2193000000007</v>
-      </c>
+      <c r="Y20" s="56"/>
     </row>
     <row r="21" spans="1:32" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="46" t="s">
@@ -6822,10 +7127,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="64" t="s">
+      <c r="O21" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="P21" s="64"/>
+      <c r="P21" s="62"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -6838,23 +7143,23 @@
     <row r="22" spans="1:32" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="47">
         <f>G18</f>
-        <v>16260.723</v>
+        <v>18622.452000000001</v>
       </c>
       <c r="D22" s="47">
         <f>J18</f>
-        <v>6261.4</v>
+        <v>7325.7999999999993</v>
       </c>
       <c r="E22" s="47">
         <f>I18</f>
-        <v>6968</v>
+        <v>11292</v>
       </c>
       <c r="F22" s="47">
         <f>K18</f>
-        <v>16967.323</v>
+        <v>22588.651999999998</v>
       </c>
       <c r="G22" s="47">
         <f>L18</f>
-        <v>9999.3229999999985</v>
+        <v>11296.651999999998</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -6867,11 +7172,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="65">
+      <c r="O22" s="63">
         <f>G24/(G18)</f>
-        <v>2.7711599304963257</v>
-      </c>
-      <c r="P22" s="65"/>
+        <v>3.0719188626771596</v>
+      </c>
+      <c r="P22" s="63"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -6897,14 +7202,14 @@
     </row>
     <row r="24" spans="1:32" ht="21" x14ac:dyDescent="0.35">
       <c r="C24" s="26" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
       <c r="G24" s="49">
         <f>AC18+K22</f>
-        <v>45061.064018500001</v>
+        <v>57206.661568099997</v>
       </c>
     </row>
     <row r="25" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6923,14 +7228,14 @@
     </row>
     <row r="27" spans="1:32" ht="21" x14ac:dyDescent="0.35">
       <c r="C27" s="32" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="48">
         <f>G24-AF18</f>
-        <v>42661.064018500001</v>
+        <v>53606.661568099997</v>
       </c>
     </row>
     <row r="28" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6942,16 +7247,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="N1:T1"/>
     <mergeCell ref="X1:AE1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="N2:T2"/>
     <mergeCell ref="X2:AE2"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="N1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to February 2023
</commit_message>
<xml_diff>
--- a/PV_investment_electricity_cost.xlsx
+++ b/PV_investment_electricity_cost.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeveloperArea\ElectricityCalculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1F1736-B4F9-4EAB-B30D-7A3CEBCFED20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF73610-0079-4B9F-BE60-201E6F1FB11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{ECB3817B-AF73-4635-88B4-AD4DB6228D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity 2020" sheetId="2" r:id="rId1"/>
     <sheet name="Electricity 2021" sheetId="4" r:id="rId2"/>
     <sheet name="Electricity 2022" sheetId="5" r:id="rId3"/>
+    <sheet name="Electricity 2023" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -448,8 +449,140 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Magnus Pernemark</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{30152069-97F8-4FDD-9F59-4A54EDCE003A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Magnus Pernemark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Data is from SolarEdge Designer. If you do't have thiese values, do an estimate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{C06B4344-013F-4B70-B35D-407BE1182CCD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Magnus Pernemark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Calculated from production plus bought minus sold.
+If a meter is used, use that value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{F5632327-5BCC-4F55-8A85-7F860FAE6485}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Magnus Pernemark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Calculated value from produced vs bought and sold
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD3" authorId="0" shapeId="0" xr:uid="{0875F381-2D81-4C43-8CD5-6B8F3C32EC85}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Magnus Pernemark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Enter this value into SolarEdge Monitor platform at Flat Rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF3" authorId="0" shapeId="0" xr:uid="{B4001153-E45F-428B-8D24-2D215CE20752}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Magnus Pernemark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If solar cells are bought with borrowed money, enter intrest cost after tax deduction</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="74">
   <si>
     <t>kWh</t>
   </si>
@@ -670,6 +803,9 @@
   </si>
   <si>
     <t>Total value of solar cells after intrest 2022</t>
+  </si>
+  <si>
+    <t>(enter this value into SolarEdge Dashboard per 2023-01-01)</t>
   </si>
 </sst>
 </file>
@@ -997,7 +1133,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1108,12 +1244,6 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1121,6 +1251,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1535,42 +1677,42 @@
       <c r="AE1" s="65"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="64"/>
-      <c r="N2" s="64" t="s">
+      <c r="J2" s="66"/>
+      <c r="N2" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
       <c r="U2" s="60" t="s">
         <v>67</v>
       </c>
       <c r="V2" s="59"/>
       <c r="W2" s="59"/>
-      <c r="X2" s="64" t="s">
+      <c r="X2" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="64"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
     </row>
     <row r="3" spans="1:33" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -3124,10 +3266,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="62" t="s">
+      <c r="O21" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="P21" s="62"/>
+      <c r="P21" s="67"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -3167,11 +3309,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="63">
+      <c r="O22" s="68">
         <f>G24/(G18)</f>
         <v>1.0192692767647242</v>
       </c>
-      <c r="P22" s="63"/>
+      <c r="P22" s="68"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -3240,16 +3382,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="X1:AE1"/>
+    <mergeCell ref="X2:AE2"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="N1:T1"/>
     <mergeCell ref="N2:T2"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="X1:AE1"/>
-    <mergeCell ref="X2:AE2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3338,42 +3480,42 @@
       <c r="AE1" s="65"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="64"/>
-      <c r="N2" s="64" t="s">
+      <c r="J2" s="66"/>
+      <c r="N2" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
       <c r="U2" s="60" t="s">
         <v>67</v>
       </c>
       <c r="V2" s="55"/>
       <c r="W2" s="59"/>
-      <c r="X2" s="64" t="s">
+      <c r="X2" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="64"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
     </row>
     <row r="3" spans="1:34" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -5122,10 +5264,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="62" t="s">
+      <c r="O21" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="P21" s="62"/>
+      <c r="P21" s="67"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -5167,11 +5309,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="63">
+      <c r="O22" s="68">
         <f>G24/(G18)</f>
         <v>1.5550322529312981</v>
       </c>
-      <c r="P22" s="63"/>
+      <c r="P22" s="68"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -5242,16 +5384,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="N1:T1"/>
     <mergeCell ref="X1:AE1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="N2:T2"/>
     <mergeCell ref="X2:AE2"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="N1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5263,8 +5405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973158C2-652A-42A8-8176-9FD76258C4A0}">
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5339,42 +5481,42 @@
       <c r="AE1" s="65"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="64"/>
-      <c r="N2" s="64" t="s">
+      <c r="J2" s="66"/>
+      <c r="N2" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
       <c r="U2" s="60" t="s">
         <v>67</v>
       </c>
       <c r="V2" s="59"/>
       <c r="W2" s="59"/>
-      <c r="X2" s="64" t="s">
+      <c r="X2" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="64"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
     </row>
     <row r="3" spans="1:34" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -5543,7 +5685,7 @@
         <v>147.54</v>
       </c>
       <c r="V4" s="14">
-        <f t="shared" ref="V4:V12" si="1">P4*I4/100</f>
+        <f t="shared" ref="V4:V11" si="1">P4*I4/100</f>
         <v>1896.8992000000001</v>
       </c>
       <c r="W4" s="14">
@@ -5555,11 +5697,11 @@
         <v>2968.5387599999995</v>
       </c>
       <c r="Y4" s="14">
-        <f t="shared" ref="Y4:Y12" si="3">(O4+((Q4+R4)*I4/100)+V4)-Z4</f>
+        <f t="shared" ref="Y4:Y11" si="3">(O4+((Q4+R4)*I4/100)+V4)-Z4</f>
         <v>1554.05448</v>
       </c>
       <c r="Z4" s="14">
-        <f t="shared" ref="Z4:Z12" si="4">J4*(S4+T4)/100</f>
+        <f t="shared" ref="Z4:Z11" si="4">J4*(S4+T4)/100</f>
         <v>13.766719999999999</v>
       </c>
       <c r="AA4" s="14">
@@ -5567,7 +5709,7 @@
         <v>1414.4842799999994</v>
       </c>
       <c r="AB4" s="15">
-        <f t="shared" ref="AB4:AB15" si="6">J4*0.6</f>
+        <f t="shared" ref="AB4:AB11" si="6">J4*0.6</f>
         <v>5.28</v>
       </c>
       <c r="AC4" s="14">
@@ -5579,7 +5721,7 @@
         <v>16.712940317834011</v>
       </c>
       <c r="AE4" s="35">
-        <f t="shared" ref="AE4:AE12" si="9">(P4+Q4+R4)/100</f>
+        <f t="shared" ref="AE4:AE11" si="9">(P4+Q4+R4)/100</f>
         <v>1.4904000000000002</v>
       </c>
       <c r="AF4" s="37">
@@ -5609,7 +5751,7 @@
         <v>473722</v>
       </c>
       <c r="H5" s="22">
-        <f t="shared" ref="H5:H18" si="10">(G5/1000)/B5</f>
+        <f t="shared" ref="H5:H15" si="10">(G5/1000)/B5</f>
         <v>0.82529965156794427</v>
       </c>
       <c r="I5" s="7">
@@ -6971,7 +7113,7 @@
         <f>SUM(G4:G17)/1000</f>
         <v>18622.452000000001</v>
       </c>
-      <c r="H18" s="66">
+      <c r="H18" s="64">
         <f>G18/B18</f>
         <v>0.97755653543307097</v>
       </c>
@@ -7127,10 +7269,10 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="62" t="s">
+      <c r="O21" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="P21" s="62"/>
+      <c r="P21" s="67"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -7172,11 +7314,11 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="63">
+      <c r="O22" s="68">
         <f>G24/(G18)</f>
         <v>3.0719188626771596</v>
       </c>
-      <c r="P22" s="63"/>
+      <c r="P22" s="68"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -7236,6 +7378,1707 @@
       <c r="G27" s="48">
         <f>G24-AF18</f>
         <v>53606.661568099997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="28"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="X1:AE1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="X2:AE2"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="N1:T1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2C1448-792D-4427-8328-87BE4957108B}">
+  <dimension ref="A1:AH28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22:P22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" customWidth="1"/>
+    <col min="22" max="23" width="10.85546875" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" customWidth="1"/>
+    <col min="25" max="25" width="10.28515625" customWidth="1"/>
+    <col min="26" max="27" width="11" customWidth="1"/>
+    <col min="28" max="28" width="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="15.85546875" customWidth="1"/>
+    <col min="32" max="32" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="10">
+        <v>2023</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="65"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="V1" s="63"/>
+      <c r="W1" s="63"/>
+      <c r="X1" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="C2" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="66"/>
+      <c r="N2" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" s="62"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66"/>
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+    </row>
+    <row r="3" spans="1:34" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="W3" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF3" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="21">
+        <v>231</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1706110</v>
+      </c>
+      <c r="D4" s="3">
+        <v>18560</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1607833</v>
+      </c>
+      <c r="F4" s="3">
+        <v>102498</v>
+      </c>
+      <c r="G4" s="3">
+        <v>116837</v>
+      </c>
+      <c r="H4" s="22">
+        <f>(G4/1000)/B4</f>
+        <v>0.50578787878787879</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1603</v>
+      </c>
+      <c r="J4" s="7">
+        <v>9</v>
+      </c>
+      <c r="K4" s="20">
+        <f t="shared" ref="K4:K15" si="0">(G4/1000)+I4-J4</f>
+        <v>1710.837</v>
+      </c>
+      <c r="L4" s="20">
+        <f>K4-I4</f>
+        <v>107.83699999999999</v>
+      </c>
+      <c r="M4" s="50">
+        <f>L4/K4</f>
+        <v>6.3031720730846938E-2</v>
+      </c>
+      <c r="N4" s="18">
+        <v>0</v>
+      </c>
+      <c r="O4" s="18">
+        <v>492.5</v>
+      </c>
+      <c r="P4" s="19">
+        <v>72.44</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>18.55</v>
+      </c>
+      <c r="R4" s="19">
+        <v>49</v>
+      </c>
+      <c r="S4" s="19">
+        <v>116.43</v>
+      </c>
+      <c r="T4" s="19">
+        <v>13.72</v>
+      </c>
+      <c r="U4" s="19">
+        <v>129.88999999999999</v>
+      </c>
+      <c r="V4" s="14">
+        <f t="shared" ref="V4:V15" si="1">P4*I4/100</f>
+        <v>1161.2131999999999</v>
+      </c>
+      <c r="W4" s="14">
+        <f>U4*I4/100</f>
+        <v>2082.1367</v>
+      </c>
+      <c r="X4" s="14">
+        <f t="shared" ref="X4:X15" si="2">(K4*(U4+Q4+R4)/100)+N4+O4</f>
+        <v>3870.3765727999998</v>
+      </c>
+      <c r="Y4" s="14">
+        <f t="shared" ref="Y4:Y15" si="3">(O4+((Q4+R4)*I4/100)+V4)-Z4</f>
+        <v>2724.8262</v>
+      </c>
+      <c r="Z4" s="14">
+        <f t="shared" ref="Z4:Z15" si="4">J4*(S4+T4)/100</f>
+        <v>11.713500000000002</v>
+      </c>
+      <c r="AA4" s="14">
+        <f t="shared" ref="AA4:AA15" si="5">X4-Y4</f>
+        <v>1145.5503727999999</v>
+      </c>
+      <c r="AB4" s="15">
+        <f t="shared" ref="AB4:AB15" si="6">J4*0.6</f>
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="AC4" s="14">
+        <f t="shared" ref="AC4:AC6" si="7">AA4+AB4</f>
+        <v>1150.9503728</v>
+      </c>
+      <c r="AD4" s="35">
+        <f t="shared" ref="AD4:AD15" si="8">AC4/(G4/1000)</f>
+        <v>9.8509065860985814</v>
+      </c>
+      <c r="AE4" s="35">
+        <f t="shared" ref="AE4:AE15" si="9">(P4+Q4+R4)/100</f>
+        <v>1.3999000000000001</v>
+      </c>
+      <c r="AF4" s="37">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="21">
+        <v>574</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1797932</v>
+      </c>
+      <c r="D5" s="3">
+        <v>93479</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1560049</v>
+      </c>
+      <c r="F5" s="3">
+        <v>238312</v>
+      </c>
+      <c r="G5" s="3">
+        <v>331362</v>
+      </c>
+      <c r="H5" s="22">
+        <f t="shared" ref="H5:H15" si="10">(G5/1000)/B5</f>
+        <v>0.57728571428571429</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1555</v>
+      </c>
+      <c r="J5" s="7">
+        <v>85</v>
+      </c>
+      <c r="K5" s="20">
+        <f t="shared" si="0"/>
+        <v>1801.3620000000001</v>
+      </c>
+      <c r="L5" s="20">
+        <f>K5-I5</f>
+        <v>246.36200000000008</v>
+      </c>
+      <c r="M5" s="50">
+        <f>L5/K5</f>
+        <v>0.13676429279622868</v>
+      </c>
+      <c r="N5" s="18">
+        <v>0</v>
+      </c>
+      <c r="O5" s="18">
+        <v>492.5</v>
+      </c>
+      <c r="P5" s="19">
+        <v>77.430000000000007</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>18.55</v>
+      </c>
+      <c r="R5" s="19">
+        <v>49</v>
+      </c>
+      <c r="S5" s="19">
+        <v>88.17</v>
+      </c>
+      <c r="T5" s="19">
+        <v>13.64</v>
+      </c>
+      <c r="U5" s="19">
+        <v>115.66</v>
+      </c>
+      <c r="V5" s="14">
+        <f t="shared" si="1"/>
+        <v>1204.0365000000002</v>
+      </c>
+      <c r="W5" s="14">
+        <f t="shared" ref="W5:W15" si="11">U5*I5/100</f>
+        <v>1798.5129999999999</v>
+      </c>
+      <c r="X5" s="14">
+        <f t="shared" si="2"/>
+        <v>3792.7753202000004</v>
+      </c>
+      <c r="Y5" s="14">
+        <f t="shared" si="3"/>
+        <v>2660.4005000000002</v>
+      </c>
+      <c r="Z5" s="14">
+        <f t="shared" si="4"/>
+        <v>86.538499999999999</v>
+      </c>
+      <c r="AA5" s="14">
+        <f t="shared" si="5"/>
+        <v>1132.3748202000002</v>
+      </c>
+      <c r="AB5" s="15">
+        <f t="shared" si="6"/>
+        <v>51</v>
+      </c>
+      <c r="AC5" s="14">
+        <f t="shared" si="7"/>
+        <v>1183.3748202000002</v>
+      </c>
+      <c r="AD5" s="35">
+        <f t="shared" si="8"/>
+        <v>3.5712448023611643</v>
+      </c>
+      <c r="AE5" s="35">
+        <f t="shared" si="9"/>
+        <v>1.4498000000000002</v>
+      </c>
+      <c r="AF5" s="37">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="21">
+        <v>1388</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="20">
+        <f>K6-I6</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="50" t="e">
+        <f>L6/K6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="18">
+        <v>0</v>
+      </c>
+      <c r="O6" s="18"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X6" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE6" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="37"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="21">
+        <v>2267</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="20">
+        <f t="shared" ref="L7:L15" si="12">K7-I7</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="50" t="e">
+        <f t="shared" ref="M7:M15" si="13">L7/K7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" s="18">
+        <v>0</v>
+      </c>
+      <c r="O7" s="18"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X7" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="14">
+        <f>AA7+AB7</f>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE7" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="37"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="21">
+        <v>3186</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="50" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="18">
+        <v>0</v>
+      </c>
+      <c r="O8" s="18"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X8" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="14">
+        <f t="shared" ref="AC8:AC15" si="14">AA8+AB8</f>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE8" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="37"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="21">
+        <v>3105</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="50" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="18">
+        <v>0</v>
+      </c>
+      <c r="O9" s="18"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W9" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X9" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC9" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE9" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF9" s="37"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="21">
+        <v>3001</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="50" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10" s="18">
+        <v>0</v>
+      </c>
+      <c r="O10" s="18"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X10" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y10" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC10" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE10" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="37"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="21">
+        <v>2483</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="50" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" s="18">
+        <v>0</v>
+      </c>
+      <c r="O11" s="18"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W11" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X11" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE11" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="37"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="52">
+        <v>1649</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="50" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N12" s="18">
+        <v>0</v>
+      </c>
+      <c r="O12" s="18"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W12" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X12" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB12" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE12" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF12" s="37"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="52">
+        <v>785</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="50" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" s="18">
+        <v>0</v>
+      </c>
+      <c r="O13" s="18"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W13" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X13" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD13" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE13" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF13" s="37"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="52">
+        <v>252</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="50" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N14" s="18">
+        <v>0</v>
+      </c>
+      <c r="O14" s="18"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X14" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE14" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF14" s="37"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="52">
+        <v>129</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="50" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="18">
+        <v>0</v>
+      </c>
+      <c r="O15" s="18"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X15" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="35" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE15" s="35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF15" s="37"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="35"/>
+      <c r="AE16" s="35"/>
+      <c r="AF16" s="37"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="O17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="P17" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q17" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="R17" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="T17" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="U17" s="39"/>
+      <c r="V17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="W17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="X17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD17" s="39"/>
+      <c r="AE17" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF17" s="39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="41">
+        <f>SUM(B4:B17)</f>
+        <v>19050</v>
+      </c>
+      <c r="C18" s="42">
+        <f>SUM(C4:C17)/1000</f>
+        <v>3504.0419999999999</v>
+      </c>
+      <c r="D18" s="42">
+        <f>SUM(D4:D17)/1000</f>
+        <v>112.039</v>
+      </c>
+      <c r="E18" s="42">
+        <f>SUM(E4:E17)/1000</f>
+        <v>3167.8820000000001</v>
+      </c>
+      <c r="F18" s="42">
+        <f>SUM(F4:F17)/1000</f>
+        <v>340.81</v>
+      </c>
+      <c r="G18" s="42">
+        <f>SUM(G4:G17)/1000</f>
+        <v>448.19900000000001</v>
+      </c>
+      <c r="H18" s="64">
+        <f>G18/B18</f>
+        <v>2.352750656167979E-2</v>
+      </c>
+      <c r="I18" s="43">
+        <f t="shared" ref="I18:O18" si="15">SUM(I4:I15)</f>
+        <v>3158</v>
+      </c>
+      <c r="J18" s="43">
+        <f t="shared" si="15"/>
+        <v>94</v>
+      </c>
+      <c r="K18" s="43">
+        <f t="shared" si="15"/>
+        <v>3512.1990000000001</v>
+      </c>
+      <c r="L18" s="43">
+        <f t="shared" si="15"/>
+        <v>354.19900000000007</v>
+      </c>
+      <c r="M18" s="51">
+        <f t="shared" ref="M18" si="16">L18/K18</f>
+        <v>0.10084821503565147</v>
+      </c>
+      <c r="N18" s="43">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="44">
+        <f t="shared" si="15"/>
+        <v>985</v>
+      </c>
+      <c r="P18" s="44">
+        <f>AVERAGE(P4:P14)</f>
+        <v>74.935000000000002</v>
+      </c>
+      <c r="Q18" s="44">
+        <f>AVERAGE(Q4:Q15)</f>
+        <v>18.55</v>
+      </c>
+      <c r="R18" s="44">
+        <f>AVERAGE(R4:R15)</f>
+        <v>49</v>
+      </c>
+      <c r="S18" s="44">
+        <f>AVERAGE(S4:S14)</f>
+        <v>102.30000000000001</v>
+      </c>
+      <c r="T18" s="44">
+        <f>AVERAGE(T4:T15)</f>
+        <v>13.68</v>
+      </c>
+      <c r="U18" s="44"/>
+      <c r="V18" s="44">
+        <f t="shared" ref="V18:AC18" si="17">SUM(V4:V15)</f>
+        <v>2365.2497000000003</v>
+      </c>
+      <c r="W18" s="44">
+        <f t="shared" si="17"/>
+        <v>3880.6496999999999</v>
+      </c>
+      <c r="X18" s="44">
+        <f t="shared" si="17"/>
+        <v>7663.1518930000002</v>
+      </c>
+      <c r="Y18" s="44">
+        <f t="shared" si="17"/>
+        <v>5385.2267000000002</v>
+      </c>
+      <c r="Z18" s="44">
+        <f t="shared" si="17"/>
+        <v>98.251999999999995</v>
+      </c>
+      <c r="AA18" s="44">
+        <f t="shared" si="17"/>
+        <v>2277.925193</v>
+      </c>
+      <c r="AB18" s="44">
+        <f t="shared" si="17"/>
+        <v>56.4</v>
+      </c>
+      <c r="AC18" s="44">
+        <f t="shared" si="17"/>
+        <v>2334.3251930000001</v>
+      </c>
+      <c r="AD18" s="45"/>
+      <c r="AE18" s="45">
+        <f>AVERAGE(AE4:AE15)</f>
+        <v>0.23747500000000002</v>
+      </c>
+      <c r="AF18" s="44">
+        <f>SUM(AF4:AF15)</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+    </row>
+    <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="57"/>
+      <c r="Y20" s="56"/>
+    </row>
+    <row r="21" spans="1:32" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+    </row>
+    <row r="22" spans="1:32" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="47">
+        <f>G18</f>
+        <v>448.19900000000001</v>
+      </c>
+      <c r="D22" s="47">
+        <f>J18</f>
+        <v>94</v>
+      </c>
+      <c r="E22" s="47">
+        <f>I18</f>
+        <v>3158</v>
+      </c>
+      <c r="F22" s="47">
+        <f>K18</f>
+        <v>3512.1990000000001</v>
+      </c>
+      <c r="G22" s="47">
+        <f>L18</f>
+        <v>354.19900000000007</v>
+      </c>
+      <c r="H22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="34">
+        <v>0</v>
+      </c>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="68">
+        <f>G24/(G18)</f>
+        <v>5.2082338269384802</v>
+      </c>
+      <c r="P22" s="68"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
+      <c r="Y22" s="56"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
+      <c r="K23" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" ht="21" x14ac:dyDescent="0.35">
+      <c r="C24" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="49">
+        <f>AC18+K22</f>
+        <v>2334.3251930000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="28"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="31"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="25"/>
+    </row>
+    <row r="27" spans="1:32" ht="21" x14ac:dyDescent="0.35">
+      <c r="C27" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="48">
+        <f>G24-AF18</f>
+        <v>1734.3251930000001</v>
       </c>
     </row>
     <row r="28" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>